<commit_message>
Commit atualizacao tesouro dia 05/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -335,7 +335,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -369,12 +369,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="8" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -389,9 +383,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -422,12 +413,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -475,6 +460,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -632,6 +620,9 @@
                   <c:pt idx="1">
                     <c:v>04/06</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>05/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -722,6 +713,9 @@
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>4.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -785,6 +779,9 @@
                   <c:pt idx="1">
                     <c:v>04/06</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>05/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -876,6 +873,9 @@
                 <c:pt idx="1" formatCode="General">
                   <c:v>3.89</c:v>
                 </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>3.93</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -891,8 +891,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1021970320"/>
-        <c:axId val="-1021967056"/>
+        <c:axId val="-203203840"/>
+        <c:axId val="-65017728"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -961,6 +961,9 @@
                         <c:pt idx="1">
                           <c:v>04/06</c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>05/06</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1055,7 +1058,7 @@
                         <c:v>0.23342387244852411</c:v>
                       </c:pt>
                       <c:pt idx="2" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23479936621722805</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1186,6 +1189,9 @@
                         <c:pt idx="1">
                           <c:v>04/06</c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>05/06</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1280,7 +1286,7 @@
                         <c:v>0.22918011530391397</c:v>
                       </c:pt>
                       <c:pt idx="2" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23053355406491119</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1349,7 +1355,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1021970320"/>
+        <c:axId val="-203203840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1392,7 +1398,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1021967056"/>
+        <c:crossAx val="-65017728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1400,7 +1406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1021967056"/>
+        <c:axId val="-65017728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,7 +1457,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1021970320"/>
+        <c:crossAx val="-203203840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1670,6 +1676,9 @@
                   <c:pt idx="1">
                     <c:v>04/06</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>05/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1760,6 +1769,9 @@
                 </c:pt>
                 <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1729.21</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1719.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1823,6 +1835,9 @@
                   <c:pt idx="1">
                     <c:v>04/06</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>05/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1914,6 +1929,9 @@
                 <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1761.23</c:v>
                 </c:pt>
+                <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1750.89</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1929,11 +1947,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1021977392"/>
-        <c:axId val="-1021976848"/>
+        <c:axId val="-65023168"/>
+        <c:axId val="-65023712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1021977392"/>
+        <c:axId val="-65023168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1976,7 +1994,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1021976848"/>
+        <c:crossAx val="-65023712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1984,7 +2002,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1021976848"/>
+        <c:axId val="-65023712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2035,7 +2053,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1021977392"/>
+        <c:crossAx val="-65023168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2224,6 +2242,9 @@
                   <c:pt idx="1">
                     <c:v>04/06</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>05/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2316,7 +2337,7 @@
                   <c:v>0.23342387244852411</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23479936621722805</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2437,6 +2458,9 @@
                   <c:pt idx="1">
                     <c:v>04/06</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>05/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2529,7 +2553,7 @@
                   <c:v>0.22918011530391397</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23053355406491119</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2603,8 +2627,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1021979568"/>
-        <c:axId val="-1021977936"/>
+        <c:axId val="-65025344"/>
+        <c:axId val="-65020448"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2673,6 +2697,9 @@
                         <c:pt idx="1">
                           <c:v>04/06</c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>05/06</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -2765,6 +2792,9 @@
                       </c:pt>
                       <c:pt idx="1" formatCode="General">
                         <c:v>4.01</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="General">
+                        <c:v>4.05</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2838,6 +2868,9 @@
                         <c:pt idx="1">
                           <c:v>04/06</c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>05/06</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -2931,6 +2964,9 @@
                       <c:pt idx="1" formatCode="General">
                         <c:v>3.89</c:v>
                       </c:pt>
+                      <c:pt idx="2" formatCode="General">
+                        <c:v>3.93</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -2941,7 +2977,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1021979568"/>
+        <c:axId val="-65025344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2984,7 +3020,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1021977936"/>
+        <c:crossAx val="-65020448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2992,7 +3028,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1021977936"/>
+        <c:axId val="-65020448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3043,7 +3079,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1021979568"/>
+        <c:crossAx val="-65025344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3139,7 +3175,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3232,6 +3267,9 @@
                   <c:pt idx="1">
                     <c:v>04/06</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>05/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3324,64 +3362,64 @@
                   <c:v>8.9394791060739359E-2</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>0.13409218659110902</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3445,6 +3483,9 @@
                   <c:pt idx="1">
                     <c:v>04/06</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>05/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3537,64 +3578,64 @@
                   <c:v>8.6746056510791536E-2</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>0.1301190847661873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3611,8 +3652,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1021975760"/>
-        <c:axId val="-1021969776"/>
+        <c:axId val="-65018816"/>
+        <c:axId val="-65032960"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3681,6 +3722,9 @@
                         <c:pt idx="1">
                           <c:v>04/06</c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>05/06</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3773,6 +3817,9 @@
                       </c:pt>
                       <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1729.21</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1719.08</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3846,6 +3893,9 @@
                         <c:pt idx="1">
                           <c:v>04/06</c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>05/06</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3939,6 +3989,9 @@
                       <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1761.23</c:v>
                       </c:pt>
+                      <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1750.89</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3949,7 +4002,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1021975760"/>
+        <c:axId val="-65018816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3992,7 +4045,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1021969776"/>
+        <c:crossAx val="-65032960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4000,7 +4053,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1021969776"/>
+        <c:axId val="-65032960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4051,7 +4104,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1021975760"/>
+        <c:crossAx val="-65018816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4065,7 +4118,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7005,7 +7057,7 @@
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="52">
+      <c r="B7" s="47">
         <v>49444</v>
       </c>
       <c r="C7">
@@ -7036,7 +7088,7 @@
         <f>((C2*D7)/100)+C2</f>
         <v>402.19179000000003</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="36">
         <f>((C2*E7)/100)+C2</f>
         <v>446.66994300000005</v>
       </c>
@@ -7054,11 +7106,11 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="42"/>
+      <c r="D10" s="37"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" s="12"/>
-      <c r="E11" s="41"/>
+      <c r="E11" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7071,7 +7123,7 @@
   <dimension ref="A2:DO11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:G4"/>
+      <selection activeCell="H4" sqref="H4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7107,953 +7159,965 @@
     <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.85546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="28.85546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="28.85546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="28.85546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="28.85546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="28.85546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="28.85546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="28.85546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="48" max="119" width="9.140625" style="45"/>
+    <col min="32" max="32" width="28.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="28.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="28.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="28.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="28.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="28.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="28.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="48" max="119" width="9.140625" style="40"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:119" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="1:119" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="P2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="Q2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="21" t="s">
+      <c r="R2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="21" t="s">
+      <c r="S2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="21" t="s">
+      <c r="T2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="21" t="s">
+      <c r="U2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="21" t="s">
+      <c r="W2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="21" t="s">
+      <c r="X2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="Y2" s="21" t="s">
+      <c r="Y2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="Z2" s="21" t="s">
+      <c r="Z2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="21" t="s">
+      <c r="AA2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="21" t="s">
+      <c r="AB2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AC2" s="21" t="s">
+      <c r="AC2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="21" t="s">
+      <c r="AD2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AE2" s="49" t="s">
+      <c r="AE2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="AF2" s="21" t="s">
+      <c r="AF2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AG2" s="49" t="s">
+      <c r="AG2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="AH2" s="21" t="s">
+      <c r="AH2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AI2" s="49" t="s">
+      <c r="AI2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="AJ2" s="21" t="s">
+      <c r="AJ2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AK2" s="21" t="s">
+      <c r="AK2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AL2" s="21" t="s">
+      <c r="AL2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AM2" s="21" t="s">
+      <c r="AM2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AN2" s="21" t="s">
+      <c r="AN2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AO2" s="21" t="s">
+      <c r="AO2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AP2" s="21" t="s">
+      <c r="AP2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AQ2" s="21" t="s">
+      <c r="AQ2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AR2" s="21" t="s">
+      <c r="AR2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AS2" s="21" t="s">
+      <c r="AS2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AT2" s="21" t="s">
+      <c r="AT2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AU2" s="21" t="s">
+      <c r="AU2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AV2" s="44"/>
-      <c r="AW2" s="44"/>
-      <c r="AX2" s="44"/>
-      <c r="AY2" s="44"/>
-      <c r="AZ2" s="44"/>
-      <c r="BA2" s="44"/>
-      <c r="BB2" s="44"/>
-      <c r="BC2" s="44"/>
-      <c r="BD2" s="44"/>
-      <c r="BE2" s="44"/>
-      <c r="BF2" s="44"/>
-      <c r="BG2" s="44"/>
-      <c r="BH2" s="44"/>
-      <c r="BI2" s="44"/>
-      <c r="BJ2" s="44"/>
-      <c r="BK2" s="44"/>
-      <c r="BL2" s="44"/>
-      <c r="BM2" s="44"/>
-      <c r="BN2" s="44"/>
-      <c r="BO2" s="44"/>
-      <c r="BP2" s="44"/>
-      <c r="BQ2" s="44"/>
-      <c r="BR2" s="44"/>
-      <c r="BS2" s="44"/>
-      <c r="BT2" s="44"/>
-      <c r="BU2" s="44"/>
-      <c r="BV2" s="44"/>
-      <c r="BW2" s="44"/>
-      <c r="BX2" s="44"/>
-      <c r="BY2" s="44"/>
-      <c r="BZ2" s="44"/>
-      <c r="CA2" s="44"/>
-      <c r="CB2" s="44"/>
-      <c r="CC2" s="44"/>
-      <c r="CD2" s="44"/>
-      <c r="CE2" s="44"/>
-      <c r="CF2" s="44"/>
-      <c r="CG2" s="44"/>
-      <c r="CH2" s="44"/>
-      <c r="CI2" s="44"/>
-      <c r="CJ2" s="44"/>
-      <c r="CK2" s="44"/>
-      <c r="CL2" s="44"/>
-      <c r="CM2" s="44"/>
-      <c r="CN2" s="44"/>
-      <c r="CO2" s="44"/>
-      <c r="CP2" s="44"/>
-      <c r="CQ2" s="44"/>
-      <c r="CR2" s="44"/>
-      <c r="CS2" s="44"/>
-      <c r="CT2" s="44"/>
-      <c r="CU2" s="44"/>
-      <c r="CV2" s="44"/>
-      <c r="CW2" s="44"/>
-      <c r="CX2" s="44"/>
-      <c r="CY2" s="44"/>
-      <c r="CZ2" s="44"/>
-      <c r="DA2" s="44"/>
-      <c r="DB2" s="44"/>
-      <c r="DC2" s="44"/>
-      <c r="DD2" s="44"/>
-      <c r="DE2" s="44"/>
-      <c r="DF2" s="44"/>
-      <c r="DG2" s="44"/>
-      <c r="DH2" s="44"/>
-      <c r="DI2" s="44"/>
-      <c r="DJ2" s="44"/>
-      <c r="DK2" s="44"/>
-      <c r="DL2" s="44"/>
-      <c r="DM2" s="44"/>
-      <c r="DN2" s="44"/>
-      <c r="DO2" s="44"/>
+      <c r="AV2" s="39"/>
+      <c r="AW2" s="39"/>
+      <c r="AX2" s="39"/>
+      <c r="AY2" s="39"/>
+      <c r="AZ2" s="39"/>
+      <c r="BA2" s="39"/>
+      <c r="BB2" s="39"/>
+      <c r="BC2" s="39"/>
+      <c r="BD2" s="39"/>
+      <c r="BE2" s="39"/>
+      <c r="BF2" s="39"/>
+      <c r="BG2" s="39"/>
+      <c r="BH2" s="39"/>
+      <c r="BI2" s="39"/>
+      <c r="BJ2" s="39"/>
+      <c r="BK2" s="39"/>
+      <c r="BL2" s="39"/>
+      <c r="BM2" s="39"/>
+      <c r="BN2" s="39"/>
+      <c r="BO2" s="39"/>
+      <c r="BP2" s="39"/>
+      <c r="BQ2" s="39"/>
+      <c r="BR2" s="39"/>
+      <c r="BS2" s="39"/>
+      <c r="BT2" s="39"/>
+      <c r="BU2" s="39"/>
+      <c r="BV2" s="39"/>
+      <c r="BW2" s="39"/>
+      <c r="BX2" s="39"/>
+      <c r="BY2" s="39"/>
+      <c r="BZ2" s="39"/>
+      <c r="CA2" s="39"/>
+      <c r="CB2" s="39"/>
+      <c r="CC2" s="39"/>
+      <c r="CD2" s="39"/>
+      <c r="CE2" s="39"/>
+      <c r="CF2" s="39"/>
+      <c r="CG2" s="39"/>
+      <c r="CH2" s="39"/>
+      <c r="CI2" s="39"/>
+      <c r="CJ2" s="39"/>
+      <c r="CK2" s="39"/>
+      <c r="CL2" s="39"/>
+      <c r="CM2" s="39"/>
+      <c r="CN2" s="39"/>
+      <c r="CO2" s="39"/>
+      <c r="CP2" s="39"/>
+      <c r="CQ2" s="39"/>
+      <c r="CR2" s="39"/>
+      <c r="CS2" s="39"/>
+      <c r="CT2" s="39"/>
+      <c r="CU2" s="39"/>
+      <c r="CV2" s="39"/>
+      <c r="CW2" s="39"/>
+      <c r="CX2" s="39"/>
+      <c r="CY2" s="39"/>
+      <c r="CZ2" s="39"/>
+      <c r="DA2" s="39"/>
+      <c r="DB2" s="39"/>
+      <c r="DC2" s="39"/>
+      <c r="DD2" s="39"/>
+      <c r="DE2" s="39"/>
+      <c r="DF2" s="39"/>
+      <c r="DG2" s="39"/>
+      <c r="DH2" s="39"/>
+      <c r="DI2" s="39"/>
+      <c r="DJ2" s="39"/>
+      <c r="DK2" s="39"/>
+      <c r="DL2" s="39"/>
+      <c r="DM2" s="39"/>
+      <c r="DN2" s="39"/>
+      <c r="DO2" s="39"/>
     </row>
-    <row r="3" spans="1:119" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="30" t="s">
+    <row r="3" spans="1:119" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="57">
+      <c r="C3" s="28"/>
+      <c r="D3" s="52">
         <v>43619</v>
       </c>
-      <c r="E3" s="56">
+      <c r="E3" s="51">
         <v>43619</v>
       </c>
-      <c r="F3" s="57">
+      <c r="F3" s="52">
         <v>43620</v>
       </c>
-      <c r="G3" s="58">
+      <c r="G3" s="53">
         <v>43620</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="26"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="27"/>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="26"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="26"/>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="26"/>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="26"/>
-      <c r="AL3" s="25"/>
-      <c r="AM3" s="26"/>
-      <c r="AN3" s="25"/>
-      <c r="AO3" s="26"/>
-      <c r="AP3" s="25"/>
-      <c r="AQ3" s="26"/>
-      <c r="AR3" s="25"/>
-      <c r="AS3" s="26"/>
-      <c r="AT3" s="25"/>
-      <c r="AU3" s="26"/>
-      <c r="AV3" s="44"/>
-      <c r="AW3" s="44"/>
-      <c r="AX3" s="44"/>
-      <c r="AY3" s="44"/>
-      <c r="AZ3" s="44"/>
-      <c r="BA3" s="44"/>
-      <c r="BB3" s="44"/>
-      <c r="BC3" s="44"/>
-      <c r="BD3" s="44"/>
-      <c r="BE3" s="44"/>
-      <c r="BF3" s="44"/>
-      <c r="BG3" s="44"/>
-      <c r="BH3" s="44"/>
-      <c r="BI3" s="44"/>
-      <c r="BJ3" s="44"/>
-      <c r="BK3" s="44"/>
-      <c r="BL3" s="44"/>
-      <c r="BM3" s="44"/>
-      <c r="BN3" s="44"/>
-      <c r="BO3" s="44"/>
-      <c r="BP3" s="44"/>
-      <c r="BQ3" s="44"/>
-      <c r="BR3" s="44"/>
-      <c r="BS3" s="44"/>
-      <c r="BT3" s="44"/>
-      <c r="BU3" s="44"/>
-      <c r="BV3" s="44"/>
-      <c r="BW3" s="44"/>
-      <c r="BX3" s="44"/>
-      <c r="BY3" s="44"/>
-      <c r="BZ3" s="44"/>
-      <c r="CA3" s="44"/>
-      <c r="CB3" s="44"/>
-      <c r="CC3" s="44"/>
-      <c r="CD3" s="44"/>
-      <c r="CE3" s="44"/>
-      <c r="CF3" s="44"/>
-      <c r="CG3" s="44"/>
-      <c r="CH3" s="44"/>
-      <c r="CI3" s="44"/>
-      <c r="CJ3" s="44"/>
-      <c r="CK3" s="44"/>
-      <c r="CL3" s="44"/>
-      <c r="CM3" s="44"/>
-      <c r="CN3" s="44"/>
-      <c r="CO3" s="44"/>
-      <c r="CP3" s="44"/>
-      <c r="CQ3" s="44"/>
-      <c r="CR3" s="44"/>
-      <c r="CS3" s="44"/>
-      <c r="CT3" s="44"/>
-      <c r="CU3" s="44"/>
-      <c r="CV3" s="44"/>
-      <c r="CW3" s="44"/>
-      <c r="CX3" s="44"/>
-      <c r="CY3" s="44"/>
-      <c r="CZ3" s="44"/>
-      <c r="DA3" s="44"/>
-      <c r="DB3" s="44"/>
-      <c r="DC3" s="44"/>
-      <c r="DD3" s="44"/>
-      <c r="DE3" s="44"/>
-      <c r="DF3" s="44"/>
-      <c r="DG3" s="44"/>
-      <c r="DH3" s="44"/>
-      <c r="DI3" s="44"/>
-      <c r="DJ3" s="44"/>
-      <c r="DK3" s="44"/>
-      <c r="DL3" s="44"/>
-      <c r="DM3" s="44"/>
-      <c r="DN3" s="44"/>
-      <c r="DO3" s="44"/>
+      <c r="H3" s="55">
+        <v>43621</v>
+      </c>
+      <c r="I3" s="55">
+        <v>43621</v>
+      </c>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="22"/>
+      <c r="AE3" s="23"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="23"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="23"/>
+      <c r="AJ3" s="22"/>
+      <c r="AK3" s="23"/>
+      <c r="AL3" s="22"/>
+      <c r="AM3" s="23"/>
+      <c r="AN3" s="22"/>
+      <c r="AO3" s="23"/>
+      <c r="AP3" s="22"/>
+      <c r="AQ3" s="23"/>
+      <c r="AR3" s="22"/>
+      <c r="AS3" s="23"/>
+      <c r="AT3" s="22"/>
+      <c r="AU3" s="23"/>
+      <c r="AV3" s="39"/>
+      <c r="AW3" s="39"/>
+      <c r="AX3" s="39"/>
+      <c r="AY3" s="39"/>
+      <c r="AZ3" s="39"/>
+      <c r="BA3" s="39"/>
+      <c r="BB3" s="39"/>
+      <c r="BC3" s="39"/>
+      <c r="BD3" s="39"/>
+      <c r="BE3" s="39"/>
+      <c r="BF3" s="39"/>
+      <c r="BG3" s="39"/>
+      <c r="BH3" s="39"/>
+      <c r="BI3" s="39"/>
+      <c r="BJ3" s="39"/>
+      <c r="BK3" s="39"/>
+      <c r="BL3" s="39"/>
+      <c r="BM3" s="39"/>
+      <c r="BN3" s="39"/>
+      <c r="BO3" s="39"/>
+      <c r="BP3" s="39"/>
+      <c r="BQ3" s="39"/>
+      <c r="BR3" s="39"/>
+      <c r="BS3" s="39"/>
+      <c r="BT3" s="39"/>
+      <c r="BU3" s="39"/>
+      <c r="BV3" s="39"/>
+      <c r="BW3" s="39"/>
+      <c r="BX3" s="39"/>
+      <c r="BY3" s="39"/>
+      <c r="BZ3" s="39"/>
+      <c r="CA3" s="39"/>
+      <c r="CB3" s="39"/>
+      <c r="CC3" s="39"/>
+      <c r="CD3" s="39"/>
+      <c r="CE3" s="39"/>
+      <c r="CF3" s="39"/>
+      <c r="CG3" s="39"/>
+      <c r="CH3" s="39"/>
+      <c r="CI3" s="39"/>
+      <c r="CJ3" s="39"/>
+      <c r="CK3" s="39"/>
+      <c r="CL3" s="39"/>
+      <c r="CM3" s="39"/>
+      <c r="CN3" s="39"/>
+      <c r="CO3" s="39"/>
+      <c r="CP3" s="39"/>
+      <c r="CQ3" s="39"/>
+      <c r="CR3" s="39"/>
+      <c r="CS3" s="39"/>
+      <c r="CT3" s="39"/>
+      <c r="CU3" s="39"/>
+      <c r="CV3" s="39"/>
+      <c r="CW3" s="39"/>
+      <c r="CX3" s="39"/>
+      <c r="CY3" s="39"/>
+      <c r="CZ3" s="39"/>
+      <c r="DA3" s="39"/>
+      <c r="DB3" s="39"/>
+      <c r="DC3" s="39"/>
+      <c r="DD3" s="39"/>
+      <c r="DE3" s="39"/>
+      <c r="DF3" s="39"/>
+      <c r="DG3" s="39"/>
+      <c r="DH3" s="39"/>
+      <c r="DI3" s="39"/>
+      <c r="DJ3" s="39"/>
+      <c r="DK3" s="39"/>
+      <c r="DL3" s="39"/>
+      <c r="DM3" s="39"/>
+      <c r="DN3" s="39"/>
+      <c r="DO3" s="39"/>
     </row>
-    <row r="4" spans="1:119" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+    <row r="4" spans="1:119" s="34" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="30">
         <v>49444</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="14">
         <v>4.09</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="15">
         <v>1707.8</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="14">
         <v>4.01</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="15">
         <v>1729.21</v>
       </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="37"/>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="37"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="37"/>
-      <c r="AF4" s="36"/>
-      <c r="AG4" s="37"/>
-      <c r="AH4" s="36"/>
-      <c r="AI4" s="37"/>
-      <c r="AJ4" s="36"/>
-      <c r="AK4" s="37"/>
-      <c r="AL4" s="36"/>
-      <c r="AM4" s="37"/>
-      <c r="AN4" s="36"/>
-      <c r="AO4" s="38"/>
-      <c r="AP4" s="36"/>
-      <c r="AQ4" s="37"/>
-      <c r="AR4" s="36"/>
-      <c r="AS4" s="37"/>
-      <c r="AT4" s="36"/>
-      <c r="AU4" s="37"/>
-      <c r="AV4" s="44"/>
-      <c r="AW4" s="44"/>
-      <c r="AX4" s="44"/>
-      <c r="AY4" s="44"/>
-      <c r="AZ4" s="44"/>
-      <c r="BA4" s="44"/>
-      <c r="BB4" s="44"/>
-      <c r="BC4" s="44"/>
-      <c r="BD4" s="44"/>
-      <c r="BE4" s="44"/>
-      <c r="BF4" s="44"/>
-      <c r="BG4" s="44"/>
-      <c r="BH4" s="44"/>
-      <c r="BI4" s="44"/>
-      <c r="BJ4" s="44"/>
-      <c r="BK4" s="44"/>
-      <c r="BL4" s="44"/>
-      <c r="BM4" s="44"/>
-      <c r="BN4" s="44"/>
-      <c r="BO4" s="44"/>
-      <c r="BP4" s="44"/>
-      <c r="BQ4" s="44"/>
-      <c r="BR4" s="44"/>
-      <c r="BS4" s="44"/>
-      <c r="BT4" s="44"/>
-      <c r="BU4" s="44"/>
-      <c r="BV4" s="44"/>
-      <c r="BW4" s="44"/>
-      <c r="BX4" s="44"/>
-      <c r="BY4" s="44"/>
-      <c r="BZ4" s="44"/>
-      <c r="CA4" s="44"/>
-      <c r="CB4" s="44"/>
-      <c r="CC4" s="44"/>
-      <c r="CD4" s="44"/>
-      <c r="CE4" s="44"/>
-      <c r="CF4" s="44"/>
-      <c r="CG4" s="44"/>
-      <c r="CH4" s="44"/>
-      <c r="CI4" s="44"/>
-      <c r="CJ4" s="44"/>
-      <c r="CK4" s="44"/>
-      <c r="CL4" s="44"/>
-      <c r="CM4" s="44"/>
-      <c r="CN4" s="44"/>
-      <c r="CO4" s="44"/>
-      <c r="CP4" s="44"/>
-      <c r="CQ4" s="44"/>
-      <c r="CR4" s="44"/>
-      <c r="CS4" s="44"/>
-      <c r="CT4" s="44"/>
-      <c r="CU4" s="44"/>
-      <c r="CV4" s="44"/>
-      <c r="CW4" s="44"/>
-      <c r="CX4" s="44"/>
-      <c r="CY4" s="44"/>
-      <c r="CZ4" s="44"/>
-      <c r="DA4" s="44"/>
-      <c r="DB4" s="44"/>
-      <c r="DC4" s="44"/>
-      <c r="DD4" s="44"/>
-      <c r="DE4" s="44"/>
-      <c r="DF4" s="44"/>
-      <c r="DG4" s="44"/>
-      <c r="DH4" s="44"/>
-      <c r="DI4" s="44"/>
-      <c r="DJ4" s="44"/>
-      <c r="DK4" s="44"/>
-      <c r="DL4" s="44"/>
-      <c r="DM4" s="44"/>
-      <c r="DN4" s="44"/>
-      <c r="DO4" s="44"/>
+      <c r="H4" s="14">
+        <v>4.05</v>
+      </c>
+      <c r="I4" s="15">
+        <v>1719.08</v>
+      </c>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="31"/>
+      <c r="AA4" s="33"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="32"/>
+      <c r="AD4" s="31"/>
+      <c r="AE4" s="32"/>
+      <c r="AF4" s="31"/>
+      <c r="AG4" s="32"/>
+      <c r="AH4" s="31"/>
+      <c r="AI4" s="32"/>
+      <c r="AJ4" s="31"/>
+      <c r="AK4" s="32"/>
+      <c r="AL4" s="31"/>
+      <c r="AM4" s="32"/>
+      <c r="AN4" s="31"/>
+      <c r="AO4" s="33"/>
+      <c r="AP4" s="31"/>
+      <c r="AQ4" s="32"/>
+      <c r="AR4" s="31"/>
+      <c r="AS4" s="32"/>
+      <c r="AT4" s="31"/>
+      <c r="AU4" s="32"/>
+      <c r="AV4" s="39"/>
+      <c r="AW4" s="39"/>
+      <c r="AX4" s="39"/>
+      <c r="AY4" s="39"/>
+      <c r="AZ4" s="39"/>
+      <c r="BA4" s="39"/>
+      <c r="BB4" s="39"/>
+      <c r="BC4" s="39"/>
+      <c r="BD4" s="39"/>
+      <c r="BE4" s="39"/>
+      <c r="BF4" s="39"/>
+      <c r="BG4" s="39"/>
+      <c r="BH4" s="39"/>
+      <c r="BI4" s="39"/>
+      <c r="BJ4" s="39"/>
+      <c r="BK4" s="39"/>
+      <c r="BL4" s="39"/>
+      <c r="BM4" s="39"/>
+      <c r="BN4" s="39"/>
+      <c r="BO4" s="39"/>
+      <c r="BP4" s="39"/>
+      <c r="BQ4" s="39"/>
+      <c r="BR4" s="39"/>
+      <c r="BS4" s="39"/>
+      <c r="BT4" s="39"/>
+      <c r="BU4" s="39"/>
+      <c r="BV4" s="39"/>
+      <c r="BW4" s="39"/>
+      <c r="BX4" s="39"/>
+      <c r="BY4" s="39"/>
+      <c r="BZ4" s="39"/>
+      <c r="CA4" s="39"/>
+      <c r="CB4" s="39"/>
+      <c r="CC4" s="39"/>
+      <c r="CD4" s="39"/>
+      <c r="CE4" s="39"/>
+      <c r="CF4" s="39"/>
+      <c r="CG4" s="39"/>
+      <c r="CH4" s="39"/>
+      <c r="CI4" s="39"/>
+      <c r="CJ4" s="39"/>
+      <c r="CK4" s="39"/>
+      <c r="CL4" s="39"/>
+      <c r="CM4" s="39"/>
+      <c r="CN4" s="39"/>
+      <c r="CO4" s="39"/>
+      <c r="CP4" s="39"/>
+      <c r="CQ4" s="39"/>
+      <c r="CR4" s="39"/>
+      <c r="CS4" s="39"/>
+      <c r="CT4" s="39"/>
+      <c r="CU4" s="39"/>
+      <c r="CV4" s="39"/>
+      <c r="CW4" s="39"/>
+      <c r="CX4" s="39"/>
+      <c r="CY4" s="39"/>
+      <c r="CZ4" s="39"/>
+      <c r="DA4" s="39"/>
+      <c r="DB4" s="39"/>
+      <c r="DC4" s="39"/>
+      <c r="DD4" s="39"/>
+      <c r="DE4" s="39"/>
+      <c r="DF4" s="39"/>
+      <c r="DG4" s="39"/>
+      <c r="DH4" s="39"/>
+      <c r="DI4" s="39"/>
+      <c r="DJ4" s="39"/>
+      <c r="DK4" s="39"/>
+      <c r="DL4" s="39"/>
+      <c r="DM4" s="39"/>
+      <c r="DN4" s="39"/>
+      <c r="DO4" s="39"/>
     </row>
-    <row r="5" spans="1:119" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:119" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="13">
         <v>49444</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="14">
         <v>3.97</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="15">
         <v>1739.41</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="14">
         <v>3.89</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="15">
         <v>1761.23</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="17"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="17"/>
-      <c r="AD5" s="47"/>
-      <c r="AE5" s="48"/>
-      <c r="AF5" s="47"/>
-      <c r="AG5" s="48"/>
-      <c r="AH5" s="47"/>
-      <c r="AI5" s="17"/>
-      <c r="AJ5" s="47"/>
-      <c r="AK5" s="48"/>
-      <c r="AL5" s="47"/>
-      <c r="AM5" s="48"/>
-      <c r="AN5" s="47"/>
-      <c r="AO5" s="53"/>
-      <c r="AP5" s="47"/>
-      <c r="AQ5" s="48"/>
-      <c r="AR5" s="47"/>
-      <c r="AS5" s="48"/>
-      <c r="AT5" s="47"/>
-      <c r="AU5" s="48"/>
+      <c r="H5" s="14">
+        <v>3.93</v>
+      </c>
+      <c r="I5" s="15">
+        <v>1750.89</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="42"/>
+      <c r="AE5" s="43"/>
+      <c r="AF5" s="42"/>
+      <c r="AG5" s="43"/>
+      <c r="AH5" s="42"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="42"/>
+      <c r="AK5" s="43"/>
+      <c r="AL5" s="42"/>
+      <c r="AM5" s="43"/>
+      <c r="AN5" s="42"/>
+      <c r="AO5" s="48"/>
+      <c r="AP5" s="42"/>
+      <c r="AQ5" s="43"/>
+      <c r="AR5" s="42"/>
+      <c r="AS5" s="43"/>
+      <c r="AT5" s="42"/>
+      <c r="AU5" s="43"/>
     </row>
-    <row r="6" spans="1:119" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+    <row r="6" spans="1:119" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="55">
+      <c r="B6" s="50">
         <f>[3]GRAFICO!$AU$6+[3]GRAFICO!$B$6</f>
         <v>403.63889447671238</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="41">
         <v>43587</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="46">
         <f>$B$6/E4</f>
         <v>0.23635021341885021</v>
       </c>
-      <c r="E6" s="50">
+      <c r="E6" s="45">
         <f>(((D4/365)*$B$7)/100)</f>
         <v>4.5138851288694319E-2</v>
       </c>
-      <c r="F6" s="51">
+      <c r="F6" s="46">
         <f>$B$6/G4</f>
         <v>0.23342387244852411</v>
       </c>
-      <c r="G6" s="50">
+      <c r="G6" s="45">
         <f>(((F4/365)*$B$7)/100)+E6</f>
         <v>8.9394791060739359E-2</v>
       </c>
-      <c r="H6" s="51" t="e">
+      <c r="H6" s="46">
         <f t="shared" ref="H6" si="0">$B$6/I4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I6" s="50">
+        <v>0.23479936621722805</v>
+      </c>
+      <c r="I6" s="45">
         <f t="shared" ref="I6:I7" si="1">(((H4/365)*$B$7)/100)+G6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="J6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="J6" s="46" t="e">
         <f t="shared" ref="J6" si="2">$B$6/K4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K6" s="50">
+      <c r="K6" s="45">
         <f t="shared" ref="K6:K7" si="3">(((J4/365)*$B$7)/100)+I6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="L6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="L6" s="46" t="e">
         <f t="shared" ref="L6" si="4">$B$6/M4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M6" s="50">
+      <c r="M6" s="45">
         <f t="shared" ref="M6:M7" si="5">(((L4/365)*$B$7)/100)+K6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="N6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="N6" s="46" t="e">
         <f t="shared" ref="N6" si="6">$B$6/O4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O6" s="50">
+      <c r="O6" s="45">
         <f t="shared" ref="O6:O7" si="7">(((N4/365)*$B$7)/100)+M6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="P6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="P6" s="46" t="e">
         <f t="shared" ref="P6" si="8">$B$6/Q4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q6" s="50">
+      <c r="Q6" s="45">
         <f t="shared" ref="Q6:Q7" si="9">(((P4/365)*$B$7)/100)+O6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="R6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="R6" s="46" t="e">
         <f t="shared" ref="R6" si="10">$B$6/S4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S6" s="50">
+      <c r="S6" s="45">
         <f t="shared" ref="S6:S7" si="11">(((R4/365)*$B$7)/100)+Q6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="T6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="T6" s="46" t="e">
         <f t="shared" ref="T6" si="12">$B$6/U4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U6" s="50">
+      <c r="U6" s="45">
         <f t="shared" ref="U6:U7" si="13">(((T4/365)*$B$7)/100)+S6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="V6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="V6" s="46" t="e">
         <f t="shared" ref="V6" si="14">$B$6/W4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="W6" s="50">
+      <c r="W6" s="45">
         <f t="shared" ref="W6:W7" si="15">(((V4/365)*$B$7)/100)+U6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="X6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="X6" s="46" t="e">
         <f t="shared" ref="X6" si="16">$B$6/Y4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y6" s="50">
+      <c r="Y6" s="45">
         <f t="shared" ref="Y6:Y7" si="17">(((X4/365)*$B$7)/100)+W6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="Z6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="Z6" s="46" t="e">
         <f t="shared" ref="Z6" si="18">$B$6/AA4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA6" s="50">
+      <c r="AA6" s="45">
         <f t="shared" ref="AA6:AA7" si="19">(((Z4/365)*$B$7)/100)+Y6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="AB6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="AB6" s="46" t="e">
         <f t="shared" ref="AB6" si="20">$B$6/AC4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AC6" s="50">
+      <c r="AC6" s="45">
         <f t="shared" ref="AC6:AC7" si="21">(((AB4/365)*$B$7)/100)+AA6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="AD6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="AD6" s="46" t="e">
         <f t="shared" ref="AD6" si="22">$B$6/AE4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE6" s="50">
+      <c r="AE6" s="45">
         <f t="shared" ref="AE6:AE7" si="23">(((AD4/365)*$B$7)/100)+AC6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="AF6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="AF6" s="46" t="e">
         <f t="shared" ref="AF6" si="24">$B$6/AG4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AG6" s="50">
+      <c r="AG6" s="45">
         <f t="shared" ref="AG6:AG7" si="25">(((AF4/365)*$B$7)/100)+AE6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="AH6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="AH6" s="46" t="e">
         <f>$B$6/AI4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AI6" s="50">
+      <c r="AI6" s="45">
         <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="AJ6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="AJ6" s="46" t="e">
         <f>$B$6/AK4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK6" s="50">
+      <c r="AK6" s="45">
         <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="AL6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="AL6" s="46" t="e">
         <f>$B$6/AM4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AM6" s="50">
+      <c r="AM6" s="45">
         <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="AN6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="AN6" s="46" t="e">
         <f>$B$6/AO4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AO6" s="50">
+      <c r="AO6" s="45">
         <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="AP6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="AP6" s="46" t="e">
         <f>$B$6/AQ4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AQ6" s="50">
+      <c r="AQ6" s="45">
         <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="AR6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="AR6" s="46" t="e">
         <f>$B$6/AS4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AS6" s="50">
+      <c r="AS6" s="45">
         <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="AT6" s="51" t="e">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="AT6" s="46" t="e">
         <f>$B$6/AU4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AU6" s="50">
+      <c r="AU6" s="45">
         <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>8.9394791060739359E-2</v>
-      </c>
-      <c r="AV6" s="54">
+        <v>0.13409218659110902</v>
+      </c>
+      <c r="AV6" s="49">
         <f>AU6-E6</f>
-        <v>4.425593977204504E-2</v>
+        <v>8.8953335302414699E-2</v>
       </c>
     </row>
     <row r="7" spans="1:119" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="55">
+      <c r="B7" s="50">
         <f>[3]GRAFICO!$AU$7+[3]GRAFICO!$B$7</f>
         <v>402.82837947123289</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="41">
         <v>43587</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="46">
         <f>$B$7/E5</f>
         <v>0.23158909024970126</v>
       </c>
-      <c r="E7" s="50">
+      <c r="E7" s="45">
         <f>(((D5/365)*$B$7)/100)</f>
         <v>4.3814484013720401E-2</v>
       </c>
-      <c r="F7" s="51">
+      <c r="F7" s="46">
         <f>$B$6/G5</f>
         <v>0.22918011530391397</v>
       </c>
-      <c r="G7" s="50">
+      <c r="G7" s="45">
         <f>(((F5/365)*$B$7)/100)+E7</f>
         <v>8.6746056510791536E-2</v>
       </c>
-      <c r="H7" s="51" t="e">
+      <c r="H7" s="46">
         <f t="shared" ref="H7" si="33">$B$6/I5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I7" s="50">
+        <v>0.23053355406491119</v>
+      </c>
+      <c r="I7" s="45">
         <f t="shared" si="1"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="J7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="J7" s="46" t="e">
         <f t="shared" ref="J7" si="34">$B$6/K5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K7" s="50">
+      <c r="K7" s="45">
         <f t="shared" si="3"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="L7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="L7" s="46" t="e">
         <f t="shared" ref="L7" si="35">$B$6/M5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M7" s="50">
+      <c r="M7" s="45">
         <f t="shared" si="5"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="N7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="N7" s="46" t="e">
         <f t="shared" ref="N7" si="36">$B$6/O5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O7" s="50">
+      <c r="O7" s="45">
         <f t="shared" si="7"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="P7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="P7" s="46" t="e">
         <f t="shared" ref="P7" si="37">$B$6/Q5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q7" s="50">
+      <c r="Q7" s="45">
         <f t="shared" si="9"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="R7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="R7" s="46" t="e">
         <f t="shared" ref="R7" si="38">$B$6/S5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S7" s="50">
+      <c r="S7" s="45">
         <f t="shared" si="11"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="T7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="T7" s="46" t="e">
         <f t="shared" ref="T7" si="39">$B$6/U5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U7" s="50">
+      <c r="U7" s="45">
         <f t="shared" si="13"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="V7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="V7" s="46" t="e">
         <f t="shared" ref="V7" si="40">$B$6/W5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="W7" s="50">
+      <c r="W7" s="45">
         <f t="shared" si="15"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="X7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="X7" s="46" t="e">
         <f t="shared" ref="X7" si="41">$B$6/Y5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y7" s="50">
+      <c r="Y7" s="45">
         <f t="shared" si="17"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="Z7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="Z7" s="46" t="e">
         <f t="shared" ref="Z7" si="42">$B$6/AA5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA7" s="50">
+      <c r="AA7" s="45">
         <f t="shared" si="19"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="AB7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="AB7" s="46" t="e">
         <f t="shared" ref="AB7" si="43">$B$6/AC5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AC7" s="50">
+      <c r="AC7" s="45">
         <f t="shared" si="21"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="AD7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="AD7" s="46" t="e">
         <f t="shared" ref="AD7" si="44">$B$6/AE5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE7" s="50">
+      <c r="AE7" s="45">
         <f t="shared" si="23"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="AF7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="AF7" s="46" t="e">
         <f>$B$6/AG5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AG7" s="50">
+      <c r="AG7" s="45">
         <f t="shared" si="25"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="AH7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="AH7" s="46" t="e">
         <f>$B$6/AI5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AI7" s="50">
+      <c r="AI7" s="45">
         <f t="shared" si="26"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="AJ7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="AJ7" s="46" t="e">
         <f>$B$6/AK5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AK7" s="50">
+      <c r="AK7" s="45">
         <f t="shared" si="27"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="AL7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="AL7" s="46" t="e">
         <f>$B$6/AM5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AM7" s="50">
+      <c r="AM7" s="45">
         <f t="shared" si="28"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="AN7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="AN7" s="46" t="e">
         <f>$B$6/AO5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AO7" s="50">
+      <c r="AO7" s="45">
         <f t="shared" si="29"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="AP7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="AP7" s="46" t="e">
         <f>$B$6/AQ5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AQ7" s="50">
+      <c r="AQ7" s="45">
         <f t="shared" si="30"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="AR7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="AR7" s="46" t="e">
         <f>$B$6/AS5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AS7" s="50">
+      <c r="AS7" s="45">
         <f t="shared" si="31"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="AT7" s="51" t="e">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="AT7" s="46" t="e">
         <f>$B$6/AU5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AU7" s="50">
+      <c r="AU7" s="45">
         <f t="shared" si="32"/>
-        <v>8.6746056510791536E-2</v>
-      </c>
-      <c r="AV7" s="54">
+        <v>0.1301190847661873</v>
+      </c>
+      <c r="AV7" s="49">
         <f>AU7-E7</f>
-        <v>4.2931572497071135E-2</v>
+        <v>8.6304600752466903E-2</v>
       </c>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.25">
-      <c r="AV8" s="54">
+      <c r="AV8" s="49">
         <f>AV6-AV7</f>
-        <v>1.3243672749739047E-3</v>
+        <v>2.6487345499477954E-3</v>
       </c>
     </row>
     <row r="10" spans="1:119" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit atualizacao tesouro 06/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -623,6 +623,9 @@
                   <c:pt idx="2">
                     <c:v>05/06</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>06/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -716,6 +719,9 @@
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>4.0599999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -782,6 +788,9 @@
                   <c:pt idx="2">
                     <c:v>05/06</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>06/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -876,6 +885,9 @@
                 <c:pt idx="2" formatCode="General">
                   <c:v>3.93</c:v>
                 </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>3.94</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -891,8 +903,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-203203840"/>
-        <c:axId val="-65017728"/>
+        <c:axId val="1980276336"/>
+        <c:axId val="1980277968"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -964,6 +976,9 @@
                         <c:pt idx="2">
                           <c:v>05/06</c:v>
                         </c:pt>
+                        <c:pt idx="3">
+                          <c:v>06/06</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1061,7 +1076,7 @@
                         <c:v>0.23479936621722805</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23510297547657491</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1192,6 +1207,9 @@
                         <c:pt idx="2">
                           <c:v>05/06</c:v>
                         </c:pt>
+                        <c:pt idx="3">
+                          <c:v>06/06</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1289,7 +1307,7 @@
                         <c:v>0.23053355406491119</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23083282501441846</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1355,7 +1373,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-203203840"/>
+        <c:axId val="1980276336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1398,7 +1416,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-65017728"/>
+        <c:crossAx val="1980277968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1406,7 +1424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-65017728"/>
+        <c:axId val="1980277968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1457,7 +1475,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-203203840"/>
+        <c:crossAx val="1980276336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1679,6 +1697,9 @@
                   <c:pt idx="2">
                     <c:v>05/06</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>06/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1772,6 +1793,9 @@
                 </c:pt>
                 <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1719.08</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1716.86</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1838,6 +1862,9 @@
                   <c:pt idx="2">
                     <c:v>05/06</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>06/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1932,6 +1959,9 @@
                 <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1750.89</c:v>
                 </c:pt>
+                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1748.62</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1947,11 +1977,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-65023168"/>
-        <c:axId val="-65023712"/>
+        <c:axId val="1980275792"/>
+        <c:axId val="1980278512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-65023168"/>
+        <c:axId val="1980275792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1994,7 +2024,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-65023712"/>
+        <c:crossAx val="1980278512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2002,7 +2032,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-65023712"/>
+        <c:axId val="1980278512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2053,7 +2083,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-65023168"/>
+        <c:crossAx val="1980275792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2245,6 +2275,9 @@
                   <c:pt idx="2">
                     <c:v>05/06</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>06/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2340,7 +2373,7 @@
                   <c:v>0.23479936621722805</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23510297547657491</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2461,6 +2494,9 @@
                   <c:pt idx="2">
                     <c:v>05/06</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>06/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2556,7 +2592,7 @@
                   <c:v>0.23053355406491119</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23083282501441846</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2627,8 +2663,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-65025344"/>
-        <c:axId val="-65020448"/>
+        <c:axId val="11699440"/>
+        <c:axId val="11701072"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2700,6 +2736,9 @@
                         <c:pt idx="2">
                           <c:v>05/06</c:v>
                         </c:pt>
+                        <c:pt idx="3">
+                          <c:v>06/06</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -2795,6 +2834,9 @@
                       </c:pt>
                       <c:pt idx="2" formatCode="General">
                         <c:v>4.05</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="General">
+                        <c:v>4.0599999999999996</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2871,6 +2913,9 @@
                         <c:pt idx="2">
                           <c:v>05/06</c:v>
                         </c:pt>
+                        <c:pt idx="3">
+                          <c:v>06/06</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -2967,6 +3012,9 @@
                       <c:pt idx="2" formatCode="General">
                         <c:v>3.93</c:v>
                       </c:pt>
+                      <c:pt idx="3" formatCode="General">
+                        <c:v>3.94</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -2977,7 +3025,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-65025344"/>
+        <c:axId val="11699440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3020,7 +3068,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-65020448"/>
+        <c:crossAx val="11701072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3028,7 +3076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-65020448"/>
+        <c:axId val="11701072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3079,7 +3127,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-65025344"/>
+        <c:crossAx val="11699440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3175,6 +3223,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3270,6 +3319,9 @@
                   <c:pt idx="2">
                     <c:v>05/06</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>06/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3365,61 +3417,61 @@
                   <c:v>0.13409218659110902</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>0.17889994606105986</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3486,6 +3538,9 @@
                   <c:pt idx="2">
                     <c:v>05/06</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>06/06</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3581,61 +3636,61 @@
                   <c:v>0.1301190847661873</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>0.17360247696116421</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3652,8 +3707,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-65018816"/>
-        <c:axId val="-65032960"/>
+        <c:axId val="11698352"/>
+        <c:axId val="11701616"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3725,6 +3780,9 @@
                         <c:pt idx="2">
                           <c:v>05/06</c:v>
                         </c:pt>
+                        <c:pt idx="3">
+                          <c:v>06/06</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3820,6 +3878,9 @@
                       </c:pt>
                       <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1719.08</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1716.86</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3896,6 +3957,9 @@
                         <c:pt idx="2">
                           <c:v>05/06</c:v>
                         </c:pt>
+                        <c:pt idx="3">
+                          <c:v>06/06</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3992,6 +4056,9 @@
                       <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1750.89</c:v>
                       </c:pt>
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1748.62</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4002,7 +4069,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-65018816"/>
+        <c:axId val="11698352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4045,7 +4112,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-65032960"/>
+        <c:crossAx val="11701616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4053,7 +4120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-65032960"/>
+        <c:axId val="11701616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4104,7 +4171,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-65018816"/>
+        <c:crossAx val="11698352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4118,6 +4185,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7123,7 +7191,7 @@
   <dimension ref="A2:DO11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:I4"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7413,8 +7481,12 @@
       <c r="I3" s="55">
         <v>43621</v>
       </c>
-      <c r="J3" s="20"/>
-      <c r="K3" s="21"/>
+      <c r="J3" s="20">
+        <v>43622</v>
+      </c>
+      <c r="K3" s="21">
+        <v>43622</v>
+      </c>
       <c r="L3" s="22"/>
       <c r="M3" s="23"/>
       <c r="N3" s="22"/>
@@ -7546,14 +7618,18 @@
       <c r="G4" s="15">
         <v>1729.21</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="31">
         <v>4.05</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="32">
         <v>1719.08</v>
       </c>
-      <c r="J4" s="31"/>
-      <c r="K4" s="32"/>
+      <c r="J4" s="31">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="K4" s="32">
+        <v>1716.86</v>
+      </c>
       <c r="L4" s="31"/>
       <c r="M4" s="32"/>
       <c r="N4" s="31"/>
@@ -7685,14 +7761,18 @@
       <c r="G5" s="15">
         <v>1761.23</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="42">
         <v>3.93</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="43">
         <v>1750.89</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15"/>
+      <c r="J5" s="42">
+        <v>3.94</v>
+      </c>
+      <c r="K5" s="43">
+        <v>1748.62</v>
+      </c>
       <c r="L5" s="14"/>
       <c r="M5" s="15"/>
       <c r="N5" s="14"/>
@@ -7765,13 +7845,13 @@
         <f t="shared" ref="I6:I7" si="1">(((H4/365)*$B$7)/100)+G6</f>
         <v>0.13409218659110902</v>
       </c>
-      <c r="J6" s="46" t="e">
+      <c r="J6" s="46">
         <f t="shared" ref="J6" si="2">$B$6/K4</f>
-        <v>#DIV/0!</v>
+        <v>0.23510297547657491</v>
       </c>
       <c r="K6" s="45">
         <f t="shared" ref="K6:K7" si="3">(((J4/365)*$B$7)/100)+I6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="L6" s="46" t="e">
         <f t="shared" ref="L6" si="4">$B$6/M4</f>
@@ -7779,7 +7859,7 @@
       </c>
       <c r="M6" s="45">
         <f t="shared" ref="M6:M7" si="5">(((L4/365)*$B$7)/100)+K6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="N6" s="46" t="e">
         <f t="shared" ref="N6" si="6">$B$6/O4</f>
@@ -7787,7 +7867,7 @@
       </c>
       <c r="O6" s="45">
         <f t="shared" ref="O6:O7" si="7">(((N4/365)*$B$7)/100)+M6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="P6" s="46" t="e">
         <f t="shared" ref="P6" si="8">$B$6/Q4</f>
@@ -7795,7 +7875,7 @@
       </c>
       <c r="Q6" s="45">
         <f t="shared" ref="Q6:Q7" si="9">(((P4/365)*$B$7)/100)+O6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="R6" s="46" t="e">
         <f t="shared" ref="R6" si="10">$B$6/S4</f>
@@ -7803,7 +7883,7 @@
       </c>
       <c r="S6" s="45">
         <f t="shared" ref="S6:S7" si="11">(((R4/365)*$B$7)/100)+Q6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="T6" s="46" t="e">
         <f t="shared" ref="T6" si="12">$B$6/U4</f>
@@ -7811,7 +7891,7 @@
       </c>
       <c r="U6" s="45">
         <f t="shared" ref="U6:U7" si="13">(((T4/365)*$B$7)/100)+S6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="V6" s="46" t="e">
         <f t="shared" ref="V6" si="14">$B$6/W4</f>
@@ -7819,7 +7899,7 @@
       </c>
       <c r="W6" s="45">
         <f t="shared" ref="W6:W7" si="15">(((V4/365)*$B$7)/100)+U6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="X6" s="46" t="e">
         <f t="shared" ref="X6" si="16">$B$6/Y4</f>
@@ -7827,7 +7907,7 @@
       </c>
       <c r="Y6" s="45">
         <f t="shared" ref="Y6:Y7" si="17">(((X4/365)*$B$7)/100)+W6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="Z6" s="46" t="e">
         <f t="shared" ref="Z6" si="18">$B$6/AA4</f>
@@ -7835,7 +7915,7 @@
       </c>
       <c r="AA6" s="45">
         <f t="shared" ref="AA6:AA7" si="19">(((Z4/365)*$B$7)/100)+Y6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="AB6" s="46" t="e">
         <f t="shared" ref="AB6" si="20">$B$6/AC4</f>
@@ -7843,7 +7923,7 @@
       </c>
       <c r="AC6" s="45">
         <f t="shared" ref="AC6:AC7" si="21">(((AB4/365)*$B$7)/100)+AA6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="AD6" s="46" t="e">
         <f t="shared" ref="AD6" si="22">$B$6/AE4</f>
@@ -7851,7 +7931,7 @@
       </c>
       <c r="AE6" s="45">
         <f t="shared" ref="AE6:AE7" si="23">(((AD4/365)*$B$7)/100)+AC6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="AF6" s="46" t="e">
         <f t="shared" ref="AF6" si="24">$B$6/AG4</f>
@@ -7859,7 +7939,7 @@
       </c>
       <c r="AG6" s="45">
         <f t="shared" ref="AG6:AG7" si="25">(((AF4/365)*$B$7)/100)+AE6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="AH6" s="46" t="e">
         <f>$B$6/AI4</f>
@@ -7867,7 +7947,7 @@
       </c>
       <c r="AI6" s="45">
         <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="AJ6" s="46" t="e">
         <f>$B$6/AK4</f>
@@ -7875,7 +7955,7 @@
       </c>
       <c r="AK6" s="45">
         <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="AL6" s="46" t="e">
         <f>$B$6/AM4</f>
@@ -7883,7 +7963,7 @@
       </c>
       <c r="AM6" s="45">
         <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="AN6" s="46" t="e">
         <f>$B$6/AO4</f>
@@ -7891,7 +7971,7 @@
       </c>
       <c r="AO6" s="45">
         <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="AP6" s="46" t="e">
         <f>$B$6/AQ4</f>
@@ -7899,7 +7979,7 @@
       </c>
       <c r="AQ6" s="45">
         <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="AR6" s="46" t="e">
         <f>$B$6/AS4</f>
@@ -7907,7 +7987,7 @@
       </c>
       <c r="AS6" s="45">
         <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="AT6" s="46" t="e">
         <f>$B$6/AU4</f>
@@ -7915,11 +7995,11 @@
       </c>
       <c r="AU6" s="45">
         <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>0.13409218659110902</v>
+        <v>0.17889994606105986</v>
       </c>
       <c r="AV6" s="49">
         <f>AU6-E6</f>
-        <v>8.8953335302414699E-2</v>
+        <v>0.13376109477236553</v>
       </c>
     </row>
     <row r="7" spans="1:119" x14ac:dyDescent="0.25">
@@ -7957,13 +8037,13 @@
         <f t="shared" si="1"/>
         <v>0.1301190847661873</v>
       </c>
-      <c r="J7" s="46" t="e">
+      <c r="J7" s="46">
         <f t="shared" ref="J7" si="34">$B$6/K5</f>
-        <v>#DIV/0!</v>
+        <v>0.23083282501441846</v>
       </c>
       <c r="K7" s="45">
         <f t="shared" si="3"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="L7" s="46" t="e">
         <f t="shared" ref="L7" si="35">$B$6/M5</f>
@@ -7971,7 +8051,7 @@
       </c>
       <c r="M7" s="45">
         <f t="shared" si="5"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="N7" s="46" t="e">
         <f t="shared" ref="N7" si="36">$B$6/O5</f>
@@ -7979,7 +8059,7 @@
       </c>
       <c r="O7" s="45">
         <f t="shared" si="7"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="P7" s="46" t="e">
         <f t="shared" ref="P7" si="37">$B$6/Q5</f>
@@ -7987,7 +8067,7 @@
       </c>
       <c r="Q7" s="45">
         <f t="shared" si="9"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="R7" s="46" t="e">
         <f t="shared" ref="R7" si="38">$B$6/S5</f>
@@ -7995,7 +8075,7 @@
       </c>
       <c r="S7" s="45">
         <f t="shared" si="11"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="T7" s="46" t="e">
         <f t="shared" ref="T7" si="39">$B$6/U5</f>
@@ -8003,7 +8083,7 @@
       </c>
       <c r="U7" s="45">
         <f t="shared" si="13"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="V7" s="46" t="e">
         <f t="shared" ref="V7" si="40">$B$6/W5</f>
@@ -8011,7 +8091,7 @@
       </c>
       <c r="W7" s="45">
         <f t="shared" si="15"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="X7" s="46" t="e">
         <f t="shared" ref="X7" si="41">$B$6/Y5</f>
@@ -8019,7 +8099,7 @@
       </c>
       <c r="Y7" s="45">
         <f t="shared" si="17"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="Z7" s="46" t="e">
         <f t="shared" ref="Z7" si="42">$B$6/AA5</f>
@@ -8027,7 +8107,7 @@
       </c>
       <c r="AA7" s="45">
         <f t="shared" si="19"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="AB7" s="46" t="e">
         <f t="shared" ref="AB7" si="43">$B$6/AC5</f>
@@ -8035,7 +8115,7 @@
       </c>
       <c r="AC7" s="45">
         <f t="shared" si="21"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="AD7" s="46" t="e">
         <f t="shared" ref="AD7" si="44">$B$6/AE5</f>
@@ -8043,7 +8123,7 @@
       </c>
       <c r="AE7" s="45">
         <f t="shared" si="23"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="AF7" s="46" t="e">
         <f>$B$6/AG5</f>
@@ -8051,7 +8131,7 @@
       </c>
       <c r="AG7" s="45">
         <f t="shared" si="25"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="AH7" s="46" t="e">
         <f>$B$6/AI5</f>
@@ -8059,7 +8139,7 @@
       </c>
       <c r="AI7" s="45">
         <f t="shared" si="26"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="AJ7" s="46" t="e">
         <f>$B$6/AK5</f>
@@ -8067,7 +8147,7 @@
       </c>
       <c r="AK7" s="45">
         <f t="shared" si="27"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="AL7" s="46" t="e">
         <f>$B$6/AM5</f>
@@ -8075,7 +8155,7 @@
       </c>
       <c r="AM7" s="45">
         <f t="shared" si="28"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="AN7" s="46" t="e">
         <f>$B$6/AO5</f>
@@ -8083,7 +8163,7 @@
       </c>
       <c r="AO7" s="45">
         <f t="shared" si="29"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="AP7" s="46" t="e">
         <f>$B$6/AQ5</f>
@@ -8091,7 +8171,7 @@
       </c>
       <c r="AQ7" s="45">
         <f t="shared" si="30"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="AR7" s="46" t="e">
         <f>$B$6/AS5</f>
@@ -8099,7 +8179,7 @@
       </c>
       <c r="AS7" s="45">
         <f t="shared" si="31"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="AT7" s="46" t="e">
         <f>$B$6/AU5</f>
@@ -8107,17 +8187,17 @@
       </c>
       <c r="AU7" s="45">
         <f t="shared" si="32"/>
-        <v>0.1301190847661873</v>
+        <v>0.17360247696116421</v>
       </c>
       <c r="AV7" s="49">
         <f>AU7-E7</f>
-        <v>8.6304600752466903E-2</v>
+        <v>0.12978799294744381</v>
       </c>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.25">
       <c r="AV8" s="49">
         <f>AV6-AV7</f>
-        <v>2.6487345499477954E-3</v>
+        <v>3.9731018249217209E-3</v>
       </c>
     </row>
     <row r="10" spans="1:119" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit atualizacao tesouro dia 10/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -626,6 +626,12 @@
                   <c:pt idx="3">
                     <c:v>06/06</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>07/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>10/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -722,6 +728,12 @@
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>4.0599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>4.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -791,6 +803,12 @@
                   <c:pt idx="3">
                     <c:v>06/06</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>07/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>10/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -888,6 +906,12 @@
                 <c:pt idx="3" formatCode="General">
                   <c:v>3.94</c:v>
                 </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>3.93</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>3.93</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -903,8 +927,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1980276336"/>
-        <c:axId val="1980277968"/>
+        <c:axId val="1588244528"/>
+        <c:axId val="1588246160"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -979,6 +1003,12 @@
                         <c:pt idx="3">
                           <c:v>06/06</c:v>
                         </c:pt>
+                        <c:pt idx="4">
+                          <c:v>07/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>10/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1079,10 +1109,10 @@
                         <c:v>0.23510297547657491</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23486904489006116</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23482258784736396</c:v>
                       </c:pt>
                       <c:pt idx="6" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1210,6 +1240,12 @@
                         <c:pt idx="3">
                           <c:v>06/06</c:v>
                         </c:pt>
+                        <c:pt idx="4">
+                          <c:v>07/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>10/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1310,10 +1346,10 @@
                         <c:v>0.23083282501441846</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23060467590865394</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23055989037277438</c:v>
                       </c:pt>
                       <c:pt idx="6" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1373,7 +1409,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1980276336"/>
+        <c:axId val="1588244528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1416,7 +1452,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1980277968"/>
+        <c:crossAx val="1588246160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1424,7 +1460,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1980277968"/>
+        <c:axId val="1588246160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1475,7 +1511,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1980276336"/>
+        <c:crossAx val="1588244528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1700,6 +1736,12 @@
                   <c:pt idx="3">
                     <c:v>06/06</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>07/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>10/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1796,6 +1838,12 @@
                 </c:pt>
                 <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1716.86</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1718.57</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1718.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1865,6 +1913,12 @@
                   <c:pt idx="3">
                     <c:v>06/06</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>07/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>10/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1962,6 +2016,12 @@
                 <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1748.62</c:v>
                 </c:pt>
+                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1750.35</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1750.69</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1977,11 +2037,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1980275792"/>
-        <c:axId val="1980278512"/>
+        <c:axId val="1588259760"/>
+        <c:axId val="1588249424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1980275792"/>
+        <c:axId val="1588259760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2024,7 +2084,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1980278512"/>
+        <c:crossAx val="1588249424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2032,7 +2092,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1980278512"/>
+        <c:axId val="1588249424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2083,7 +2143,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1980275792"/>
+        <c:crossAx val="1588259760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2278,6 +2338,12 @@
                   <c:pt idx="3">
                     <c:v>06/06</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>07/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>10/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2376,10 +2442,10 @@
                   <c:v>0.23510297547657491</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23486904489006116</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23482258784736396</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2497,6 +2563,12 @@
                   <c:pt idx="3">
                     <c:v>06/06</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>07/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>10/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2595,10 +2667,10 @@
                   <c:v>0.23083282501441846</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23060467590865394</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23055989037277438</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2663,8 +2735,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="11699440"/>
-        <c:axId val="11701072"/>
+        <c:axId val="1588258128"/>
+        <c:axId val="1588247792"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2739,6 +2811,12 @@
                         <c:pt idx="3">
                           <c:v>06/06</c:v>
                         </c:pt>
+                        <c:pt idx="4">
+                          <c:v>07/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>10/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -2837,6 +2915,12 @@
                       </c:pt>
                       <c:pt idx="3" formatCode="General">
                         <c:v>4.0599999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="4" formatCode="General">
+                        <c:v>4.05</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="General">
+                        <c:v>4.05</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2916,6 +3000,12 @@
                         <c:pt idx="3">
                           <c:v>06/06</c:v>
                         </c:pt>
+                        <c:pt idx="4">
+                          <c:v>07/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>10/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3015,6 +3105,12 @@
                       <c:pt idx="3" formatCode="General">
                         <c:v>3.94</c:v>
                       </c:pt>
+                      <c:pt idx="4" formatCode="General">
+                        <c:v>3.93</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="General">
+                        <c:v>3.93</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3025,7 +3121,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="11699440"/>
+        <c:axId val="1588258128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3068,7 +3164,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11701072"/>
+        <c:crossAx val="1588247792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3076,7 +3172,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11701072"/>
+        <c:axId val="1588247792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3127,7 +3223,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11699440"/>
+        <c:crossAx val="1588258128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3223,7 +3319,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3322,6 +3417,12 @@
                   <c:pt idx="3">
                     <c:v>06/06</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>07/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>10/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3420,58 +3521,58 @@
                   <c:v>0.17889994606105986</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.22359734159142952</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>0.26829473712179919</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3541,6 +3642,12 @@
                   <c:pt idx="3">
                     <c:v>06/06</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>07/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>10/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3639,58 +3746,58 @@
                   <c:v>0.17360247696116421</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.21697550521655998</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>0.26034853347195575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3707,8 +3814,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="11698352"/>
-        <c:axId val="11701616"/>
+        <c:axId val="1588251056"/>
+        <c:axId val="1588258672"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3783,6 +3890,12 @@
                         <c:pt idx="3">
                           <c:v>06/06</c:v>
                         </c:pt>
+                        <c:pt idx="4">
+                          <c:v>07/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>10/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3881,6 +3994,12 @@
                       </c:pt>
                       <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1716.86</c:v>
+                      </c:pt>
+                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1718.57</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1718.91</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3960,6 +4079,12 @@
                         <c:pt idx="3">
                           <c:v>06/06</c:v>
                         </c:pt>
+                        <c:pt idx="4">
+                          <c:v>07/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>10/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4059,6 +4184,12 @@
                       <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1748.62</c:v>
                       </c:pt>
+                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1750.35</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1750.69</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4069,7 +4200,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="11698352"/>
+        <c:axId val="1588251056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4112,7 +4243,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11701616"/>
+        <c:crossAx val="1588258672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4120,7 +4251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11701616"/>
+        <c:axId val="1588258672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4171,7 +4302,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11698352"/>
+        <c:crossAx val="1588251056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4185,7 +4316,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7190,8 +7320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7487,10 +7617,18 @@
       <c r="K3" s="21">
         <v>43622</v>
       </c>
-      <c r="L3" s="22"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="23"/>
+      <c r="L3" s="22">
+        <v>43623</v>
+      </c>
+      <c r="M3" s="23">
+        <v>43623</v>
+      </c>
+      <c r="N3" s="22">
+        <v>43626</v>
+      </c>
+      <c r="O3" s="23">
+        <v>43626</v>
+      </c>
       <c r="P3" s="22"/>
       <c r="Q3" s="23"/>
       <c r="R3" s="22"/>
@@ -7630,10 +7768,18 @@
       <c r="K4" s="32">
         <v>1716.86</v>
       </c>
-      <c r="L4" s="31"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="32"/>
+      <c r="L4" s="31">
+        <v>4.05</v>
+      </c>
+      <c r="M4" s="32">
+        <v>1718.57</v>
+      </c>
+      <c r="N4" s="31">
+        <v>4.05</v>
+      </c>
+      <c r="O4" s="32">
+        <v>1718.91</v>
+      </c>
       <c r="P4" s="31"/>
       <c r="Q4" s="32"/>
       <c r="R4" s="31"/>
@@ -7773,10 +7919,18 @@
       <c r="K5" s="43">
         <v>1748.62</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="15"/>
+      <c r="L5" s="42">
+        <v>3.93</v>
+      </c>
+      <c r="M5" s="15">
+        <v>1750.35</v>
+      </c>
+      <c r="N5" s="42">
+        <v>3.93</v>
+      </c>
+      <c r="O5" s="15">
+        <v>1750.69</v>
+      </c>
       <c r="P5" s="14"/>
       <c r="Q5" s="15"/>
       <c r="R5" s="14"/>
@@ -7853,21 +8007,21 @@
         <f t="shared" ref="K6:K7" si="3">(((J4/365)*$B$7)/100)+I6</f>
         <v>0.17889994606105986</v>
       </c>
-      <c r="L6" s="46" t="e">
+      <c r="L6" s="46">
         <f t="shared" ref="L6" si="4">$B$6/M4</f>
-        <v>#DIV/0!</v>
+        <v>0.23486904489006116</v>
       </c>
       <c r="M6" s="45">
         <f t="shared" ref="M6:M7" si="5">(((L4/365)*$B$7)/100)+K6</f>
-        <v>0.17889994606105986</v>
-      </c>
-      <c r="N6" s="46" t="e">
+        <v>0.22359734159142952</v>
+      </c>
+      <c r="N6" s="46">
         <f t="shared" ref="N6" si="6">$B$6/O4</f>
-        <v>#DIV/0!</v>
+        <v>0.23482258784736396</v>
       </c>
       <c r="O6" s="45">
         <f t="shared" ref="O6:O7" si="7">(((N4/365)*$B$7)/100)+M6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="P6" s="46" t="e">
         <f t="shared" ref="P6" si="8">$B$6/Q4</f>
@@ -7875,7 +8029,7 @@
       </c>
       <c r="Q6" s="45">
         <f t="shared" ref="Q6:Q7" si="9">(((P4/365)*$B$7)/100)+O6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="R6" s="46" t="e">
         <f t="shared" ref="R6" si="10">$B$6/S4</f>
@@ -7883,7 +8037,7 @@
       </c>
       <c r="S6" s="45">
         <f t="shared" ref="S6:S7" si="11">(((R4/365)*$B$7)/100)+Q6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="T6" s="46" t="e">
         <f t="shared" ref="T6" si="12">$B$6/U4</f>
@@ -7891,7 +8045,7 @@
       </c>
       <c r="U6" s="45">
         <f t="shared" ref="U6:U7" si="13">(((T4/365)*$B$7)/100)+S6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="V6" s="46" t="e">
         <f t="shared" ref="V6" si="14">$B$6/W4</f>
@@ -7899,7 +8053,7 @@
       </c>
       <c r="W6" s="45">
         <f t="shared" ref="W6:W7" si="15">(((V4/365)*$B$7)/100)+U6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="X6" s="46" t="e">
         <f t="shared" ref="X6" si="16">$B$6/Y4</f>
@@ -7907,7 +8061,7 @@
       </c>
       <c r="Y6" s="45">
         <f t="shared" ref="Y6:Y7" si="17">(((X4/365)*$B$7)/100)+W6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="Z6" s="46" t="e">
         <f t="shared" ref="Z6" si="18">$B$6/AA4</f>
@@ -7915,7 +8069,7 @@
       </c>
       <c r="AA6" s="45">
         <f t="shared" ref="AA6:AA7" si="19">(((Z4/365)*$B$7)/100)+Y6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="AB6" s="46" t="e">
         <f t="shared" ref="AB6" si="20">$B$6/AC4</f>
@@ -7923,7 +8077,7 @@
       </c>
       <c r="AC6" s="45">
         <f t="shared" ref="AC6:AC7" si="21">(((AB4/365)*$B$7)/100)+AA6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="AD6" s="46" t="e">
         <f t="shared" ref="AD6" si="22">$B$6/AE4</f>
@@ -7931,7 +8085,7 @@
       </c>
       <c r="AE6" s="45">
         <f t="shared" ref="AE6:AE7" si="23">(((AD4/365)*$B$7)/100)+AC6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="AF6" s="46" t="e">
         <f t="shared" ref="AF6" si="24">$B$6/AG4</f>
@@ -7939,7 +8093,7 @@
       </c>
       <c r="AG6" s="45">
         <f t="shared" ref="AG6:AG7" si="25">(((AF4/365)*$B$7)/100)+AE6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="AH6" s="46" t="e">
         <f>$B$6/AI4</f>
@@ -7947,7 +8101,7 @@
       </c>
       <c r="AI6" s="45">
         <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="AJ6" s="46" t="e">
         <f>$B$6/AK4</f>
@@ -7955,7 +8109,7 @@
       </c>
       <c r="AK6" s="45">
         <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="AL6" s="46" t="e">
         <f>$B$6/AM4</f>
@@ -7963,7 +8117,7 @@
       </c>
       <c r="AM6" s="45">
         <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="AN6" s="46" t="e">
         <f>$B$6/AO4</f>
@@ -7971,7 +8125,7 @@
       </c>
       <c r="AO6" s="45">
         <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="AP6" s="46" t="e">
         <f>$B$6/AQ4</f>
@@ -7979,7 +8133,7 @@
       </c>
       <c r="AQ6" s="45">
         <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="AR6" s="46" t="e">
         <f>$B$6/AS4</f>
@@ -7987,7 +8141,7 @@
       </c>
       <c r="AS6" s="45">
         <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="AT6" s="46" t="e">
         <f>$B$6/AU4</f>
@@ -7995,11 +8149,11 @@
       </c>
       <c r="AU6" s="45">
         <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>0.17889994606105986</v>
+        <v>0.26829473712179919</v>
       </c>
       <c r="AV6" s="49">
         <f>AU6-E6</f>
-        <v>0.13376109477236553</v>
+        <v>0.22315588583310486</v>
       </c>
     </row>
     <row r="7" spans="1:119" x14ac:dyDescent="0.25">
@@ -8045,21 +8199,21 @@
         <f t="shared" si="3"/>
         <v>0.17360247696116421</v>
       </c>
-      <c r="L7" s="46" t="e">
+      <c r="L7" s="46">
         <f t="shared" ref="L7" si="35">$B$6/M5</f>
-        <v>#DIV/0!</v>
+        <v>0.23060467590865394</v>
       </c>
       <c r="M7" s="45">
         <f t="shared" si="5"/>
-        <v>0.17360247696116421</v>
-      </c>
-      <c r="N7" s="46" t="e">
+        <v>0.21697550521655998</v>
+      </c>
+      <c r="N7" s="46">
         <f t="shared" ref="N7" si="36">$B$6/O5</f>
-        <v>#DIV/0!</v>
+        <v>0.23055989037277438</v>
       </c>
       <c r="O7" s="45">
         <f t="shared" si="7"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="P7" s="46" t="e">
         <f t="shared" ref="P7" si="37">$B$6/Q5</f>
@@ -8067,7 +8221,7 @@
       </c>
       <c r="Q7" s="45">
         <f t="shared" si="9"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="R7" s="46" t="e">
         <f t="shared" ref="R7" si="38">$B$6/S5</f>
@@ -8075,7 +8229,7 @@
       </c>
       <c r="S7" s="45">
         <f t="shared" si="11"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="T7" s="46" t="e">
         <f t="shared" ref="T7" si="39">$B$6/U5</f>
@@ -8083,7 +8237,7 @@
       </c>
       <c r="U7" s="45">
         <f t="shared" si="13"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="V7" s="46" t="e">
         <f t="shared" ref="V7" si="40">$B$6/W5</f>
@@ -8091,7 +8245,7 @@
       </c>
       <c r="W7" s="45">
         <f t="shared" si="15"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="X7" s="46" t="e">
         <f t="shared" ref="X7" si="41">$B$6/Y5</f>
@@ -8099,7 +8253,7 @@
       </c>
       <c r="Y7" s="45">
         <f t="shared" si="17"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="Z7" s="46" t="e">
         <f t="shared" ref="Z7" si="42">$B$6/AA5</f>
@@ -8107,7 +8261,7 @@
       </c>
       <c r="AA7" s="45">
         <f t="shared" si="19"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="AB7" s="46" t="e">
         <f t="shared" ref="AB7" si="43">$B$6/AC5</f>
@@ -8115,7 +8269,7 @@
       </c>
       <c r="AC7" s="45">
         <f t="shared" si="21"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="AD7" s="46" t="e">
         <f t="shared" ref="AD7" si="44">$B$6/AE5</f>
@@ -8123,7 +8277,7 @@
       </c>
       <c r="AE7" s="45">
         <f t="shared" si="23"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="AF7" s="46" t="e">
         <f>$B$6/AG5</f>
@@ -8131,7 +8285,7 @@
       </c>
       <c r="AG7" s="45">
         <f t="shared" si="25"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="AH7" s="46" t="e">
         <f>$B$6/AI5</f>
@@ -8139,7 +8293,7 @@
       </c>
       <c r="AI7" s="45">
         <f t="shared" si="26"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="AJ7" s="46" t="e">
         <f>$B$6/AK5</f>
@@ -8147,7 +8301,7 @@
       </c>
       <c r="AK7" s="45">
         <f t="shared" si="27"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="AL7" s="46" t="e">
         <f>$B$6/AM5</f>
@@ -8155,7 +8309,7 @@
       </c>
       <c r="AM7" s="45">
         <f t="shared" si="28"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="AN7" s="46" t="e">
         <f>$B$6/AO5</f>
@@ -8163,7 +8317,7 @@
       </c>
       <c r="AO7" s="45">
         <f t="shared" si="29"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="AP7" s="46" t="e">
         <f>$B$6/AQ5</f>
@@ -8171,7 +8325,7 @@
       </c>
       <c r="AQ7" s="45">
         <f t="shared" si="30"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="AR7" s="46" t="e">
         <f>$B$6/AS5</f>
@@ -8179,7 +8333,7 @@
       </c>
       <c r="AS7" s="45">
         <f t="shared" si="31"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="AT7" s="46" t="e">
         <f>$B$6/AU5</f>
@@ -8187,17 +8341,17 @@
       </c>
       <c r="AU7" s="45">
         <f t="shared" si="32"/>
-        <v>0.17360247696116421</v>
+        <v>0.26034853347195575</v>
       </c>
       <c r="AV7" s="49">
         <f>AU7-E7</f>
-        <v>0.12978799294744381</v>
+        <v>0.21653404945823534</v>
       </c>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.25">
       <c r="AV8" s="49">
         <f>AV6-AV7</f>
-        <v>3.9731018249217209E-3</v>
+        <v>6.6218363748695164E-3</v>
       </c>
     </row>
     <row r="10" spans="1:119" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit atualizacao tesouro 11/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -632,6 +632,9 @@
                   <c:pt idx="5">
                     <c:v>10/jun</c:v>
                   </c:pt>
+                  <c:pt idx="6">
+                    <c:v>11/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -734,6 +737,9 @@
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
                   <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>4.0199999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -809,6 +815,9 @@
                   <c:pt idx="5">
                     <c:v>10/jun</c:v>
                   </c:pt>
+                  <c:pt idx="6">
+                    <c:v>11/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -912,6 +921,9 @@
                 <c:pt idx="5" formatCode="General">
                   <c:v>3.93</c:v>
                 </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>3.9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -927,8 +939,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1588244528"/>
-        <c:axId val="1588246160"/>
+        <c:axId val="-1900239456"/>
+        <c:axId val="-1900240000"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1009,6 +1021,9 @@
                         <c:pt idx="5">
                           <c:v>10/jun</c:v>
                         </c:pt>
+                        <c:pt idx="6">
+                          <c:v>11/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1115,7 +1130,7 @@
                         <c:v>0.23482258784736396</c:v>
                       </c:pt>
                       <c:pt idx="6" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.233703634028922</c:v>
                       </c:pt>
                       <c:pt idx="7" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1246,6 +1261,9 @@
                         <c:pt idx="5">
                           <c:v>10/jun</c:v>
                         </c:pt>
+                        <c:pt idx="6">
+                          <c:v>11/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1352,7 +1370,7 @@
                         <c:v>0.23055989037277438</c:v>
                       </c:pt>
                       <c:pt idx="6" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.2294602260708509</c:v>
                       </c:pt>
                       <c:pt idx="7" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1409,7 +1427,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1588244528"/>
+        <c:axId val="-1900239456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1452,7 +1470,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1588246160"/>
+        <c:crossAx val="-1900240000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1460,7 +1478,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1588246160"/>
+        <c:axId val="-1900240000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1511,7 +1529,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1588244528"/>
+        <c:crossAx val="-1900239456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1742,6 +1760,9 @@
                   <c:pt idx="5">
                     <c:v>10/jun</c:v>
                   </c:pt>
+                  <c:pt idx="6">
+                    <c:v>11/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1844,6 +1865,9 @@
                 </c:pt>
                 <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1718.91</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1727.14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1919,6 +1943,9 @@
                   <c:pt idx="5">
                     <c:v>10/jun</c:v>
                   </c:pt>
+                  <c:pt idx="6">
+                    <c:v>11/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2022,6 +2049,9 @@
                 <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1750.69</c:v>
                 </c:pt>
+                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1759.08</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2037,11 +2067,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1588259760"/>
-        <c:axId val="1588249424"/>
+        <c:axId val="-1900233472"/>
+        <c:axId val="-1900243264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1588259760"/>
+        <c:axId val="-1900233472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2084,7 +2114,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1588249424"/>
+        <c:crossAx val="-1900243264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2092,7 +2122,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1588249424"/>
+        <c:axId val="-1900243264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2143,7 +2173,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1588259760"/>
+        <c:crossAx val="-1900233472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2344,6 +2374,9 @@
                   <c:pt idx="5">
                     <c:v>10/jun</c:v>
                   </c:pt>
+                  <c:pt idx="6">
+                    <c:v>11/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2448,7 +2481,7 @@
                   <c:v>0.23482258784736396</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.233703634028922</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2569,6 +2602,9 @@
                   <c:pt idx="5">
                     <c:v>10/jun</c:v>
                   </c:pt>
+                  <c:pt idx="6">
+                    <c:v>11/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2673,7 +2709,7 @@
                   <c:v>0.23055989037277438</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.2294602260708509</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2735,8 +2771,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1588258128"/>
-        <c:axId val="1588247792"/>
+        <c:axId val="-1900232928"/>
+        <c:axId val="-1900241632"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2817,6 +2853,9 @@
                         <c:pt idx="5">
                           <c:v>10/jun</c:v>
                         </c:pt>
+                        <c:pt idx="6">
+                          <c:v>11/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -2921,6 +2960,9 @@
                       </c:pt>
                       <c:pt idx="5" formatCode="General">
                         <c:v>4.05</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="General">
+                        <c:v>4.0199999999999996</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3006,6 +3048,9 @@
                         <c:pt idx="5">
                           <c:v>10/jun</c:v>
                         </c:pt>
+                        <c:pt idx="6">
+                          <c:v>11/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3111,6 +3156,9 @@
                       <c:pt idx="5" formatCode="General">
                         <c:v>3.93</c:v>
                       </c:pt>
+                      <c:pt idx="6" formatCode="General">
+                        <c:v>3.9</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3121,7 +3169,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1588258128"/>
+        <c:axId val="-1900232928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3164,7 +3212,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1588247792"/>
+        <c:crossAx val="-1900241632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3172,7 +3220,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1588247792"/>
+        <c:axId val="-1900241632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3223,7 +3271,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1588258128"/>
+        <c:crossAx val="-1900232928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3319,6 +3367,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3423,6 +3472,9 @@
                   <c:pt idx="5">
                     <c:v>10/jun</c:v>
                   </c:pt>
+                  <c:pt idx="6">
+                    <c:v>11/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3527,52 +3579,52 @@
                   <c:v>0.26829473712179919</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>0.31266104083342539</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3648,6 +3700,9 @@
                   <c:pt idx="5">
                     <c:v>10/jun</c:v>
                   </c:pt>
+                  <c:pt idx="6">
+                    <c:v>11/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3752,52 +3807,52 @@
                   <c:v>0.26034853347195575</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>0.30339046990860802</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3814,8 +3869,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1588251056"/>
-        <c:axId val="1588258672"/>
+        <c:axId val="-1900230208"/>
+        <c:axId val="-1900244352"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3896,6 +3951,9 @@
                         <c:pt idx="5">
                           <c:v>10/jun</c:v>
                         </c:pt>
+                        <c:pt idx="6">
+                          <c:v>11/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4000,6 +4058,9 @@
                       </c:pt>
                       <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1718.91</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1727.14</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4085,6 +4146,9 @@
                         <c:pt idx="5">
                           <c:v>10/jun</c:v>
                         </c:pt>
+                        <c:pt idx="6">
+                          <c:v>11/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4190,6 +4254,9 @@
                       <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1750.69</c:v>
                       </c:pt>
+                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1759.08</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4200,7 +4267,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1588251056"/>
+        <c:axId val="-1900230208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4243,7 +4310,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1588258672"/>
+        <c:crossAx val="-1900244352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4251,7 +4318,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1588258672"/>
+        <c:axId val="-1900244352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4302,7 +4369,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1588251056"/>
+        <c:crossAx val="-1900230208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4316,6 +4383,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7320,8 +7388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4:Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7629,8 +7697,12 @@
       <c r="O3" s="23">
         <v>43626</v>
       </c>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="23"/>
+      <c r="P3" s="22">
+        <v>43627</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>43627</v>
+      </c>
       <c r="R3" s="22"/>
       <c r="S3" s="23"/>
       <c r="T3" s="22"/>
@@ -7780,8 +7852,12 @@
       <c r="O4" s="32">
         <v>1718.91</v>
       </c>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="32"/>
+      <c r="P4" s="31">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="Q4" s="32">
+        <v>1727.14</v>
+      </c>
       <c r="R4" s="31"/>
       <c r="S4" s="32"/>
       <c r="T4" s="31"/>
@@ -7931,8 +8007,12 @@
       <c r="O5" s="15">
         <v>1750.69</v>
       </c>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="15"/>
+      <c r="P5" s="42">
+        <v>3.9</v>
+      </c>
+      <c r="Q5" s="43">
+        <v>1759.08</v>
+      </c>
       <c r="R5" s="14"/>
       <c r="S5" s="15"/>
       <c r="T5" s="14"/>
@@ -8023,13 +8103,13 @@
         <f t="shared" ref="O6:O7" si="7">(((N4/365)*$B$7)/100)+M6</f>
         <v>0.26829473712179919</v>
       </c>
-      <c r="P6" s="46" t="e">
+      <c r="P6" s="46">
         <f t="shared" ref="P6" si="8">$B$6/Q4</f>
-        <v>#DIV/0!</v>
+        <v>0.233703634028922</v>
       </c>
       <c r="Q6" s="45">
         <f t="shared" ref="Q6:Q7" si="9">(((P4/365)*$B$7)/100)+O6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="R6" s="46" t="e">
         <f t="shared" ref="R6" si="10">$B$6/S4</f>
@@ -8037,7 +8117,7 @@
       </c>
       <c r="S6" s="45">
         <f t="shared" ref="S6:S7" si="11">(((R4/365)*$B$7)/100)+Q6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="T6" s="46" t="e">
         <f t="shared" ref="T6" si="12">$B$6/U4</f>
@@ -8045,7 +8125,7 @@
       </c>
       <c r="U6" s="45">
         <f t="shared" ref="U6:U7" si="13">(((T4/365)*$B$7)/100)+S6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="V6" s="46" t="e">
         <f t="shared" ref="V6" si="14">$B$6/W4</f>
@@ -8053,7 +8133,7 @@
       </c>
       <c r="W6" s="45">
         <f t="shared" ref="W6:W7" si="15">(((V4/365)*$B$7)/100)+U6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="X6" s="46" t="e">
         <f t="shared" ref="X6" si="16">$B$6/Y4</f>
@@ -8061,7 +8141,7 @@
       </c>
       <c r="Y6" s="45">
         <f t="shared" ref="Y6:Y7" si="17">(((X4/365)*$B$7)/100)+W6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="Z6" s="46" t="e">
         <f t="shared" ref="Z6" si="18">$B$6/AA4</f>
@@ -8069,7 +8149,7 @@
       </c>
       <c r="AA6" s="45">
         <f t="shared" ref="AA6:AA7" si="19">(((Z4/365)*$B$7)/100)+Y6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="AB6" s="46" t="e">
         <f t="shared" ref="AB6" si="20">$B$6/AC4</f>
@@ -8077,7 +8157,7 @@
       </c>
       <c r="AC6" s="45">
         <f t="shared" ref="AC6:AC7" si="21">(((AB4/365)*$B$7)/100)+AA6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="AD6" s="46" t="e">
         <f t="shared" ref="AD6" si="22">$B$6/AE4</f>
@@ -8085,7 +8165,7 @@
       </c>
       <c r="AE6" s="45">
         <f t="shared" ref="AE6:AE7" si="23">(((AD4/365)*$B$7)/100)+AC6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="AF6" s="46" t="e">
         <f t="shared" ref="AF6" si="24">$B$6/AG4</f>
@@ -8093,7 +8173,7 @@
       </c>
       <c r="AG6" s="45">
         <f t="shared" ref="AG6:AG7" si="25">(((AF4/365)*$B$7)/100)+AE6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="AH6" s="46" t="e">
         <f>$B$6/AI4</f>
@@ -8101,7 +8181,7 @@
       </c>
       <c r="AI6" s="45">
         <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="AJ6" s="46" t="e">
         <f>$B$6/AK4</f>
@@ -8109,7 +8189,7 @@
       </c>
       <c r="AK6" s="45">
         <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="AL6" s="46" t="e">
         <f>$B$6/AM4</f>
@@ -8117,7 +8197,7 @@
       </c>
       <c r="AM6" s="45">
         <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="AN6" s="46" t="e">
         <f>$B$6/AO4</f>
@@ -8125,7 +8205,7 @@
       </c>
       <c r="AO6" s="45">
         <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="AP6" s="46" t="e">
         <f>$B$6/AQ4</f>
@@ -8133,7 +8213,7 @@
       </c>
       <c r="AQ6" s="45">
         <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="AR6" s="46" t="e">
         <f>$B$6/AS4</f>
@@ -8141,7 +8221,7 @@
       </c>
       <c r="AS6" s="45">
         <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="AT6" s="46" t="e">
         <f>$B$6/AU4</f>
@@ -8149,11 +8229,11 @@
       </c>
       <c r="AU6" s="45">
         <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>0.26829473712179919</v>
+        <v>0.31266104083342539</v>
       </c>
       <c r="AV6" s="49">
         <f>AU6-E6</f>
-        <v>0.22315588583310486</v>
+        <v>0.26752218954473106</v>
       </c>
     </row>
     <row r="7" spans="1:119" x14ac:dyDescent="0.25">
@@ -8215,13 +8295,13 @@
         <f t="shared" si="7"/>
         <v>0.26034853347195575</v>
       </c>
-      <c r="P7" s="46" t="e">
+      <c r="P7" s="46">
         <f t="shared" ref="P7" si="37">$B$6/Q5</f>
-        <v>#DIV/0!</v>
+        <v>0.2294602260708509</v>
       </c>
       <c r="Q7" s="45">
         <f t="shared" si="9"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="R7" s="46" t="e">
         <f t="shared" ref="R7" si="38">$B$6/S5</f>
@@ -8229,7 +8309,7 @@
       </c>
       <c r="S7" s="45">
         <f t="shared" si="11"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="T7" s="46" t="e">
         <f t="shared" ref="T7" si="39">$B$6/U5</f>
@@ -8237,7 +8317,7 @@
       </c>
       <c r="U7" s="45">
         <f t="shared" si="13"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="V7" s="46" t="e">
         <f t="shared" ref="V7" si="40">$B$6/W5</f>
@@ -8245,7 +8325,7 @@
       </c>
       <c r="W7" s="45">
         <f t="shared" si="15"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="X7" s="46" t="e">
         <f t="shared" ref="X7" si="41">$B$6/Y5</f>
@@ -8253,7 +8333,7 @@
       </c>
       <c r="Y7" s="45">
         <f t="shared" si="17"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="Z7" s="46" t="e">
         <f t="shared" ref="Z7" si="42">$B$6/AA5</f>
@@ -8261,7 +8341,7 @@
       </c>
       <c r="AA7" s="45">
         <f t="shared" si="19"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="AB7" s="46" t="e">
         <f t="shared" ref="AB7" si="43">$B$6/AC5</f>
@@ -8269,7 +8349,7 @@
       </c>
       <c r="AC7" s="45">
         <f t="shared" si="21"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="AD7" s="46" t="e">
         <f t="shared" ref="AD7" si="44">$B$6/AE5</f>
@@ -8277,7 +8357,7 @@
       </c>
       <c r="AE7" s="45">
         <f t="shared" si="23"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="AF7" s="46" t="e">
         <f>$B$6/AG5</f>
@@ -8285,7 +8365,7 @@
       </c>
       <c r="AG7" s="45">
         <f t="shared" si="25"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="AH7" s="46" t="e">
         <f>$B$6/AI5</f>
@@ -8293,7 +8373,7 @@
       </c>
       <c r="AI7" s="45">
         <f t="shared" si="26"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="AJ7" s="46" t="e">
         <f>$B$6/AK5</f>
@@ -8301,7 +8381,7 @@
       </c>
       <c r="AK7" s="45">
         <f t="shared" si="27"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="AL7" s="46" t="e">
         <f>$B$6/AM5</f>
@@ -8309,7 +8389,7 @@
       </c>
       <c r="AM7" s="45">
         <f t="shared" si="28"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="AN7" s="46" t="e">
         <f>$B$6/AO5</f>
@@ -8317,7 +8397,7 @@
       </c>
       <c r="AO7" s="45">
         <f t="shared" si="29"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="AP7" s="46" t="e">
         <f>$B$6/AQ5</f>
@@ -8325,7 +8405,7 @@
       </c>
       <c r="AQ7" s="45">
         <f t="shared" si="30"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="AR7" s="46" t="e">
         <f>$B$6/AS5</f>
@@ -8333,7 +8413,7 @@
       </c>
       <c r="AS7" s="45">
         <f t="shared" si="31"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="AT7" s="46" t="e">
         <f>$B$6/AU5</f>
@@ -8341,17 +8421,17 @@
       </c>
       <c r="AU7" s="45">
         <f t="shared" si="32"/>
-        <v>0.26034853347195575</v>
+        <v>0.30339046990860802</v>
       </c>
       <c r="AV7" s="49">
         <f>AU7-E7</f>
-        <v>0.21653404945823534</v>
+        <v>0.25957598589488762</v>
       </c>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.25">
       <c r="AV8" s="49">
         <f>AV6-AV7</f>
-        <v>6.6218363748695164E-3</v>
+        <v>7.9462036498434419E-3</v>
       </c>
     </row>
     <row r="10" spans="1:119" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit atualizacao tesouro dia 13/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -527,7 +527,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -635,6 +634,12 @@
                   <c:pt idx="6">
                     <c:v>11/jun</c:v>
                   </c:pt>
+                  <c:pt idx="7">
+                    <c:v>12/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>13/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -739,6 +744,12 @@
                   <c:v>4.05</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
                   <c:v>4.0199999999999996</c:v>
                 </c:pt>
               </c:numCache>
@@ -818,6 +829,12 @@
                   <c:pt idx="6">
                     <c:v>11/jun</c:v>
                   </c:pt>
+                  <c:pt idx="7">
+                    <c:v>12/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>13/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -924,6 +941,12 @@
                 <c:pt idx="6" formatCode="General">
                   <c:v>3.9</c:v>
                 </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>3.89</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>3.9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -939,8 +962,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1900239456"/>
-        <c:axId val="-1900240000"/>
+        <c:axId val="-1276850832"/>
+        <c:axId val="-1276853008"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1024,6 +1047,12 @@
                         <c:pt idx="6">
                           <c:v>11/jun</c:v>
                         </c:pt>
+                        <c:pt idx="7">
+                          <c:v>12/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>13/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1133,10 +1162,10 @@
                         <c:v>0.233703634028922</c:v>
                       </c:pt>
                       <c:pt idx="7" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23330109730926896</c:v>
                       </c:pt>
                       <c:pt idx="8" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23361030568789315</c:v>
                       </c:pt>
                       <c:pt idx="9" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1264,6 +1293,12 @@
                         <c:pt idx="6">
                           <c:v>11/jun</c:v>
                         </c:pt>
+                        <c:pt idx="7">
+                          <c:v>12/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>13/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1373,10 +1408,10 @@
                         <c:v>0.2294602260708509</c:v>
                       </c:pt>
                       <c:pt idx="7" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22906566245961513</c:v>
                       </c:pt>
                       <c:pt idx="8" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22937155889252647</c:v>
                       </c:pt>
                       <c:pt idx="9" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1427,7 +1462,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1900239456"/>
+        <c:axId val="-1276850832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1470,7 +1505,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1900240000"/>
+        <c:crossAx val="-1276853008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1478,7 +1513,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1900240000"/>
+        <c:axId val="-1276853008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1529,7 +1564,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1900239456"/>
+        <c:crossAx val="-1276850832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1543,7 +1578,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1655,7 +1689,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1763,6 +1796,12 @@
                   <c:pt idx="6">
                     <c:v>11/jun</c:v>
                   </c:pt>
+                  <c:pt idx="7">
+                    <c:v>12/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>13/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1868,6 +1907,12 @@
                 </c:pt>
                 <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1727.14</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1730.12</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1727.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1946,6 +1991,12 @@
                   <c:pt idx="6">
                     <c:v>11/jun</c:v>
                   </c:pt>
+                  <c:pt idx="7">
+                    <c:v>12/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>13/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2052,6 +2103,12 @@
                 <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1759.08</c:v>
                 </c:pt>
+                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1762.11</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1759.76</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2067,11 +2124,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1900233472"/>
-        <c:axId val="-1900243264"/>
+        <c:axId val="-1276838864"/>
+        <c:axId val="-1276848656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1900233472"/>
+        <c:axId val="-1276838864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2114,7 +2171,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1900243264"/>
+        <c:crossAx val="-1276848656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2122,7 +2179,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1900243264"/>
+        <c:axId val="-1276848656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2173,7 +2230,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1900233472"/>
+        <c:crossAx val="-1276838864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2187,7 +2244,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2377,6 +2433,12 @@
                   <c:pt idx="6">
                     <c:v>11/jun</c:v>
                   </c:pt>
+                  <c:pt idx="7">
+                    <c:v>12/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>13/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2484,10 +2546,10 @@
                   <c:v>0.233703634028922</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23330109730926896</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23361030568789315</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2605,6 +2667,12 @@
                   <c:pt idx="6">
                     <c:v>11/jun</c:v>
                   </c:pt>
+                  <c:pt idx="7">
+                    <c:v>12/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>13/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2712,10 +2780,10 @@
                   <c:v>0.2294602260708509</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22906566245961513</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22937155889252647</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2771,8 +2839,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1900232928"/>
-        <c:axId val="-1900241632"/>
+        <c:axId val="-1276847568"/>
+        <c:axId val="-1276841040"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2856,6 +2924,12 @@
                         <c:pt idx="6">
                           <c:v>11/jun</c:v>
                         </c:pt>
+                        <c:pt idx="7">
+                          <c:v>12/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>13/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -2962,6 +3036,12 @@
                         <c:v>4.05</c:v>
                       </c:pt>
                       <c:pt idx="6" formatCode="General">
+                        <c:v>4.0199999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="7" formatCode="General">
+                        <c:v>4.01</c:v>
+                      </c:pt>
+                      <c:pt idx="8" formatCode="General">
                         <c:v>4.0199999999999996</c:v>
                       </c:pt>
                     </c:numCache>
@@ -3051,6 +3131,12 @@
                         <c:pt idx="6">
                           <c:v>11/jun</c:v>
                         </c:pt>
+                        <c:pt idx="7">
+                          <c:v>12/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>13/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3159,6 +3245,12 @@
                       <c:pt idx="6" formatCode="General">
                         <c:v>3.9</c:v>
                       </c:pt>
+                      <c:pt idx="7" formatCode="General">
+                        <c:v>3.89</c:v>
+                      </c:pt>
+                      <c:pt idx="8" formatCode="General">
+                        <c:v>3.9</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3169,7 +3261,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1900232928"/>
+        <c:axId val="-1276847568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3212,7 +3304,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1900241632"/>
+        <c:crossAx val="-1276841040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3220,7 +3312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1900241632"/>
+        <c:axId val="-1276841040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3271,7 +3363,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1900232928"/>
+        <c:crossAx val="-1276847568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3367,7 +3459,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3475,6 +3566,12 @@
                   <c:pt idx="6">
                     <c:v>11/jun</c:v>
                   </c:pt>
+                  <c:pt idx="7">
+                    <c:v>12/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>13/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3582,49 +3679,49 @@
                   <c:v>0.31266104083342539</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.35691698060547045</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>0.40128328431709664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3703,6 +3800,12 @@
                   <c:pt idx="6">
                     <c:v>11/jun</c:v>
                   </c:pt>
+                  <c:pt idx="7">
+                    <c:v>12/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>13/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3810,49 +3913,49 @@
                   <c:v>0.30339046990860802</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.34632204240567915</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>0.38936397884233143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3869,8 +3972,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1900230208"/>
-        <c:axId val="-1900244352"/>
+        <c:axId val="-1276853552"/>
+        <c:axId val="-1276850288"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3954,6 +4057,12 @@
                         <c:pt idx="6">
                           <c:v>11/jun</c:v>
                         </c:pt>
+                        <c:pt idx="7">
+                          <c:v>12/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>13/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4061,6 +4170,12 @@
                       </c:pt>
                       <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1727.14</c:v>
+                      </c:pt>
+                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1730.12</c:v>
+                      </c:pt>
+                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1727.83</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4149,6 +4264,12 @@
                         <c:pt idx="6">
                           <c:v>11/jun</c:v>
                         </c:pt>
+                        <c:pt idx="7">
+                          <c:v>12/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>13/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4257,6 +4378,12 @@
                       <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1759.08</c:v>
                       </c:pt>
+                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1762.11</c:v>
+                      </c:pt>
+                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1759.76</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4267,7 +4394,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1900230208"/>
+        <c:axId val="-1276853552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4310,7 +4437,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1900244352"/>
+        <c:crossAx val="-1276850288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4318,7 +4445,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1900244352"/>
+        <c:axId val="-1276850288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4369,7 +4496,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1900230208"/>
+        <c:crossAx val="-1276853552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4383,7 +4510,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7388,8 +7514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4:Q5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4:U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7703,10 +7829,18 @@
       <c r="Q3" s="23">
         <v>43627</v>
       </c>
-      <c r="R3" s="22"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="23"/>
+      <c r="R3" s="22">
+        <v>43628</v>
+      </c>
+      <c r="S3" s="23">
+        <v>43628</v>
+      </c>
+      <c r="T3" s="22">
+        <v>43629</v>
+      </c>
+      <c r="U3" s="23">
+        <v>43629</v>
+      </c>
       <c r="V3" s="22"/>
       <c r="W3" s="23"/>
       <c r="X3" s="22"/>
@@ -7858,10 +7992,18 @@
       <c r="Q4" s="32">
         <v>1727.14</v>
       </c>
-      <c r="R4" s="31"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="32"/>
+      <c r="R4" s="31">
+        <v>4.01</v>
+      </c>
+      <c r="S4" s="32">
+        <v>1730.12</v>
+      </c>
+      <c r="T4" s="14">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="U4" s="15">
+        <v>1727.83</v>
+      </c>
       <c r="V4" s="31"/>
       <c r="W4" s="32"/>
       <c r="X4" s="31"/>
@@ -8013,10 +8155,18 @@
       <c r="Q5" s="43">
         <v>1759.08</v>
       </c>
-      <c r="R5" s="14"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="15"/>
+      <c r="R5" s="42">
+        <v>3.89</v>
+      </c>
+      <c r="S5" s="43">
+        <v>1762.11</v>
+      </c>
+      <c r="T5" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="U5" s="15">
+        <v>1759.76</v>
+      </c>
       <c r="V5" s="14"/>
       <c r="W5" s="15"/>
       <c r="X5" s="14"/>
@@ -8111,21 +8261,21 @@
         <f t="shared" ref="Q6:Q7" si="9">(((P4/365)*$B$7)/100)+O6</f>
         <v>0.31266104083342539</v>
       </c>
-      <c r="R6" s="46" t="e">
+      <c r="R6" s="46">
         <f t="shared" ref="R6" si="10">$B$6/S4</f>
-        <v>#DIV/0!</v>
+        <v>0.23330109730926896</v>
       </c>
       <c r="S6" s="45">
         <f t="shared" ref="S6:S7" si="11">(((R4/365)*$B$7)/100)+Q6</f>
-        <v>0.31266104083342539</v>
-      </c>
-      <c r="T6" s="46" t="e">
+        <v>0.35691698060547045</v>
+      </c>
+      <c r="T6" s="46">
         <f t="shared" ref="T6" si="12">$B$6/U4</f>
-        <v>#DIV/0!</v>
+        <v>0.23361030568789315</v>
       </c>
       <c r="U6" s="45">
         <f t="shared" ref="U6:U7" si="13">(((T4/365)*$B$7)/100)+S6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="V6" s="46" t="e">
         <f t="shared" ref="V6" si="14">$B$6/W4</f>
@@ -8133,7 +8283,7 @@
       </c>
       <c r="W6" s="45">
         <f t="shared" ref="W6:W7" si="15">(((V4/365)*$B$7)/100)+U6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="X6" s="46" t="e">
         <f t="shared" ref="X6" si="16">$B$6/Y4</f>
@@ -8141,7 +8291,7 @@
       </c>
       <c r="Y6" s="45">
         <f t="shared" ref="Y6:Y7" si="17">(((X4/365)*$B$7)/100)+W6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="Z6" s="46" t="e">
         <f t="shared" ref="Z6" si="18">$B$6/AA4</f>
@@ -8149,7 +8299,7 @@
       </c>
       <c r="AA6" s="45">
         <f t="shared" ref="AA6:AA7" si="19">(((Z4/365)*$B$7)/100)+Y6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="AB6" s="46" t="e">
         <f t="shared" ref="AB6" si="20">$B$6/AC4</f>
@@ -8157,7 +8307,7 @@
       </c>
       <c r="AC6" s="45">
         <f t="shared" ref="AC6:AC7" si="21">(((AB4/365)*$B$7)/100)+AA6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="AD6" s="46" t="e">
         <f t="shared" ref="AD6" si="22">$B$6/AE4</f>
@@ -8165,7 +8315,7 @@
       </c>
       <c r="AE6" s="45">
         <f t="shared" ref="AE6:AE7" si="23">(((AD4/365)*$B$7)/100)+AC6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="AF6" s="46" t="e">
         <f t="shared" ref="AF6" si="24">$B$6/AG4</f>
@@ -8173,7 +8323,7 @@
       </c>
       <c r="AG6" s="45">
         <f t="shared" ref="AG6:AG7" si="25">(((AF4/365)*$B$7)/100)+AE6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="AH6" s="46" t="e">
         <f>$B$6/AI4</f>
@@ -8181,7 +8331,7 @@
       </c>
       <c r="AI6" s="45">
         <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="AJ6" s="46" t="e">
         <f>$B$6/AK4</f>
@@ -8189,7 +8339,7 @@
       </c>
       <c r="AK6" s="45">
         <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="AL6" s="46" t="e">
         <f>$B$6/AM4</f>
@@ -8197,7 +8347,7 @@
       </c>
       <c r="AM6" s="45">
         <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="AN6" s="46" t="e">
         <f>$B$6/AO4</f>
@@ -8205,7 +8355,7 @@
       </c>
       <c r="AO6" s="45">
         <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="AP6" s="46" t="e">
         <f>$B$6/AQ4</f>
@@ -8213,7 +8363,7 @@
       </c>
       <c r="AQ6" s="45">
         <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="AR6" s="46" t="e">
         <f>$B$6/AS4</f>
@@ -8221,7 +8371,7 @@
       </c>
       <c r="AS6" s="45">
         <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="AT6" s="46" t="e">
         <f>$B$6/AU4</f>
@@ -8229,11 +8379,11 @@
       </c>
       <c r="AU6" s="45">
         <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>0.31266104083342539</v>
+        <v>0.40128328431709664</v>
       </c>
       <c r="AV6" s="49">
         <f>AU6-E6</f>
-        <v>0.26752218954473106</v>
+        <v>0.35614443302840232</v>
       </c>
     </row>
     <row r="7" spans="1:119" x14ac:dyDescent="0.25">
@@ -8303,21 +8453,21 @@
         <f t="shared" si="9"/>
         <v>0.30339046990860802</v>
       </c>
-      <c r="R7" s="46" t="e">
+      <c r="R7" s="46">
         <f t="shared" ref="R7" si="38">$B$6/S5</f>
-        <v>#DIV/0!</v>
+        <v>0.22906566245961513</v>
       </c>
       <c r="S7" s="45">
         <f t="shared" si="11"/>
-        <v>0.30339046990860802</v>
-      </c>
-      <c r="T7" s="46" t="e">
+        <v>0.34632204240567915</v>
+      </c>
+      <c r="T7" s="46">
         <f t="shared" ref="T7" si="39">$B$6/U5</f>
-        <v>#DIV/0!</v>
+        <v>0.22937155889252647</v>
       </c>
       <c r="U7" s="45">
         <f t="shared" si="13"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="V7" s="46" t="e">
         <f t="shared" ref="V7" si="40">$B$6/W5</f>
@@ -8325,7 +8475,7 @@
       </c>
       <c r="W7" s="45">
         <f t="shared" si="15"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="X7" s="46" t="e">
         <f t="shared" ref="X7" si="41">$B$6/Y5</f>
@@ -8333,7 +8483,7 @@
       </c>
       <c r="Y7" s="45">
         <f t="shared" si="17"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="Z7" s="46" t="e">
         <f t="shared" ref="Z7" si="42">$B$6/AA5</f>
@@ -8341,7 +8491,7 @@
       </c>
       <c r="AA7" s="45">
         <f t="shared" si="19"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="AB7" s="46" t="e">
         <f t="shared" ref="AB7" si="43">$B$6/AC5</f>
@@ -8349,7 +8499,7 @@
       </c>
       <c r="AC7" s="45">
         <f t="shared" si="21"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="AD7" s="46" t="e">
         <f t="shared" ref="AD7" si="44">$B$6/AE5</f>
@@ -8357,7 +8507,7 @@
       </c>
       <c r="AE7" s="45">
         <f t="shared" si="23"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="AF7" s="46" t="e">
         <f>$B$6/AG5</f>
@@ -8365,7 +8515,7 @@
       </c>
       <c r="AG7" s="45">
         <f t="shared" si="25"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="AH7" s="46" t="e">
         <f>$B$6/AI5</f>
@@ -8373,7 +8523,7 @@
       </c>
       <c r="AI7" s="45">
         <f t="shared" si="26"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="AJ7" s="46" t="e">
         <f>$B$6/AK5</f>
@@ -8381,7 +8531,7 @@
       </c>
       <c r="AK7" s="45">
         <f t="shared" si="27"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="AL7" s="46" t="e">
         <f>$B$6/AM5</f>
@@ -8389,7 +8539,7 @@
       </c>
       <c r="AM7" s="45">
         <f t="shared" si="28"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="AN7" s="46" t="e">
         <f>$B$6/AO5</f>
@@ -8397,7 +8547,7 @@
       </c>
       <c r="AO7" s="45">
         <f t="shared" si="29"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="AP7" s="46" t="e">
         <f>$B$6/AQ5</f>
@@ -8405,7 +8555,7 @@
       </c>
       <c r="AQ7" s="45">
         <f t="shared" si="30"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="AR7" s="46" t="e">
         <f>$B$6/AS5</f>
@@ -8413,7 +8563,7 @@
       </c>
       <c r="AS7" s="45">
         <f t="shared" si="31"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="AT7" s="46" t="e">
         <f>$B$6/AU5</f>
@@ -8421,17 +8571,17 @@
       </c>
       <c r="AU7" s="45">
         <f t="shared" si="32"/>
-        <v>0.30339046990860802</v>
+        <v>0.38936397884233143</v>
       </c>
       <c r="AV7" s="49">
         <f>AU7-E7</f>
-        <v>0.25957598589488762</v>
+        <v>0.34554949482861103</v>
       </c>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.25">
       <c r="AV8" s="49">
         <f>AV6-AV7</f>
-        <v>7.9462036498434419E-3</v>
+        <v>1.0594938199791293E-2</v>
       </c>
     </row>
     <row r="10" spans="1:119" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit atualizacao tesouro 14/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -640,6 +640,9 @@
                   <c:pt idx="8">
                     <c:v>13/jun</c:v>
                   </c:pt>
+                  <c:pt idx="9">
+                    <c:v>14/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -751,6 +754,9 @@
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
                   <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>4.03</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -835,6 +841,9 @@
                   <c:pt idx="8">
                     <c:v>13/jun</c:v>
                   </c:pt>
+                  <c:pt idx="9">
+                    <c:v>14/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -947,6 +956,9 @@
                 <c:pt idx="8" formatCode="General">
                   <c:v>3.9</c:v>
                 </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>3.91</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -962,8 +974,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1276850832"/>
-        <c:axId val="-1276853008"/>
+        <c:axId val="-707901200"/>
+        <c:axId val="-707906640"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1053,6 +1065,9 @@
                         <c:pt idx="8">
                           <c:v>13/jun</c:v>
                         </c:pt>
+                        <c:pt idx="9">
+                          <c:v>14/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1168,7 +1183,7 @@
                         <c:v>0.23361030568789315</c:v>
                       </c:pt>
                       <c:pt idx="9" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23391897915256724</c:v>
                       </c:pt>
                       <c:pt idx="10" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1299,6 +1314,9 @@
                         <c:pt idx="8">
                           <c:v>13/jun</c:v>
                         </c:pt>
+                        <c:pt idx="9">
+                          <c:v>14/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1414,7 +1432,7 @@
                         <c:v>0.22937155889252647</c:v>
                       </c:pt>
                       <c:pt idx="9" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22967696650585082</c:v>
                       </c:pt>
                       <c:pt idx="10" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1462,7 +1480,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1276850832"/>
+        <c:axId val="-707901200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1505,7 +1523,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1276853008"/>
+        <c:crossAx val="-707906640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1513,7 +1531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1276853008"/>
+        <c:axId val="-707906640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1564,7 +1582,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1276850832"/>
+        <c:crossAx val="-707901200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1802,6 +1820,9 @@
                   <c:pt idx="8">
                     <c:v>13/jun</c:v>
                   </c:pt>
+                  <c:pt idx="9">
+                    <c:v>14/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1913,6 +1934,9 @@
                 </c:pt>
                 <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1727.83</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1725.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1997,6 +2021,9 @@
                   <c:pt idx="8">
                     <c:v>13/jun</c:v>
                   </c:pt>
+                  <c:pt idx="9">
+                    <c:v>14/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2109,6 +2136,9 @@
                 <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1759.76</c:v>
                 </c:pt>
+                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1757.42</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2124,11 +2154,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1276838864"/>
-        <c:axId val="-1276848656"/>
+        <c:axId val="-707904464"/>
+        <c:axId val="-707902288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1276838864"/>
+        <c:axId val="-707904464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2171,7 +2201,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1276848656"/>
+        <c:crossAx val="-707902288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2179,7 +2209,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1276848656"/>
+        <c:axId val="-707902288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2230,7 +2260,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1276838864"/>
+        <c:crossAx val="-707904464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2439,6 +2469,9 @@
                   <c:pt idx="8">
                     <c:v>13/jun</c:v>
                   </c:pt>
+                  <c:pt idx="9">
+                    <c:v>14/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2552,7 +2585,7 @@
                   <c:v>0.23361030568789315</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23391897915256724</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2673,6 +2706,9 @@
                   <c:pt idx="8">
                     <c:v>13/jun</c:v>
                   </c:pt>
+                  <c:pt idx="9">
+                    <c:v>14/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2786,7 +2822,7 @@
                   <c:v>0.22937155889252647</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22967696650585082</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2839,8 +2875,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1276847568"/>
-        <c:axId val="-1276841040"/>
+        <c:axId val="-707893040"/>
+        <c:axId val="-707903920"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2930,6 +2966,9 @@
                         <c:pt idx="8">
                           <c:v>13/jun</c:v>
                         </c:pt>
+                        <c:pt idx="9">
+                          <c:v>14/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3043,6 +3082,9 @@
                       </c:pt>
                       <c:pt idx="8" formatCode="General">
                         <c:v>4.0199999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="9" formatCode="General">
+                        <c:v>4.03</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3137,6 +3179,9 @@
                         <c:pt idx="8">
                           <c:v>13/jun</c:v>
                         </c:pt>
+                        <c:pt idx="9">
+                          <c:v>14/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3251,6 +3296,9 @@
                       <c:pt idx="8" formatCode="General">
                         <c:v>3.9</c:v>
                       </c:pt>
+                      <c:pt idx="9" formatCode="General">
+                        <c:v>3.91</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3261,7 +3309,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1276847568"/>
+        <c:axId val="-707893040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3304,7 +3352,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1276841040"/>
+        <c:crossAx val="-707903920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3312,7 +3360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1276841040"/>
+        <c:axId val="-707903920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3363,7 +3411,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1276847568"/>
+        <c:crossAx val="-707893040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3572,6 +3620,9 @@
                   <c:pt idx="8">
                     <c:v>13/jun</c:v>
                   </c:pt>
+                  <c:pt idx="9">
+                    <c:v>14/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3685,43 +3736,43 @@
                   <c:v>0.40128328431709664</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>0.44575995196830398</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>0.44575995196830398</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>0.44575995196830398</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>0.44575995196830398</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>0.44575995196830398</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>0.44575995196830398</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>0.44575995196830398</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>0.44575995196830398</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>0.44575995196830398</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>0.44575995196830398</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>0.44575995196830398</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>0.44575995196830398</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>0.44575995196830398</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3806,6 +3857,9 @@
                   <c:pt idx="8">
                     <c:v>13/jun</c:v>
                   </c:pt>
+                  <c:pt idx="9">
+                    <c:v>14/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3919,43 +3973,43 @@
                   <c:v>0.38936397884233143</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>0.43251627921856484</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>0.43251627921856484</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>0.43251627921856484</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>0.43251627921856484</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>0.43251627921856484</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>0.43251627921856484</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>0.43251627921856484</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>0.43251627921856484</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>0.43251627921856484</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>0.43251627921856484</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>0.43251627921856484</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>0.43251627921856484</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>0.43251627921856484</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3972,8 +4026,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1276853552"/>
-        <c:axId val="-1276850288"/>
+        <c:axId val="-707901744"/>
+        <c:axId val="-707892496"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4063,6 +4117,9 @@
                         <c:pt idx="8">
                           <c:v>13/jun</c:v>
                         </c:pt>
+                        <c:pt idx="9">
+                          <c:v>14/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4176,6 +4233,9 @@
                       </c:pt>
                       <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1727.83</c:v>
+                      </c:pt>
+                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1725.55</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4270,6 +4330,9 @@
                         <c:pt idx="8">
                           <c:v>13/jun</c:v>
                         </c:pt>
+                        <c:pt idx="9">
+                          <c:v>14/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4384,6 +4447,9 @@
                       <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1759.76</c:v>
                       </c:pt>
+                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1757.42</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4394,7 +4460,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1276853552"/>
+        <c:axId val="-707901744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4437,7 +4503,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1276850288"/>
+        <c:crossAx val="-707892496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4445,7 +4511,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1276850288"/>
+        <c:axId val="-707892496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4496,7 +4562,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1276853552"/>
+        <c:crossAx val="-707901744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7514,8 +7580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4:U4"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7841,8 +7907,12 @@
       <c r="U3" s="23">
         <v>43629</v>
       </c>
-      <c r="V3" s="22"/>
-      <c r="W3" s="23"/>
+      <c r="V3" s="22">
+        <v>43630</v>
+      </c>
+      <c r="W3" s="23">
+        <v>43630</v>
+      </c>
       <c r="X3" s="22"/>
       <c r="Y3" s="23"/>
       <c r="Z3" s="22"/>
@@ -7998,14 +8068,18 @@
       <c r="S4" s="32">
         <v>1730.12</v>
       </c>
-      <c r="T4" s="14">
+      <c r="T4" s="31">
         <v>4.0199999999999996</v>
       </c>
-      <c r="U4" s="15">
+      <c r="U4" s="32">
         <v>1727.83</v>
       </c>
-      <c r="V4" s="31"/>
-      <c r="W4" s="32"/>
+      <c r="V4" s="31">
+        <v>4.03</v>
+      </c>
+      <c r="W4" s="32">
+        <v>1725.55</v>
+      </c>
       <c r="X4" s="31"/>
       <c r="Y4" s="32"/>
       <c r="Z4" s="31"/>
@@ -8161,14 +8235,18 @@
       <c r="S5" s="43">
         <v>1762.11</v>
       </c>
-      <c r="T5" s="14">
+      <c r="T5" s="42">
         <v>3.9</v>
       </c>
-      <c r="U5" s="15">
+      <c r="U5" s="43">
         <v>1759.76</v>
       </c>
-      <c r="V5" s="14"/>
-      <c r="W5" s="15"/>
+      <c r="V5" s="42">
+        <v>3.91</v>
+      </c>
+      <c r="W5" s="43">
+        <v>1757.42</v>
+      </c>
       <c r="X5" s="14"/>
       <c r="Y5" s="15"/>
       <c r="Z5" s="14"/>
@@ -8277,13 +8355,13 @@
         <f t="shared" ref="U6:U7" si="13">(((T4/365)*$B$7)/100)+S6</f>
         <v>0.40128328431709664</v>
       </c>
-      <c r="V6" s="46" t="e">
+      <c r="V6" s="46">
         <f t="shared" ref="V6" si="14">$B$6/W4</f>
-        <v>#DIV/0!</v>
+        <v>0.23391897915256724</v>
       </c>
       <c r="W6" s="45">
         <f t="shared" ref="W6:W7" si="15">(((V4/365)*$B$7)/100)+U6</f>
-        <v>0.40128328431709664</v>
+        <v>0.44575995196830398</v>
       </c>
       <c r="X6" s="46" t="e">
         <f t="shared" ref="X6" si="16">$B$6/Y4</f>
@@ -8291,7 +8369,7 @@
       </c>
       <c r="Y6" s="45">
         <f t="shared" ref="Y6:Y7" si="17">(((X4/365)*$B$7)/100)+W6</f>
-        <v>0.40128328431709664</v>
+        <v>0.44575995196830398</v>
       </c>
       <c r="Z6" s="46" t="e">
         <f t="shared" ref="Z6" si="18">$B$6/AA4</f>
@@ -8299,7 +8377,7 @@
       </c>
       <c r="AA6" s="45">
         <f t="shared" ref="AA6:AA7" si="19">(((Z4/365)*$B$7)/100)+Y6</f>
-        <v>0.40128328431709664</v>
+        <v>0.44575995196830398</v>
       </c>
       <c r="AB6" s="46" t="e">
         <f t="shared" ref="AB6" si="20">$B$6/AC4</f>
@@ -8307,7 +8385,7 @@
       </c>
       <c r="AC6" s="45">
         <f t="shared" ref="AC6:AC7" si="21">(((AB4/365)*$B$7)/100)+AA6</f>
-        <v>0.40128328431709664</v>
+        <v>0.44575995196830398</v>
       </c>
       <c r="AD6" s="46" t="e">
         <f t="shared" ref="AD6" si="22">$B$6/AE4</f>
@@ -8315,7 +8393,7 @@
       </c>
       <c r="AE6" s="45">
         <f t="shared" ref="AE6:AE7" si="23">(((AD4/365)*$B$7)/100)+AC6</f>
-        <v>0.40128328431709664</v>
+        <v>0.44575995196830398</v>
       </c>
       <c r="AF6" s="46" t="e">
         <f t="shared" ref="AF6" si="24">$B$6/AG4</f>
@@ -8323,7 +8401,7 @@
       </c>
       <c r="AG6" s="45">
         <f t="shared" ref="AG6:AG7" si="25">(((AF4/365)*$B$7)/100)+AE6</f>
-        <v>0.40128328431709664</v>
+        <v>0.44575995196830398</v>
       </c>
       <c r="AH6" s="46" t="e">
         <f>$B$6/AI4</f>
@@ -8331,7 +8409,7 @@
       </c>
       <c r="AI6" s="45">
         <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
-        <v>0.40128328431709664</v>
+        <v>0.44575995196830398</v>
       </c>
       <c r="AJ6" s="46" t="e">
         <f>$B$6/AK4</f>
@@ -8339,7 +8417,7 @@
       </c>
       <c r="AK6" s="45">
         <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
-        <v>0.40128328431709664</v>
+        <v>0.44575995196830398</v>
       </c>
       <c r="AL6" s="46" t="e">
         <f>$B$6/AM4</f>
@@ -8347,7 +8425,7 @@
       </c>
       <c r="AM6" s="45">
         <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>0.40128328431709664</v>
+        <v>0.44575995196830398</v>
       </c>
       <c r="AN6" s="46" t="e">
         <f>$B$6/AO4</f>
@@ -8355,7 +8433,7 @@
       </c>
       <c r="AO6" s="45">
         <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>0.40128328431709664</v>
+        <v>0.44575995196830398</v>
       </c>
       <c r="AP6" s="46" t="e">
         <f>$B$6/AQ4</f>
@@ -8363,7 +8441,7 @@
       </c>
       <c r="AQ6" s="45">
         <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>0.40128328431709664</v>
+        <v>0.44575995196830398</v>
       </c>
       <c r="AR6" s="46" t="e">
         <f>$B$6/AS4</f>
@@ -8371,7 +8449,7 @@
       </c>
       <c r="AS6" s="45">
         <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>0.40128328431709664</v>
+        <v>0.44575995196830398</v>
       </c>
       <c r="AT6" s="46" t="e">
         <f>$B$6/AU4</f>
@@ -8379,11 +8457,11 @@
       </c>
       <c r="AU6" s="45">
         <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>0.40128328431709664</v>
+        <v>0.44575995196830398</v>
       </c>
       <c r="AV6" s="49">
         <f>AU6-E6</f>
-        <v>0.35614443302840232</v>
+        <v>0.40062110067960965</v>
       </c>
     </row>
     <row r="7" spans="1:119" x14ac:dyDescent="0.25">
@@ -8469,13 +8547,13 @@
         <f t="shared" si="13"/>
         <v>0.38936397884233143</v>
       </c>
-      <c r="V7" s="46" t="e">
+      <c r="V7" s="46">
         <f t="shared" ref="V7" si="40">$B$6/W5</f>
-        <v>#DIV/0!</v>
+        <v>0.22967696650585082</v>
       </c>
       <c r="W7" s="45">
         <f t="shared" si="15"/>
-        <v>0.38936397884233143</v>
+        <v>0.43251627921856484</v>
       </c>
       <c r="X7" s="46" t="e">
         <f t="shared" ref="X7" si="41">$B$6/Y5</f>
@@ -8483,7 +8561,7 @@
       </c>
       <c r="Y7" s="45">
         <f t="shared" si="17"/>
-        <v>0.38936397884233143</v>
+        <v>0.43251627921856484</v>
       </c>
       <c r="Z7" s="46" t="e">
         <f t="shared" ref="Z7" si="42">$B$6/AA5</f>
@@ -8491,7 +8569,7 @@
       </c>
       <c r="AA7" s="45">
         <f t="shared" si="19"/>
-        <v>0.38936397884233143</v>
+        <v>0.43251627921856484</v>
       </c>
       <c r="AB7" s="46" t="e">
         <f t="shared" ref="AB7" si="43">$B$6/AC5</f>
@@ -8499,7 +8577,7 @@
       </c>
       <c r="AC7" s="45">
         <f t="shared" si="21"/>
-        <v>0.38936397884233143</v>
+        <v>0.43251627921856484</v>
       </c>
       <c r="AD7" s="46" t="e">
         <f t="shared" ref="AD7" si="44">$B$6/AE5</f>
@@ -8507,7 +8585,7 @@
       </c>
       <c r="AE7" s="45">
         <f t="shared" si="23"/>
-        <v>0.38936397884233143</v>
+        <v>0.43251627921856484</v>
       </c>
       <c r="AF7" s="46" t="e">
         <f>$B$6/AG5</f>
@@ -8515,7 +8593,7 @@
       </c>
       <c r="AG7" s="45">
         <f t="shared" si="25"/>
-        <v>0.38936397884233143</v>
+        <v>0.43251627921856484</v>
       </c>
       <c r="AH7" s="46" t="e">
         <f>$B$6/AI5</f>
@@ -8523,7 +8601,7 @@
       </c>
       <c r="AI7" s="45">
         <f t="shared" si="26"/>
-        <v>0.38936397884233143</v>
+        <v>0.43251627921856484</v>
       </c>
       <c r="AJ7" s="46" t="e">
         <f>$B$6/AK5</f>
@@ -8531,7 +8609,7 @@
       </c>
       <c r="AK7" s="45">
         <f t="shared" si="27"/>
-        <v>0.38936397884233143</v>
+        <v>0.43251627921856484</v>
       </c>
       <c r="AL7" s="46" t="e">
         <f>$B$6/AM5</f>
@@ -8539,7 +8617,7 @@
       </c>
       <c r="AM7" s="45">
         <f t="shared" si="28"/>
-        <v>0.38936397884233143</v>
+        <v>0.43251627921856484</v>
       </c>
       <c r="AN7" s="46" t="e">
         <f>$B$6/AO5</f>
@@ -8547,7 +8625,7 @@
       </c>
       <c r="AO7" s="45">
         <f t="shared" si="29"/>
-        <v>0.38936397884233143</v>
+        <v>0.43251627921856484</v>
       </c>
       <c r="AP7" s="46" t="e">
         <f>$B$6/AQ5</f>
@@ -8555,7 +8633,7 @@
       </c>
       <c r="AQ7" s="45">
         <f t="shared" si="30"/>
-        <v>0.38936397884233143</v>
+        <v>0.43251627921856484</v>
       </c>
       <c r="AR7" s="46" t="e">
         <f>$B$6/AS5</f>
@@ -8563,7 +8641,7 @@
       </c>
       <c r="AS7" s="45">
         <f t="shared" si="31"/>
-        <v>0.38936397884233143</v>
+        <v>0.43251627921856484</v>
       </c>
       <c r="AT7" s="46" t="e">
         <f>$B$6/AU5</f>
@@ -8571,17 +8649,17 @@
       </c>
       <c r="AU7" s="45">
         <f t="shared" si="32"/>
-        <v>0.38936397884233143</v>
+        <v>0.43251627921856484</v>
       </c>
       <c r="AV7" s="49">
         <f>AU7-E7</f>
-        <v>0.34554949482861103</v>
+        <v>0.38870179520484444</v>
       </c>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.25">
       <c r="AV8" s="49">
         <f>AV6-AV7</f>
-        <v>1.0594938199791293E-2</v>
+        <v>1.1919305474765218E-2</v>
       </c>
     </row>
     <row r="10" spans="1:119" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit atualizacao tesouro dia 17/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -643,6 +643,9 @@
                   <c:pt idx="9">
                     <c:v>14/jun</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>15/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -757,6 +760,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
                   <c:v>4.03</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>4.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -844,6 +850,9 @@
                   <c:pt idx="9">
                     <c:v>14/jun</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>15/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -959,6 +968,9 @@
                 <c:pt idx="9" formatCode="General">
                   <c:v>3.91</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>3.89</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -974,8 +986,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-707901200"/>
-        <c:axId val="-707906640"/>
+        <c:axId val="1610072928"/>
+        <c:axId val="1610066944"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1068,6 +1080,9 @@
                         <c:pt idx="9">
                           <c:v>14/jun</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>15/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1186,7 +1201,7 @@
                         <c:v>0.23391897915256724</c:v>
                       </c:pt>
                       <c:pt idx="10" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23317036923366918</c:v>
                       </c:pt>
                       <c:pt idx="11" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1317,6 +1332,9 @@
                         <c:pt idx="9">
                           <c:v>14/jun</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>15/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1435,7 +1453,7 @@
                         <c:v>0.22967696650585082</c:v>
                       </c:pt>
                       <c:pt idx="10" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22894093511699048</c:v>
                       </c:pt>
                       <c:pt idx="11" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1480,7 +1498,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-707901200"/>
+        <c:axId val="1610072928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1523,7 +1541,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-707906640"/>
+        <c:crossAx val="1610066944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1531,7 +1549,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-707906640"/>
+        <c:axId val="1610066944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1582,7 +1600,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-707901200"/>
+        <c:crossAx val="1610072928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1823,6 +1841,9 @@
                   <c:pt idx="9">
                     <c:v>14/jun</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>15/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1937,6 +1958,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1725.55</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1731.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2024,6 +2048,9 @@
                   <c:pt idx="9">
                     <c:v>14/jun</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>15/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2139,6 +2166,9 @@
                 <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1757.42</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1763.07</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2154,11 +2184,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-707904464"/>
-        <c:axId val="-707902288"/>
+        <c:axId val="1610067488"/>
+        <c:axId val="1610074016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-707904464"/>
+        <c:axId val="1610067488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2201,7 +2231,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-707902288"/>
+        <c:crossAx val="1610074016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2209,7 +2239,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-707902288"/>
+        <c:axId val="1610074016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2260,7 +2290,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-707904464"/>
+        <c:crossAx val="1610067488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2472,6 +2502,9 @@
                   <c:pt idx="9">
                     <c:v>14/jun</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>15/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2588,7 +2621,7 @@
                   <c:v>0.23391897915256724</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23317036923366918</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2709,6 +2742,9 @@
                   <c:pt idx="9">
                     <c:v>14/jun</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>15/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2825,7 +2861,7 @@
                   <c:v>0.22967696650585082</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22894093511699048</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2875,8 +2911,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-707893040"/>
-        <c:axId val="-707903920"/>
+        <c:axId val="1610063136"/>
+        <c:axId val="1610063680"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2969,6 +3005,9 @@
                         <c:pt idx="9">
                           <c:v>14/jun</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>15/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3085,6 +3124,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="General">
                         <c:v>4.03</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>4.01</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3182,6 +3224,9 @@
                         <c:pt idx="9">
                           <c:v>14/jun</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>15/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3299,6 +3344,9 @@
                       <c:pt idx="9" formatCode="General">
                         <c:v>3.91</c:v>
                       </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>3.89</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3309,7 +3357,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-707893040"/>
+        <c:axId val="1610063136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3352,7 +3400,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-707903920"/>
+        <c:crossAx val="1610063680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3360,7 +3408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-707903920"/>
+        <c:axId val="1610063680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3411,7 +3459,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-707893040"/>
+        <c:crossAx val="1610063136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3623,6 +3671,9 @@
                   <c:pt idx="9">
                     <c:v>14/jun</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>15/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3739,40 +3790,40 @@
                   <c:v>0.44575995196830398</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.44575995196830398</c:v>
+                  <c:v>0.49001589174034904</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.44575995196830398</c:v>
+                  <c:v>0.49001589174034904</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.44575995196830398</c:v>
+                  <c:v>0.49001589174034904</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.44575995196830398</c:v>
+                  <c:v>0.49001589174034904</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.44575995196830398</c:v>
+                  <c:v>0.49001589174034904</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.44575995196830398</c:v>
+                  <c:v>0.49001589174034904</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.44575995196830398</c:v>
+                  <c:v>0.49001589174034904</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.44575995196830398</c:v>
+                  <c:v>0.49001589174034904</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.44575995196830398</c:v>
+                  <c:v>0.49001589174034904</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.44575995196830398</c:v>
+                  <c:v>0.49001589174034904</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.44575995196830398</c:v>
+                  <c:v>0.49001589174034904</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.44575995196830398</c:v>
+                  <c:v>0.49001589174034904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3860,6 +3911,9 @@
                   <c:pt idx="9">
                     <c:v>14/jun</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>15/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3976,40 +4030,40 @@
                   <c:v>0.43251627921856484</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43251627921856484</c:v>
+                  <c:v>0.47544785171563597</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43251627921856484</c:v>
+                  <c:v>0.47544785171563597</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43251627921856484</c:v>
+                  <c:v>0.47544785171563597</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43251627921856484</c:v>
+                  <c:v>0.47544785171563597</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43251627921856484</c:v>
+                  <c:v>0.47544785171563597</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43251627921856484</c:v>
+                  <c:v>0.47544785171563597</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43251627921856484</c:v>
+                  <c:v>0.47544785171563597</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43251627921856484</c:v>
+                  <c:v>0.47544785171563597</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43251627921856484</c:v>
+                  <c:v>0.47544785171563597</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43251627921856484</c:v>
+                  <c:v>0.47544785171563597</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43251627921856484</c:v>
+                  <c:v>0.47544785171563597</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43251627921856484</c:v>
+                  <c:v>0.47544785171563597</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4026,8 +4080,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-707901744"/>
-        <c:axId val="-707892496"/>
+        <c:axId val="1610065312"/>
+        <c:axId val="1610065856"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4120,6 +4174,9 @@
                         <c:pt idx="9">
                           <c:v>14/jun</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>15/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4236,6 +4293,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1725.55</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1731.09</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4333,6 +4393,9 @@
                         <c:pt idx="9">
                           <c:v>14/jun</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>15/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4450,6 +4513,9 @@
                       <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1757.42</c:v>
                       </c:pt>
+                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1763.07</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4460,7 +4526,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-707901744"/>
+        <c:axId val="1610065312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4503,7 +4569,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-707892496"/>
+        <c:crossAx val="1610065856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4511,7 +4577,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-707892496"/>
+        <c:axId val="1610065856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4562,7 +4628,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-707901744"/>
+        <c:crossAx val="1610065312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7580,8 +7646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4:Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7913,8 +7979,12 @@
       <c r="W3" s="23">
         <v>43630</v>
       </c>
-      <c r="X3" s="22"/>
-      <c r="Y3" s="23"/>
+      <c r="X3" s="22">
+        <v>43631</v>
+      </c>
+      <c r="Y3" s="23">
+        <v>43631</v>
+      </c>
       <c r="Z3" s="22"/>
       <c r="AA3" s="23"/>
       <c r="AB3" s="22"/>
@@ -8080,8 +8150,12 @@
       <c r="W4" s="32">
         <v>1725.55</v>
       </c>
-      <c r="X4" s="31"/>
-      <c r="Y4" s="32"/>
+      <c r="X4" s="31">
+        <v>4.01</v>
+      </c>
+      <c r="Y4" s="32">
+        <v>1731.09</v>
+      </c>
       <c r="Z4" s="31"/>
       <c r="AA4" s="33"/>
       <c r="AB4" s="31"/>
@@ -8247,8 +8321,12 @@
       <c r="W5" s="43">
         <v>1757.42</v>
       </c>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="15"/>
+      <c r="X5" s="42">
+        <v>3.89</v>
+      </c>
+      <c r="Y5" s="43">
+        <v>1763.07</v>
+      </c>
       <c r="Z5" s="14"/>
       <c r="AA5" s="15"/>
       <c r="AB5" s="14"/>
@@ -8363,13 +8441,13 @@
         <f t="shared" ref="W6:W7" si="15">(((V4/365)*$B$7)/100)+U6</f>
         <v>0.44575995196830398</v>
       </c>
-      <c r="X6" s="46" t="e">
+      <c r="X6" s="46">
         <f t="shared" ref="X6" si="16">$B$6/Y4</f>
-        <v>#DIV/0!</v>
+        <v>0.23317036923366918</v>
       </c>
       <c r="Y6" s="45">
         <f t="shared" ref="Y6:Y7" si="17">(((X4/365)*$B$7)/100)+W6</f>
-        <v>0.44575995196830398</v>
+        <v>0.49001589174034904</v>
       </c>
       <c r="Z6" s="46" t="e">
         <f t="shared" ref="Z6" si="18">$B$6/AA4</f>
@@ -8377,7 +8455,7 @@
       </c>
       <c r="AA6" s="45">
         <f t="shared" ref="AA6:AA7" si="19">(((Z4/365)*$B$7)/100)+Y6</f>
-        <v>0.44575995196830398</v>
+        <v>0.49001589174034904</v>
       </c>
       <c r="AB6" s="46" t="e">
         <f t="shared" ref="AB6" si="20">$B$6/AC4</f>
@@ -8385,7 +8463,7 @@
       </c>
       <c r="AC6" s="45">
         <f t="shared" ref="AC6:AC7" si="21">(((AB4/365)*$B$7)/100)+AA6</f>
-        <v>0.44575995196830398</v>
+        <v>0.49001589174034904</v>
       </c>
       <c r="AD6" s="46" t="e">
         <f t="shared" ref="AD6" si="22">$B$6/AE4</f>
@@ -8393,7 +8471,7 @@
       </c>
       <c r="AE6" s="45">
         <f t="shared" ref="AE6:AE7" si="23">(((AD4/365)*$B$7)/100)+AC6</f>
-        <v>0.44575995196830398</v>
+        <v>0.49001589174034904</v>
       </c>
       <c r="AF6" s="46" t="e">
         <f t="shared" ref="AF6" si="24">$B$6/AG4</f>
@@ -8401,7 +8479,7 @@
       </c>
       <c r="AG6" s="45">
         <f t="shared" ref="AG6:AG7" si="25">(((AF4/365)*$B$7)/100)+AE6</f>
-        <v>0.44575995196830398</v>
+        <v>0.49001589174034904</v>
       </c>
       <c r="AH6" s="46" t="e">
         <f>$B$6/AI4</f>
@@ -8409,7 +8487,7 @@
       </c>
       <c r="AI6" s="45">
         <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
-        <v>0.44575995196830398</v>
+        <v>0.49001589174034904</v>
       </c>
       <c r="AJ6" s="46" t="e">
         <f>$B$6/AK4</f>
@@ -8417,7 +8495,7 @@
       </c>
       <c r="AK6" s="45">
         <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
-        <v>0.44575995196830398</v>
+        <v>0.49001589174034904</v>
       </c>
       <c r="AL6" s="46" t="e">
         <f>$B$6/AM4</f>
@@ -8425,7 +8503,7 @@
       </c>
       <c r="AM6" s="45">
         <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>0.44575995196830398</v>
+        <v>0.49001589174034904</v>
       </c>
       <c r="AN6" s="46" t="e">
         <f>$B$6/AO4</f>
@@ -8433,7 +8511,7 @@
       </c>
       <c r="AO6" s="45">
         <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>0.44575995196830398</v>
+        <v>0.49001589174034904</v>
       </c>
       <c r="AP6" s="46" t="e">
         <f>$B$6/AQ4</f>
@@ -8441,7 +8519,7 @@
       </c>
       <c r="AQ6" s="45">
         <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>0.44575995196830398</v>
+        <v>0.49001589174034904</v>
       </c>
       <c r="AR6" s="46" t="e">
         <f>$B$6/AS4</f>
@@ -8449,7 +8527,7 @@
       </c>
       <c r="AS6" s="45">
         <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>0.44575995196830398</v>
+        <v>0.49001589174034904</v>
       </c>
       <c r="AT6" s="46" t="e">
         <f>$B$6/AU4</f>
@@ -8457,11 +8535,11 @@
       </c>
       <c r="AU6" s="45">
         <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>0.44575995196830398</v>
+        <v>0.49001589174034904</v>
       </c>
       <c r="AV6" s="49">
         <f>AU6-E6</f>
-        <v>0.40062110067960965</v>
+        <v>0.44487704045165472</v>
       </c>
     </row>
     <row r="7" spans="1:119" x14ac:dyDescent="0.25">
@@ -8555,13 +8633,13 @@
         <f t="shared" si="15"/>
         <v>0.43251627921856484</v>
       </c>
-      <c r="X7" s="46" t="e">
+      <c r="X7" s="46">
         <f t="shared" ref="X7" si="41">$B$6/Y5</f>
-        <v>#DIV/0!</v>
+        <v>0.22894093511699048</v>
       </c>
       <c r="Y7" s="45">
         <f t="shared" si="17"/>
-        <v>0.43251627921856484</v>
+        <v>0.47544785171563597</v>
       </c>
       <c r="Z7" s="46" t="e">
         <f t="shared" ref="Z7" si="42">$B$6/AA5</f>
@@ -8569,7 +8647,7 @@
       </c>
       <c r="AA7" s="45">
         <f t="shared" si="19"/>
-        <v>0.43251627921856484</v>
+        <v>0.47544785171563597</v>
       </c>
       <c r="AB7" s="46" t="e">
         <f t="shared" ref="AB7" si="43">$B$6/AC5</f>
@@ -8577,7 +8655,7 @@
       </c>
       <c r="AC7" s="45">
         <f t="shared" si="21"/>
-        <v>0.43251627921856484</v>
+        <v>0.47544785171563597</v>
       </c>
       <c r="AD7" s="46" t="e">
         <f t="shared" ref="AD7" si="44">$B$6/AE5</f>
@@ -8585,7 +8663,7 @@
       </c>
       <c r="AE7" s="45">
         <f t="shared" si="23"/>
-        <v>0.43251627921856484</v>
+        <v>0.47544785171563597</v>
       </c>
       <c r="AF7" s="46" t="e">
         <f>$B$6/AG5</f>
@@ -8593,7 +8671,7 @@
       </c>
       <c r="AG7" s="45">
         <f t="shared" si="25"/>
-        <v>0.43251627921856484</v>
+        <v>0.47544785171563597</v>
       </c>
       <c r="AH7" s="46" t="e">
         <f>$B$6/AI5</f>
@@ -8601,7 +8679,7 @@
       </c>
       <c r="AI7" s="45">
         <f t="shared" si="26"/>
-        <v>0.43251627921856484</v>
+        <v>0.47544785171563597</v>
       </c>
       <c r="AJ7" s="46" t="e">
         <f>$B$6/AK5</f>
@@ -8609,7 +8687,7 @@
       </c>
       <c r="AK7" s="45">
         <f t="shared" si="27"/>
-        <v>0.43251627921856484</v>
+        <v>0.47544785171563597</v>
       </c>
       <c r="AL7" s="46" t="e">
         <f>$B$6/AM5</f>
@@ -8617,7 +8695,7 @@
       </c>
       <c r="AM7" s="45">
         <f t="shared" si="28"/>
-        <v>0.43251627921856484</v>
+        <v>0.47544785171563597</v>
       </c>
       <c r="AN7" s="46" t="e">
         <f>$B$6/AO5</f>
@@ -8625,7 +8703,7 @@
       </c>
       <c r="AO7" s="45">
         <f t="shared" si="29"/>
-        <v>0.43251627921856484</v>
+        <v>0.47544785171563597</v>
       </c>
       <c r="AP7" s="46" t="e">
         <f>$B$6/AQ5</f>
@@ -8633,7 +8711,7 @@
       </c>
       <c r="AQ7" s="45">
         <f t="shared" si="30"/>
-        <v>0.43251627921856484</v>
+        <v>0.47544785171563597</v>
       </c>
       <c r="AR7" s="46" t="e">
         <f>$B$6/AS5</f>
@@ -8641,7 +8719,7 @@
       </c>
       <c r="AS7" s="45">
         <f t="shared" si="31"/>
-        <v>0.43251627921856484</v>
+        <v>0.47544785171563597</v>
       </c>
       <c r="AT7" s="46" t="e">
         <f>$B$6/AU5</f>
@@ -8649,17 +8727,17 @@
       </c>
       <c r="AU7" s="45">
         <f t="shared" si="32"/>
-        <v>0.43251627921856484</v>
+        <v>0.47544785171563597</v>
       </c>
       <c r="AV7" s="49">
         <f>AU7-E7</f>
-        <v>0.38870179520484444</v>
+        <v>0.43163336770191557</v>
       </c>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.25">
       <c r="AV8" s="49">
         <f>AV6-AV7</f>
-        <v>1.1919305474765218E-2</v>
+        <v>1.3243672749739144E-2</v>
       </c>
     </row>
     <row r="10" spans="1:119" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit atualizacao tesouro 19/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -644,7 +644,13 @@
                     <c:v>14/jun</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>15/jun</c:v>
+                    <c:v>17/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>18/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>19/jun</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -762,6 +768,12 @@
                   <c:v>4.03</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
+                  <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
                   <c:v>4.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -851,7 +863,13 @@
                     <c:v>14/jun</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>15/jun</c:v>
+                    <c:v>17/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>18/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>19/jun</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -971,6 +989,12 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>3.89</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>3.88</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>3.89</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -986,8 +1010,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1610072928"/>
-        <c:axId val="1610066944"/>
+        <c:axId val="1758053232"/>
+        <c:axId val="1758045616"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1081,7 +1105,13 @@
                           <c:v>14/jun</c:v>
                         </c:pt>
                         <c:pt idx="10">
-                          <c:v>15/jun</c:v>
+                          <c:v>17/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>18/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>19/jun</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1204,10 +1234,10 @@
                         <c:v>0.23317036923366918</c:v>
                       </c:pt>
                       <c:pt idx="11" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23277772012659234</c:v>
                       </c:pt>
                       <c:pt idx="12" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.23309496403817884</c:v>
                       </c:pt>
                       <c:pt idx="13" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1333,7 +1363,13 @@
                           <c:v>14/jun</c:v>
                         </c:pt>
                         <c:pt idx="10">
-                          <c:v>15/jun</c:v>
+                          <c:v>17/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>18/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>19/jun</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1456,10 +1492,10 @@
                         <c:v>0.22894093511699048</c:v>
                       </c:pt>
                       <c:pt idx="11" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.2285559185956787</c:v>
                       </c:pt>
                       <c:pt idx="12" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22886824020725002</c:v>
                       </c:pt>
                       <c:pt idx="13" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1498,7 +1534,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1610072928"/>
+        <c:axId val="1758053232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1541,7 +1577,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1610066944"/>
+        <c:crossAx val="1758045616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1549,7 +1585,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1610066944"/>
+        <c:axId val="1758045616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1600,7 +1636,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1610072928"/>
+        <c:crossAx val="1758053232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1842,7 +1878,13 @@
                     <c:v>14/jun</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>15/jun</c:v>
+                    <c:v>17/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>18/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>19/jun</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1961,6 +2003,12 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1731.09</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1734.01</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1731.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2049,7 +2097,13 @@
                     <c:v>14/jun</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>15/jun</c:v>
+                    <c:v>17/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>18/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>19/jun</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2169,6 +2223,12 @@
                 <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1763.07</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1766.04</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1763.63</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2184,11 +2244,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1610067488"/>
-        <c:axId val="1610074016"/>
+        <c:axId val="1758048336"/>
+        <c:axId val="1758049968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1610067488"/>
+        <c:axId val="1758048336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2231,7 +2291,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1610074016"/>
+        <c:crossAx val="1758049968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2239,7 +2299,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1610074016"/>
+        <c:axId val="1758049968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2290,7 +2350,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1610067488"/>
+        <c:crossAx val="1758048336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2385,7 +2445,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2503,7 +2562,13 @@
                     <c:v>14/jun</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>15/jun</c:v>
+                    <c:v>17/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>18/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>19/jun</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2624,10 +2689,10 @@
                   <c:v>0.23317036923366918</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23277772012659234</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.23309496403817884</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2743,7 +2808,13 @@
                     <c:v>14/jun</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>15/jun</c:v>
+                    <c:v>17/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>18/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>19/jun</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2864,10 +2935,10 @@
                   <c:v>0.22894093511699048</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.2285559185956787</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22886824020725002</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2911,8 +2982,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1610063136"/>
-        <c:axId val="1610063680"/>
+        <c:axId val="1758047248"/>
+        <c:axId val="1758051600"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3006,7 +3077,13 @@
                           <c:v>14/jun</c:v>
                         </c:pt>
                         <c:pt idx="10">
-                          <c:v>15/jun</c:v>
+                          <c:v>17/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>18/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>19/jun</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -3126,6 +3203,12 @@
                         <c:v>4.03</c:v>
                       </c:pt>
                       <c:pt idx="10" formatCode="General">
+                        <c:v>4.01</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="General">
                         <c:v>4.01</c:v>
                       </c:pt>
                     </c:numCache>
@@ -3225,7 +3308,13 @@
                           <c:v>14/jun</c:v>
                         </c:pt>
                         <c:pt idx="10">
-                          <c:v>15/jun</c:v>
+                          <c:v>17/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>18/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>19/jun</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -3347,6 +3436,12 @@
                       <c:pt idx="10" formatCode="General">
                         <c:v>3.89</c:v>
                       </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>3.88</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="General">
+                        <c:v>3.89</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3357,7 +3452,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1610063136"/>
+        <c:axId val="1758047248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3400,7 +3495,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1610063680"/>
+        <c:crossAx val="1758051600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3408,7 +3503,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1610063680"/>
+        <c:axId val="1758051600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3459,7 +3554,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1610063136"/>
+        <c:crossAx val="1758047248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3473,7 +3568,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3672,7 +3766,13 @@
                     <c:v>14/jun</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>15/jun</c:v>
+                    <c:v>17/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>18/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>19/jun</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3793,37 +3893,37 @@
                   <c:v>0.49001589174034904</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.49001589174034904</c:v>
+                  <c:v>0.53416146757281291</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.49001589174034904</c:v>
+                  <c:v>0.57841740734485791</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.49001589174034904</c:v>
+                  <c:v>0.57841740734485791</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.49001589174034904</c:v>
+                  <c:v>0.57841740734485791</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.49001589174034904</c:v>
+                  <c:v>0.57841740734485791</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.49001589174034904</c:v>
+                  <c:v>0.57841740734485791</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.49001589174034904</c:v>
+                  <c:v>0.57841740734485791</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.49001589174034904</c:v>
+                  <c:v>0.57841740734485791</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.49001589174034904</c:v>
+                  <c:v>0.57841740734485791</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.49001589174034904</c:v>
+                  <c:v>0.57841740734485791</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.49001589174034904</c:v>
+                  <c:v>0.57841740734485791</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3912,7 +4012,13 @@
                     <c:v>14/jun</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>15/jun</c:v>
+                    <c:v>17/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>18/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>19/jun</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -4033,37 +4139,37 @@
                   <c:v>0.47544785171563597</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.47544785171563597</c:v>
+                  <c:v>0.51826906027312591</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.47544785171563597</c:v>
+                  <c:v>0.56120063277019705</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.47544785171563597</c:v>
+                  <c:v>0.56120063277019705</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.47544785171563597</c:v>
+                  <c:v>0.56120063277019705</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.47544785171563597</c:v>
+                  <c:v>0.56120063277019705</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.47544785171563597</c:v>
+                  <c:v>0.56120063277019705</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.47544785171563597</c:v>
+                  <c:v>0.56120063277019705</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.47544785171563597</c:v>
+                  <c:v>0.56120063277019705</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.47544785171563597</c:v>
+                  <c:v>0.56120063277019705</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.47544785171563597</c:v>
+                  <c:v>0.56120063277019705</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.47544785171563597</c:v>
+                  <c:v>0.56120063277019705</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4080,8 +4186,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1610065312"/>
-        <c:axId val="1610065856"/>
+        <c:axId val="1758048880"/>
+        <c:axId val="1758052144"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4175,7 +4281,13 @@
                           <c:v>14/jun</c:v>
                         </c:pt>
                         <c:pt idx="10">
-                          <c:v>15/jun</c:v>
+                          <c:v>17/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>18/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>19/jun</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -4296,6 +4408,12 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1731.09</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1734.01</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1731.65</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4394,7 +4512,13 @@
                           <c:v>14/jun</c:v>
                         </c:pt>
                         <c:pt idx="10">
-                          <c:v>15/jun</c:v>
+                          <c:v>17/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>18/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>19/jun</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -4516,6 +4640,12 @@
                       <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1763.07</c:v>
                       </c:pt>
+                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1766.04</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1763.63</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4526,7 +4656,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1610065312"/>
+        <c:axId val="1758048880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4569,7 +4699,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1610065856"/>
+        <c:crossAx val="1758052144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4577,7 +4707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1610065856"/>
+        <c:axId val="1758052144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4628,7 +4758,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1610065312"/>
+        <c:crossAx val="1758048880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7548,7 +7678,7 @@
       </c>
       <c r="H2" s="6">
         <f>GRAFICO!AC4</f>
-        <v>0</v>
+        <v>1731.65</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -7646,8 +7776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4:Y5"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7980,15 +8110,23 @@
         <v>43630</v>
       </c>
       <c r="X3" s="22">
-        <v>43631</v>
+        <v>43633</v>
       </c>
       <c r="Y3" s="23">
-        <v>43631</v>
-      </c>
-      <c r="Z3" s="22"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="22"/>
-      <c r="AC3" s="24"/>
+        <v>43633</v>
+      </c>
+      <c r="Z3" s="22">
+        <v>43634</v>
+      </c>
+      <c r="AA3" s="23">
+        <v>43634</v>
+      </c>
+      <c r="AB3" s="22">
+        <v>43635</v>
+      </c>
+      <c r="AC3" s="24">
+        <v>43635</v>
+      </c>
       <c r="AD3" s="22"/>
       <c r="AE3" s="23"/>
       <c r="AF3" s="22"/>
@@ -8153,13 +8291,21 @@
       <c r="X4" s="31">
         <v>4.01</v>
       </c>
-      <c r="Y4" s="32">
+      <c r="Y4" s="33">
         <v>1731.09</v>
       </c>
-      <c r="Z4" s="31"/>
-      <c r="AA4" s="33"/>
-      <c r="AB4" s="31"/>
-      <c r="AC4" s="32"/>
+      <c r="Z4" s="31">
+        <v>4</v>
+      </c>
+      <c r="AA4" s="32">
+        <v>1734.01</v>
+      </c>
+      <c r="AB4" s="31">
+        <v>4.01</v>
+      </c>
+      <c r="AC4" s="32">
+        <v>1731.65</v>
+      </c>
       <c r="AD4" s="31"/>
       <c r="AE4" s="32"/>
       <c r="AF4" s="31"/>
@@ -8324,13 +8470,21 @@
       <c r="X5" s="42">
         <v>3.89</v>
       </c>
-      <c r="Y5" s="43">
+      <c r="Y5" s="48">
         <v>1763.07</v>
       </c>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="15"/>
+      <c r="Z5" s="42">
+        <v>3.88</v>
+      </c>
+      <c r="AA5" s="43">
+        <v>1766.04</v>
+      </c>
+      <c r="AB5" s="42">
+        <v>3.89</v>
+      </c>
+      <c r="AC5" s="43">
+        <v>1763.63</v>
+      </c>
       <c r="AD5" s="42"/>
       <c r="AE5" s="43"/>
       <c r="AF5" s="42"/>
@@ -8449,21 +8603,21 @@
         <f t="shared" ref="Y6:Y7" si="17">(((X4/365)*$B$7)/100)+W6</f>
         <v>0.49001589174034904</v>
       </c>
-      <c r="Z6" s="46" t="e">
+      <c r="Z6" s="46">
         <f t="shared" ref="Z6" si="18">$B$6/AA4</f>
-        <v>#DIV/0!</v>
+        <v>0.23277772012659234</v>
       </c>
       <c r="AA6" s="45">
         <f t="shared" ref="AA6:AA7" si="19">(((Z4/365)*$B$7)/100)+Y6</f>
-        <v>0.49001589174034904</v>
-      </c>
-      <c r="AB6" s="46" t="e">
+        <v>0.53416146757281291</v>
+      </c>
+      <c r="AB6" s="46">
         <f t="shared" ref="AB6" si="20">$B$6/AC4</f>
-        <v>#DIV/0!</v>
+        <v>0.23309496403817884</v>
       </c>
       <c r="AC6" s="45">
         <f t="shared" ref="AC6:AC7" si="21">(((AB4/365)*$B$7)/100)+AA6</f>
-        <v>0.49001589174034904</v>
+        <v>0.57841740734485791</v>
       </c>
       <c r="AD6" s="46" t="e">
         <f t="shared" ref="AD6" si="22">$B$6/AE4</f>
@@ -8471,7 +8625,7 @@
       </c>
       <c r="AE6" s="45">
         <f t="shared" ref="AE6:AE7" si="23">(((AD4/365)*$B$7)/100)+AC6</f>
-        <v>0.49001589174034904</v>
+        <v>0.57841740734485791</v>
       </c>
       <c r="AF6" s="46" t="e">
         <f t="shared" ref="AF6" si="24">$B$6/AG4</f>
@@ -8479,7 +8633,7 @@
       </c>
       <c r="AG6" s="45">
         <f t="shared" ref="AG6:AG7" si="25">(((AF4/365)*$B$7)/100)+AE6</f>
-        <v>0.49001589174034904</v>
+        <v>0.57841740734485791</v>
       </c>
       <c r="AH6" s="46" t="e">
         <f>$B$6/AI4</f>
@@ -8487,7 +8641,7 @@
       </c>
       <c r="AI6" s="45">
         <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
-        <v>0.49001589174034904</v>
+        <v>0.57841740734485791</v>
       </c>
       <c r="AJ6" s="46" t="e">
         <f>$B$6/AK4</f>
@@ -8495,7 +8649,7 @@
       </c>
       <c r="AK6" s="45">
         <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
-        <v>0.49001589174034904</v>
+        <v>0.57841740734485791</v>
       </c>
       <c r="AL6" s="46" t="e">
         <f>$B$6/AM4</f>
@@ -8503,7 +8657,7 @@
       </c>
       <c r="AM6" s="45">
         <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>0.49001589174034904</v>
+        <v>0.57841740734485791</v>
       </c>
       <c r="AN6" s="46" t="e">
         <f>$B$6/AO4</f>
@@ -8511,7 +8665,7 @@
       </c>
       <c r="AO6" s="45">
         <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>0.49001589174034904</v>
+        <v>0.57841740734485791</v>
       </c>
       <c r="AP6" s="46" t="e">
         <f>$B$6/AQ4</f>
@@ -8519,7 +8673,7 @@
       </c>
       <c r="AQ6" s="45">
         <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>0.49001589174034904</v>
+        <v>0.57841740734485791</v>
       </c>
       <c r="AR6" s="46" t="e">
         <f>$B$6/AS4</f>
@@ -8527,7 +8681,7 @@
       </c>
       <c r="AS6" s="45">
         <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>0.49001589174034904</v>
+        <v>0.57841740734485791</v>
       </c>
       <c r="AT6" s="46" t="e">
         <f>$B$6/AU4</f>
@@ -8535,11 +8689,11 @@
       </c>
       <c r="AU6" s="45">
         <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>0.49001589174034904</v>
+        <v>0.57841740734485791</v>
       </c>
       <c r="AV6" s="49">
         <f>AU6-E6</f>
-        <v>0.44487704045165472</v>
+        <v>0.53327855605616359</v>
       </c>
     </row>
     <row r="7" spans="1:119" x14ac:dyDescent="0.25">
@@ -8641,21 +8795,21 @@
         <f t="shared" si="17"/>
         <v>0.47544785171563597</v>
       </c>
-      <c r="Z7" s="46" t="e">
+      <c r="Z7" s="46">
         <f t="shared" ref="Z7" si="42">$B$6/AA5</f>
-        <v>#DIV/0!</v>
+        <v>0.2285559185956787</v>
       </c>
       <c r="AA7" s="45">
         <f t="shared" si="19"/>
-        <v>0.47544785171563597</v>
-      </c>
-      <c r="AB7" s="46" t="e">
+        <v>0.51826906027312591</v>
+      </c>
+      <c r="AB7" s="46">
         <f t="shared" ref="AB7" si="43">$B$6/AC5</f>
-        <v>#DIV/0!</v>
+        <v>0.22886824020725002</v>
       </c>
       <c r="AC7" s="45">
         <f t="shared" si="21"/>
-        <v>0.47544785171563597</v>
+        <v>0.56120063277019705</v>
       </c>
       <c r="AD7" s="46" t="e">
         <f t="shared" ref="AD7" si="44">$B$6/AE5</f>
@@ -8663,7 +8817,7 @@
       </c>
       <c r="AE7" s="45">
         <f t="shared" si="23"/>
-        <v>0.47544785171563597</v>
+        <v>0.56120063277019705</v>
       </c>
       <c r="AF7" s="46" t="e">
         <f>$B$6/AG5</f>
@@ -8671,7 +8825,7 @@
       </c>
       <c r="AG7" s="45">
         <f t="shared" si="25"/>
-        <v>0.47544785171563597</v>
+        <v>0.56120063277019705</v>
       </c>
       <c r="AH7" s="46" t="e">
         <f>$B$6/AI5</f>
@@ -8679,7 +8833,7 @@
       </c>
       <c r="AI7" s="45">
         <f t="shared" si="26"/>
-        <v>0.47544785171563597</v>
+        <v>0.56120063277019705</v>
       </c>
       <c r="AJ7" s="46" t="e">
         <f>$B$6/AK5</f>
@@ -8687,7 +8841,7 @@
       </c>
       <c r="AK7" s="45">
         <f t="shared" si="27"/>
-        <v>0.47544785171563597</v>
+        <v>0.56120063277019705</v>
       </c>
       <c r="AL7" s="46" t="e">
         <f>$B$6/AM5</f>
@@ -8695,7 +8849,7 @@
       </c>
       <c r="AM7" s="45">
         <f t="shared" si="28"/>
-        <v>0.47544785171563597</v>
+        <v>0.56120063277019705</v>
       </c>
       <c r="AN7" s="46" t="e">
         <f>$B$6/AO5</f>
@@ -8703,7 +8857,7 @@
       </c>
       <c r="AO7" s="45">
         <f t="shared" si="29"/>
-        <v>0.47544785171563597</v>
+        <v>0.56120063277019705</v>
       </c>
       <c r="AP7" s="46" t="e">
         <f>$B$6/AQ5</f>
@@ -8711,7 +8865,7 @@
       </c>
       <c r="AQ7" s="45">
         <f t="shared" si="30"/>
-        <v>0.47544785171563597</v>
+        <v>0.56120063277019705</v>
       </c>
       <c r="AR7" s="46" t="e">
         <f>$B$6/AS5</f>
@@ -8719,7 +8873,7 @@
       </c>
       <c r="AS7" s="45">
         <f t="shared" si="31"/>
-        <v>0.47544785171563597</v>
+        <v>0.56120063277019705</v>
       </c>
       <c r="AT7" s="46" t="e">
         <f>$B$6/AU5</f>
@@ -8727,17 +8881,17 @@
       </c>
       <c r="AU7" s="45">
         <f t="shared" si="32"/>
-        <v>0.47544785171563597</v>
+        <v>0.56120063277019705</v>
       </c>
       <c r="AV7" s="49">
         <f>AU7-E7</f>
-        <v>0.43163336770191557</v>
+        <v>0.51738614875647659</v>
       </c>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.25">
       <c r="AV8" s="49">
         <f>AV6-AV7</f>
-        <v>1.3243672749739144E-2</v>
+        <v>1.5892407299686995E-2</v>
       </c>
     </row>
     <row r="10" spans="1:119" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit atualizacao tesouro 21/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -652,6 +652,9 @@
                   <c:pt idx="12">
                     <c:v>19/jun</c:v>
                   </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -775,6 +778,9 @@
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
                   <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>3.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -871,6 +877,9 @@
                   <c:pt idx="12">
                     <c:v>19/jun</c:v>
                   </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -995,6 +1004,9 @@
                 <c:pt idx="12" formatCode="General">
                   <c:v>3.89</c:v>
                 </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>3.77</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1010,8 +1022,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1758053232"/>
-        <c:axId val="1758045616"/>
+        <c:axId val="143739840"/>
+        <c:axId val="2032116624"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1113,6 +1125,9 @@
                         <c:pt idx="12">
                           <c:v>19/jun</c:v>
                         </c:pt>
+                        <c:pt idx="13">
+                          <c:v>21/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1240,7 +1255,7 @@
                         <c:v>0.23309496403817884</c:v>
                       </c:pt>
                       <c:pt idx="13" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22883191006157477</c:v>
                       </c:pt>
                       <c:pt idx="14" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1371,6 +1386,9 @@
                         <c:pt idx="12">
                           <c:v>19/jun</c:v>
                         </c:pt>
+                        <c:pt idx="13">
+                          <c:v>21/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1498,7 +1516,7 @@
                         <c:v>0.22886824020725002</c:v>
                       </c:pt>
                       <c:pt idx="13" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22467945877101289</c:v>
                       </c:pt>
                       <c:pt idx="14" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1534,7 +1552,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1758053232"/>
+        <c:axId val="143739840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1577,7 +1595,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1758045616"/>
+        <c:crossAx val="2032116624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1585,7 +1603,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1758045616"/>
+        <c:axId val="2032116624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,7 +1654,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1758053232"/>
+        <c:crossAx val="143739840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1886,6 +1904,9 @@
                   <c:pt idx="12">
                     <c:v>19/jun</c:v>
                   </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2009,6 +2030,9 @@
                 </c:pt>
                 <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1731.65</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1763.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2105,6 +2129,9 @@
                   <c:pt idx="12">
                     <c:v>19/jun</c:v>
                   </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2229,6 +2256,9 @@
                 <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1763.63</c:v>
                 </c:pt>
+                <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1796.51</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2244,11 +2274,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1758048336"/>
-        <c:axId val="1758049968"/>
+        <c:axId val="143752352"/>
+        <c:axId val="143737120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1758048336"/>
+        <c:axId val="143752352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2291,7 +2321,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1758049968"/>
+        <c:crossAx val="143737120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2299,7 +2329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1758049968"/>
+        <c:axId val="143737120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2350,7 +2380,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1758048336"/>
+        <c:crossAx val="143752352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2570,6 +2600,9 @@
                   <c:pt idx="12">
                     <c:v>19/jun</c:v>
                   </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2695,7 +2728,7 @@
                   <c:v>0.23309496403817884</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22883191006157477</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2816,6 +2849,9 @@
                   <c:pt idx="12">
                     <c:v>19/jun</c:v>
                   </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2941,7 +2977,7 @@
                   <c:v>0.22886824020725002</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22467945877101289</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2982,8 +3018,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1758047248"/>
-        <c:axId val="1758051600"/>
+        <c:axId val="147631120"/>
+        <c:axId val="147627312"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3085,6 +3121,9 @@
                         <c:pt idx="12">
                           <c:v>19/jun</c:v>
                         </c:pt>
+                        <c:pt idx="13">
+                          <c:v>21/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3210,6 +3249,9 @@
                       </c:pt>
                       <c:pt idx="12" formatCode="General">
                         <c:v>4.01</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="General">
+                        <c:v>3.89</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3316,6 +3358,9 @@
                         <c:pt idx="12">
                           <c:v>19/jun</c:v>
                         </c:pt>
+                        <c:pt idx="13">
+                          <c:v>21/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3442,6 +3487,9 @@
                       <c:pt idx="12" formatCode="General">
                         <c:v>3.89</c:v>
                       </c:pt>
+                      <c:pt idx="13" formatCode="General">
+                        <c:v>3.77</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3452,7 +3500,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1758047248"/>
+        <c:axId val="147631120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3495,7 +3543,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1758051600"/>
+        <c:crossAx val="147627312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3503,7 +3551,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1758051600"/>
+        <c:axId val="147627312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3554,7 +3602,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1758047248"/>
+        <c:crossAx val="147631120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3774,6 +3822,9 @@
                   <c:pt idx="12">
                     <c:v>19/jun</c:v>
                   </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3899,31 +3950,31 @@
                   <c:v>0.57841740734485791</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.57841740734485791</c:v>
+                  <c:v>0.62134897984192905</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.57841740734485791</c:v>
+                  <c:v>0.62134897984192905</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.57841740734485791</c:v>
+                  <c:v>0.62134897984192905</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.57841740734485791</c:v>
+                  <c:v>0.62134897984192905</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.57841740734485791</c:v>
+                  <c:v>0.62134897984192905</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.57841740734485791</c:v>
+                  <c:v>0.62134897984192905</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.57841740734485791</c:v>
+                  <c:v>0.62134897984192905</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.57841740734485791</c:v>
+                  <c:v>0.62134897984192905</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.57841740734485791</c:v>
+                  <c:v>0.62134897984192905</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4020,6 +4071,9 @@
                   <c:pt idx="12">
                     <c:v>19/jun</c:v>
                   </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -4145,31 +4199,31 @@
                   <c:v>0.56120063277019705</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.56120063277019705</c:v>
+                  <c:v>0.6028078379922942</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.56120063277019705</c:v>
+                  <c:v>0.6028078379922942</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.56120063277019705</c:v>
+                  <c:v>0.6028078379922942</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.56120063277019705</c:v>
+                  <c:v>0.6028078379922942</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.56120063277019705</c:v>
+                  <c:v>0.6028078379922942</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.56120063277019705</c:v>
+                  <c:v>0.6028078379922942</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.56120063277019705</c:v>
+                  <c:v>0.6028078379922942</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.56120063277019705</c:v>
+                  <c:v>0.6028078379922942</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.56120063277019705</c:v>
+                  <c:v>0.6028078379922942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4186,8 +4240,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1758048880"/>
-        <c:axId val="1758052144"/>
+        <c:axId val="147632208"/>
+        <c:axId val="147628400"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4289,6 +4343,9 @@
                         <c:pt idx="12">
                           <c:v>19/jun</c:v>
                         </c:pt>
+                        <c:pt idx="13">
+                          <c:v>21/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4414,6 +4471,9 @@
                       </c:pt>
                       <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1731.65</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1763.91</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4520,6 +4580,9 @@
                         <c:pt idx="12">
                           <c:v>19/jun</c:v>
                         </c:pt>
+                        <c:pt idx="13">
+                          <c:v>21/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4646,6 +4709,9 @@
                       <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1763.63</c:v>
                       </c:pt>
+                      <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1796.51</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4656,7 +4722,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1758048880"/>
+        <c:axId val="147632208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4699,7 +4765,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1758052144"/>
+        <c:crossAx val="147628400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4707,7 +4773,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1758052144"/>
+        <c:axId val="147628400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4758,7 +4824,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1758048880"/>
+        <c:crossAx val="147632208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7777,7 +7843,7 @@
   <dimension ref="A2:DO11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AD5" sqref="AD5"/>
+      <selection activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8127,8 +8193,12 @@
       <c r="AC3" s="24">
         <v>43635</v>
       </c>
-      <c r="AD3" s="22"/>
-      <c r="AE3" s="23"/>
+      <c r="AD3" s="22">
+        <v>43637</v>
+      </c>
+      <c r="AE3" s="23">
+        <v>43637</v>
+      </c>
       <c r="AF3" s="22"/>
       <c r="AG3" s="23"/>
       <c r="AH3" s="22"/>
@@ -8306,8 +8376,12 @@
       <c r="AC4" s="32">
         <v>1731.65</v>
       </c>
-      <c r="AD4" s="31"/>
-      <c r="AE4" s="32"/>
+      <c r="AD4" s="31">
+        <v>3.89</v>
+      </c>
+      <c r="AE4" s="32">
+        <v>1763.91</v>
+      </c>
       <c r="AF4" s="31"/>
       <c r="AG4" s="32"/>
       <c r="AH4" s="31"/>
@@ -8485,8 +8559,12 @@
       <c r="AC5" s="43">
         <v>1763.63</v>
       </c>
-      <c r="AD5" s="42"/>
-      <c r="AE5" s="43"/>
+      <c r="AD5" s="42">
+        <v>3.77</v>
+      </c>
+      <c r="AE5" s="43">
+        <v>1796.51</v>
+      </c>
       <c r="AF5" s="42"/>
       <c r="AG5" s="43"/>
       <c r="AH5" s="42"/>
@@ -8619,13 +8697,13 @@
         <f t="shared" ref="AC6:AC7" si="21">(((AB4/365)*$B$7)/100)+AA6</f>
         <v>0.57841740734485791</v>
       </c>
-      <c r="AD6" s="46" t="e">
+      <c r="AD6" s="46">
         <f t="shared" ref="AD6" si="22">$B$6/AE4</f>
-        <v>#DIV/0!</v>
+        <v>0.22883191006157477</v>
       </c>
       <c r="AE6" s="45">
         <f t="shared" ref="AE6:AE7" si="23">(((AD4/365)*$B$7)/100)+AC6</f>
-        <v>0.57841740734485791</v>
+        <v>0.62134897984192905</v>
       </c>
       <c r="AF6" s="46" t="e">
         <f t="shared" ref="AF6" si="24">$B$6/AG4</f>
@@ -8633,7 +8711,7 @@
       </c>
       <c r="AG6" s="45">
         <f t="shared" ref="AG6:AG7" si="25">(((AF4/365)*$B$7)/100)+AE6</f>
-        <v>0.57841740734485791</v>
+        <v>0.62134897984192905</v>
       </c>
       <c r="AH6" s="46" t="e">
         <f>$B$6/AI4</f>
@@ -8641,7 +8719,7 @@
       </c>
       <c r="AI6" s="45">
         <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
-        <v>0.57841740734485791</v>
+        <v>0.62134897984192905</v>
       </c>
       <c r="AJ6" s="46" t="e">
         <f>$B$6/AK4</f>
@@ -8649,7 +8727,7 @@
       </c>
       <c r="AK6" s="45">
         <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
-        <v>0.57841740734485791</v>
+        <v>0.62134897984192905</v>
       </c>
       <c r="AL6" s="46" t="e">
         <f>$B$6/AM4</f>
@@ -8657,7 +8735,7 @@
       </c>
       <c r="AM6" s="45">
         <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>0.57841740734485791</v>
+        <v>0.62134897984192905</v>
       </c>
       <c r="AN6" s="46" t="e">
         <f>$B$6/AO4</f>
@@ -8665,7 +8743,7 @@
       </c>
       <c r="AO6" s="45">
         <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>0.57841740734485791</v>
+        <v>0.62134897984192905</v>
       </c>
       <c r="AP6" s="46" t="e">
         <f>$B$6/AQ4</f>
@@ -8673,7 +8751,7 @@
       </c>
       <c r="AQ6" s="45">
         <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>0.57841740734485791</v>
+        <v>0.62134897984192905</v>
       </c>
       <c r="AR6" s="46" t="e">
         <f>$B$6/AS4</f>
@@ -8681,7 +8759,7 @@
       </c>
       <c r="AS6" s="45">
         <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>0.57841740734485791</v>
+        <v>0.62134897984192905</v>
       </c>
       <c r="AT6" s="46" t="e">
         <f>$B$6/AU4</f>
@@ -8689,11 +8767,11 @@
       </c>
       <c r="AU6" s="45">
         <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>0.57841740734485791</v>
+        <v>0.62134897984192905</v>
       </c>
       <c r="AV6" s="49">
         <f>AU6-E6</f>
-        <v>0.53327855605616359</v>
+        <v>0.57621012855323472</v>
       </c>
     </row>
     <row r="7" spans="1:119" x14ac:dyDescent="0.25">
@@ -8811,13 +8889,13 @@
         <f t="shared" si="21"/>
         <v>0.56120063277019705</v>
       </c>
-      <c r="AD7" s="46" t="e">
+      <c r="AD7" s="46">
         <f t="shared" ref="AD7" si="44">$B$6/AE5</f>
-        <v>#DIV/0!</v>
+        <v>0.22467945877101289</v>
       </c>
       <c r="AE7" s="45">
         <f t="shared" si="23"/>
-        <v>0.56120063277019705</v>
+        <v>0.6028078379922942</v>
       </c>
       <c r="AF7" s="46" t="e">
         <f>$B$6/AG5</f>
@@ -8825,7 +8903,7 @@
       </c>
       <c r="AG7" s="45">
         <f t="shared" si="25"/>
-        <v>0.56120063277019705</v>
+        <v>0.6028078379922942</v>
       </c>
       <c r="AH7" s="46" t="e">
         <f>$B$6/AI5</f>
@@ -8833,7 +8911,7 @@
       </c>
       <c r="AI7" s="45">
         <f t="shared" si="26"/>
-        <v>0.56120063277019705</v>
+        <v>0.6028078379922942</v>
       </c>
       <c r="AJ7" s="46" t="e">
         <f>$B$6/AK5</f>
@@ -8841,7 +8919,7 @@
       </c>
       <c r="AK7" s="45">
         <f t="shared" si="27"/>
-        <v>0.56120063277019705</v>
+        <v>0.6028078379922942</v>
       </c>
       <c r="AL7" s="46" t="e">
         <f>$B$6/AM5</f>
@@ -8849,7 +8927,7 @@
       </c>
       <c r="AM7" s="45">
         <f t="shared" si="28"/>
-        <v>0.56120063277019705</v>
+        <v>0.6028078379922942</v>
       </c>
       <c r="AN7" s="46" t="e">
         <f>$B$6/AO5</f>
@@ -8857,7 +8935,7 @@
       </c>
       <c r="AO7" s="45">
         <f t="shared" si="29"/>
-        <v>0.56120063277019705</v>
+        <v>0.6028078379922942</v>
       </c>
       <c r="AP7" s="46" t="e">
         <f>$B$6/AQ5</f>
@@ -8865,7 +8943,7 @@
       </c>
       <c r="AQ7" s="45">
         <f t="shared" si="30"/>
-        <v>0.56120063277019705</v>
+        <v>0.6028078379922942</v>
       </c>
       <c r="AR7" s="46" t="e">
         <f>$B$6/AS5</f>
@@ -8873,7 +8951,7 @@
       </c>
       <c r="AS7" s="45">
         <f t="shared" si="31"/>
-        <v>0.56120063277019705</v>
+        <v>0.6028078379922942</v>
       </c>
       <c r="AT7" s="46" t="e">
         <f>$B$6/AU5</f>
@@ -8881,17 +8959,17 @@
       </c>
       <c r="AU7" s="45">
         <f t="shared" si="32"/>
-        <v>0.56120063277019705</v>
+        <v>0.6028078379922942</v>
       </c>
       <c r="AV7" s="49">
         <f>AU7-E7</f>
-        <v>0.51738614875647659</v>
+        <v>0.55899335397857386</v>
       </c>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.25">
       <c r="AV8" s="49">
         <f>AV6-AV7</f>
-        <v>1.5892407299686995E-2</v>
+        <v>1.7216774574660865E-2</v>
       </c>
     </row>
     <row r="10" spans="1:119" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit atualizacao tesouro 24/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -655,6 +655,9 @@
                   <c:pt idx="13">
                     <c:v>21/jun</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>24/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -780,6 +783,9 @@
                   <c:v>4.01</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
+                  <c:v>3.89</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
                   <c:v>3.89</c:v>
                 </c:pt>
               </c:numCache>
@@ -880,6 +886,9 @@
                   <c:pt idx="13">
                     <c:v>21/jun</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>24/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1007,6 +1016,9 @@
                 <c:pt idx="13" formatCode="General">
                   <c:v>3.77</c:v>
                 </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>3.77</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1022,8 +1034,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143739840"/>
-        <c:axId val="2032116624"/>
+        <c:axId val="1931528528"/>
+        <c:axId val="1931529072"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1128,6 +1140,9 @@
                         <c:pt idx="13">
                           <c:v>21/jun</c:v>
                         </c:pt>
+                        <c:pt idx="14">
+                          <c:v>24/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1258,7 +1273,7 @@
                         <c:v>0.22883191006157477</c:v>
                       </c:pt>
                       <c:pt idx="14" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22879688834286319</c:v>
                       </c:pt>
                       <c:pt idx="15" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1389,6 +1404,9 @@
                         <c:pt idx="13">
                           <c:v>21/jun</c:v>
                         </c:pt>
+                        <c:pt idx="14">
+                          <c:v>24/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1519,7 +1537,7 @@
                         <c:v>0.22467945877101289</c:v>
                       </c:pt>
                       <c:pt idx="14" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22464569645516558</c:v>
                       </c:pt>
                       <c:pt idx="15" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1552,7 +1570,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143739840"/>
+        <c:axId val="1931528528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1595,7 +1613,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2032116624"/>
+        <c:crossAx val="1931529072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1603,7 +1621,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2032116624"/>
+        <c:axId val="1931529072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1654,7 +1672,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143739840"/>
+        <c:crossAx val="1931528528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1907,6 +1925,9 @@
                   <c:pt idx="13">
                     <c:v>21/jun</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>24/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2033,6 +2054,9 @@
                 </c:pt>
                 <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1763.91</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1764.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2132,6 +2156,9 @@
                   <c:pt idx="13">
                     <c:v>21/jun</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>24/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2259,6 +2286,9 @@
                 <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1796.51</c:v>
                 </c:pt>
+                <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1796.78</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2274,11 +2304,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143752352"/>
-        <c:axId val="143737120"/>
+        <c:axId val="1931530160"/>
+        <c:axId val="1931530704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143752352"/>
+        <c:axId val="1931530160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2321,7 +2351,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143737120"/>
+        <c:crossAx val="1931530704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2329,7 +2359,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143737120"/>
+        <c:axId val="1931530704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2380,7 +2410,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143752352"/>
+        <c:crossAx val="1931530160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2603,6 +2633,9 @@
                   <c:pt idx="13">
                     <c:v>21/jun</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>24/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2731,7 +2764,7 @@
                   <c:v>0.22883191006157477</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22879688834286319</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2852,6 +2885,9 @@
                   <c:pt idx="13">
                     <c:v>21/jun</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>24/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2980,7 +3016,7 @@
                   <c:v>0.22467945877101289</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22464569645516558</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00">
                   <c:v>0</c:v>
@@ -3018,8 +3054,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147631120"/>
-        <c:axId val="147627312"/>
+        <c:axId val="1931536144"/>
+        <c:axId val="1931532880"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3124,6 +3160,9 @@
                         <c:pt idx="13">
                           <c:v>21/jun</c:v>
                         </c:pt>
+                        <c:pt idx="14">
+                          <c:v>24/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3251,6 +3290,9 @@
                         <c:v>4.01</c:v>
                       </c:pt>
                       <c:pt idx="13" formatCode="General">
+                        <c:v>3.89</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="General">
                         <c:v>3.89</c:v>
                       </c:pt>
                     </c:numCache>
@@ -3361,6 +3403,9 @@
                         <c:pt idx="13">
                           <c:v>21/jun</c:v>
                         </c:pt>
+                        <c:pt idx="14">
+                          <c:v>24/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3490,6 +3535,9 @@
                       <c:pt idx="13" formatCode="General">
                         <c:v>3.77</c:v>
                       </c:pt>
+                      <c:pt idx="14" formatCode="General">
+                        <c:v>3.77</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3500,7 +3548,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="147631120"/>
+        <c:axId val="1931536144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3543,7 +3591,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147627312"/>
+        <c:crossAx val="1931532880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3551,7 +3599,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147627312"/>
+        <c:axId val="1931532880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3602,7 +3650,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147631120"/>
+        <c:crossAx val="1931536144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3825,6 +3873,9 @@
                   <c:pt idx="13">
                     <c:v>21/jun</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>24/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3953,28 +4004,28 @@
                   <c:v>0.62134897984192905</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.62134897984192905</c:v>
+                  <c:v>0.66428055233900019</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.62134897984192905</c:v>
+                  <c:v>0.66428055233900019</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.62134897984192905</c:v>
+                  <c:v>0.66428055233900019</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.62134897984192905</c:v>
+                  <c:v>0.66428055233900019</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.62134897984192905</c:v>
+                  <c:v>0.66428055233900019</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.62134897984192905</c:v>
+                  <c:v>0.66428055233900019</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.62134897984192905</c:v>
+                  <c:v>0.66428055233900019</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.62134897984192905</c:v>
+                  <c:v>0.66428055233900019</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4074,6 +4125,9 @@
                   <c:pt idx="13">
                     <c:v>21/jun</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>24/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -4202,28 +4256,28 @@
                   <c:v>0.6028078379922942</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.6028078379922942</c:v>
+                  <c:v>0.64441504321439136</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.6028078379922942</c:v>
+                  <c:v>0.64441504321439136</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.6028078379922942</c:v>
+                  <c:v>0.64441504321439136</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.6028078379922942</c:v>
+                  <c:v>0.64441504321439136</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.6028078379922942</c:v>
+                  <c:v>0.64441504321439136</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.6028078379922942</c:v>
+                  <c:v>0.64441504321439136</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.6028078379922942</c:v>
+                  <c:v>0.64441504321439136</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.6028078379922942</c:v>
+                  <c:v>0.64441504321439136</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4240,8 +4294,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147632208"/>
-        <c:axId val="147628400"/>
+        <c:axId val="1931532336"/>
+        <c:axId val="1931539952"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4346,6 +4400,9 @@
                         <c:pt idx="13">
                           <c:v>21/jun</c:v>
                         </c:pt>
+                        <c:pt idx="14">
+                          <c:v>24/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4474,6 +4531,9 @@
                       </c:pt>
                       <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1763.91</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1764.18</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4583,6 +4643,9 @@
                         <c:pt idx="13">
                           <c:v>21/jun</c:v>
                         </c:pt>
+                        <c:pt idx="14">
+                          <c:v>24/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4712,6 +4775,9 @@
                       <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1796.51</c:v>
                       </c:pt>
+                      <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1796.78</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4722,7 +4788,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="147632208"/>
+        <c:axId val="1931532336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4765,7 +4831,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147628400"/>
+        <c:crossAx val="1931539952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4773,7 +4839,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147628400"/>
+        <c:axId val="1931539952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4824,7 +4890,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147632208"/>
+        <c:crossAx val="1931532336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7842,8 +7908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AE4" sqref="AE4"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AG4" sqref="AG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8199,8 +8265,12 @@
       <c r="AE3" s="23">
         <v>43637</v>
       </c>
-      <c r="AF3" s="22"/>
-      <c r="AG3" s="23"/>
+      <c r="AF3" s="22">
+        <v>43640</v>
+      </c>
+      <c r="AG3" s="23">
+        <v>43640</v>
+      </c>
       <c r="AH3" s="22"/>
       <c r="AI3" s="23"/>
       <c r="AJ3" s="22"/>
@@ -8382,8 +8452,12 @@
       <c r="AE4" s="32">
         <v>1763.91</v>
       </c>
-      <c r="AF4" s="31"/>
-      <c r="AG4" s="32"/>
+      <c r="AF4" s="31">
+        <v>3.89</v>
+      </c>
+      <c r="AG4" s="32">
+        <v>1764.18</v>
+      </c>
       <c r="AH4" s="31"/>
       <c r="AI4" s="32"/>
       <c r="AJ4" s="31"/>
@@ -8565,8 +8639,12 @@
       <c r="AE5" s="43">
         <v>1796.51</v>
       </c>
-      <c r="AF5" s="42"/>
-      <c r="AG5" s="43"/>
+      <c r="AF5" s="42">
+        <v>3.77</v>
+      </c>
+      <c r="AG5" s="43">
+        <v>1796.78</v>
+      </c>
       <c r="AH5" s="42"/>
       <c r="AI5" s="15"/>
       <c r="AJ5" s="42"/>
@@ -8705,13 +8783,13 @@
         <f t="shared" ref="AE6:AE7" si="23">(((AD4/365)*$B$7)/100)+AC6</f>
         <v>0.62134897984192905</v>
       </c>
-      <c r="AF6" s="46" t="e">
+      <c r="AF6" s="46">
         <f t="shared" ref="AF6" si="24">$B$6/AG4</f>
-        <v>#DIV/0!</v>
+        <v>0.22879688834286319</v>
       </c>
       <c r="AG6" s="45">
         <f t="shared" ref="AG6:AG7" si="25">(((AF4/365)*$B$7)/100)+AE6</f>
-        <v>0.62134897984192905</v>
+        <v>0.66428055233900019</v>
       </c>
       <c r="AH6" s="46" t="e">
         <f>$B$6/AI4</f>
@@ -8719,7 +8797,7 @@
       </c>
       <c r="AI6" s="45">
         <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
-        <v>0.62134897984192905</v>
+        <v>0.66428055233900019</v>
       </c>
       <c r="AJ6" s="46" t="e">
         <f>$B$6/AK4</f>
@@ -8727,7 +8805,7 @@
       </c>
       <c r="AK6" s="45">
         <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
-        <v>0.62134897984192905</v>
+        <v>0.66428055233900019</v>
       </c>
       <c r="AL6" s="46" t="e">
         <f>$B$6/AM4</f>
@@ -8735,7 +8813,7 @@
       </c>
       <c r="AM6" s="45">
         <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>0.62134897984192905</v>
+        <v>0.66428055233900019</v>
       </c>
       <c r="AN6" s="46" t="e">
         <f>$B$6/AO4</f>
@@ -8743,7 +8821,7 @@
       </c>
       <c r="AO6" s="45">
         <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>0.62134897984192905</v>
+        <v>0.66428055233900019</v>
       </c>
       <c r="AP6" s="46" t="e">
         <f>$B$6/AQ4</f>
@@ -8751,7 +8829,7 @@
       </c>
       <c r="AQ6" s="45">
         <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>0.62134897984192905</v>
+        <v>0.66428055233900019</v>
       </c>
       <c r="AR6" s="46" t="e">
         <f>$B$6/AS4</f>
@@ -8759,7 +8837,7 @@
       </c>
       <c r="AS6" s="45">
         <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>0.62134897984192905</v>
+        <v>0.66428055233900019</v>
       </c>
       <c r="AT6" s="46" t="e">
         <f>$B$6/AU4</f>
@@ -8767,11 +8845,11 @@
       </c>
       <c r="AU6" s="45">
         <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>0.62134897984192905</v>
+        <v>0.66428055233900019</v>
       </c>
       <c r="AV6" s="49">
         <f>AU6-E6</f>
-        <v>0.57621012855323472</v>
+        <v>0.61914170105030586</v>
       </c>
     </row>
     <row r="7" spans="1:119" x14ac:dyDescent="0.25">
@@ -8897,13 +8975,13 @@
         <f t="shared" si="23"/>
         <v>0.6028078379922942</v>
       </c>
-      <c r="AF7" s="46" t="e">
+      <c r="AF7" s="46">
         <f>$B$6/AG5</f>
-        <v>#DIV/0!</v>
+        <v>0.22464569645516558</v>
       </c>
       <c r="AG7" s="45">
         <f t="shared" si="25"/>
-        <v>0.6028078379922942</v>
+        <v>0.64441504321439136</v>
       </c>
       <c r="AH7" s="46" t="e">
         <f>$B$6/AI5</f>
@@ -8911,7 +8989,7 @@
       </c>
       <c r="AI7" s="45">
         <f t="shared" si="26"/>
-        <v>0.6028078379922942</v>
+        <v>0.64441504321439136</v>
       </c>
       <c r="AJ7" s="46" t="e">
         <f>$B$6/AK5</f>
@@ -8919,7 +8997,7 @@
       </c>
       <c r="AK7" s="45">
         <f t="shared" si="27"/>
-        <v>0.6028078379922942</v>
+        <v>0.64441504321439136</v>
       </c>
       <c r="AL7" s="46" t="e">
         <f>$B$6/AM5</f>
@@ -8927,7 +9005,7 @@
       </c>
       <c r="AM7" s="45">
         <f t="shared" si="28"/>
-        <v>0.6028078379922942</v>
+        <v>0.64441504321439136</v>
       </c>
       <c r="AN7" s="46" t="e">
         <f>$B$6/AO5</f>
@@ -8935,7 +9013,7 @@
       </c>
       <c r="AO7" s="45">
         <f t="shared" si="29"/>
-        <v>0.6028078379922942</v>
+        <v>0.64441504321439136</v>
       </c>
       <c r="AP7" s="46" t="e">
         <f>$B$6/AQ5</f>
@@ -8943,7 +9021,7 @@
       </c>
       <c r="AQ7" s="45">
         <f t="shared" si="30"/>
-        <v>0.6028078379922942</v>
+        <v>0.64441504321439136</v>
       </c>
       <c r="AR7" s="46" t="e">
         <f>$B$6/AS5</f>
@@ -8951,7 +9029,7 @@
       </c>
       <c r="AS7" s="45">
         <f t="shared" si="31"/>
-        <v>0.6028078379922942</v>
+        <v>0.64441504321439136</v>
       </c>
       <c r="AT7" s="46" t="e">
         <f>$B$6/AU5</f>
@@ -8959,17 +9037,17 @@
       </c>
       <c r="AU7" s="45">
         <f t="shared" si="32"/>
-        <v>0.6028078379922942</v>
+        <v>0.64441504321439136</v>
       </c>
       <c r="AV7" s="49">
         <f>AU7-E7</f>
-        <v>0.55899335397857386</v>
+        <v>0.6006005592006709</v>
       </c>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.25">
       <c r="AV8" s="49">
         <f>AV6-AV7</f>
-        <v>1.7216774574660865E-2</v>
+        <v>1.8541141849634957E-2</v>
       </c>
     </row>
     <row r="10" spans="1:119" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit atualizacao tesouro 25/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -527,6 +527,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -658,6 +659,9 @@
                   <c:pt idx="14">
                     <c:v>24/jun</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>25/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -787,6 +791,9 @@
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
                   <c:v>3.89</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>3.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -889,6 +896,9 @@
                   <c:pt idx="14">
                     <c:v>24/jun</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>25/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1019,6 +1029,9 @@
                 <c:pt idx="14" formatCode="General">
                   <c:v>3.77</c:v>
                 </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>3.76</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1034,8 +1047,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1931528528"/>
-        <c:axId val="1931529072"/>
+        <c:axId val="1554215520"/>
+        <c:axId val="1554216064"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1143,6 +1156,9 @@
                         <c:pt idx="14">
                           <c:v>24/jun</c:v>
                         </c:pt>
+                        <c:pt idx="15">
+                          <c:v>25/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1276,7 +1292,7 @@
                         <c:v>0.22879688834286319</c:v>
                       </c:pt>
                       <c:pt idx="15" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22841235575741298</c:v>
                       </c:pt>
                       <c:pt idx="16" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1407,6 +1423,9 @@
                         <c:pt idx="14">
                           <c:v>24/jun</c:v>
                         </c:pt>
+                        <c:pt idx="15">
+                          <c:v>25/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1540,7 +1559,7 @@
                         <c:v>0.22464569645516558</c:v>
                       </c:pt>
                       <c:pt idx="15" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22426999509760159</c:v>
                       </c:pt>
                       <c:pt idx="16" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1570,7 +1589,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1931528528"/>
+        <c:axId val="1554215520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1613,7 +1632,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1931529072"/>
+        <c:crossAx val="1554216064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1621,7 +1640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1931529072"/>
+        <c:axId val="1554216064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1672,7 +1691,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1931528528"/>
+        <c:crossAx val="1554215520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1686,6 +1705,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1797,6 +1817,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1928,6 +1949,9 @@
                   <c:pt idx="14">
                     <c:v>24/jun</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>25/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2057,6 +2081,9 @@
                 </c:pt>
                 <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1764.18</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1767.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2159,6 +2186,9 @@
                   <c:pt idx="14">
                     <c:v>24/jun</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>25/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2289,6 +2319,9 @@
                 <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1796.78</c:v>
                 </c:pt>
+                <c:pt idx="15" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1799.79</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2304,11 +2337,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1931530160"/>
-        <c:axId val="1931530704"/>
+        <c:axId val="1554212256"/>
+        <c:axId val="1554223680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1931530160"/>
+        <c:axId val="1554212256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2351,7 +2384,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1931530704"/>
+        <c:crossAx val="1554223680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2359,7 +2392,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1931530704"/>
+        <c:axId val="1554223680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2410,7 +2443,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1931530160"/>
+        <c:crossAx val="1554212256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2424,6 +2457,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2505,6 +2539,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2636,6 +2671,9 @@
                   <c:pt idx="14">
                     <c:v>24/jun</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>25/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2767,7 +2805,7 @@
                   <c:v>0.22879688834286319</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22841235575741298</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2888,6 +2926,9 @@
                   <c:pt idx="14">
                     <c:v>24/jun</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>25/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3019,7 +3060,7 @@
                   <c:v>0.22464569645516558</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22426999509760159</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00">
                   <c:v>0</c:v>
@@ -3054,8 +3095,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1931536144"/>
-        <c:axId val="1931532880"/>
+        <c:axId val="1554213344"/>
+        <c:axId val="1554213888"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3163,6 +3204,9 @@
                         <c:pt idx="14">
                           <c:v>24/jun</c:v>
                         </c:pt>
+                        <c:pt idx="15">
+                          <c:v>25/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3294,6 +3338,9 @@
                       </c:pt>
                       <c:pt idx="14" formatCode="General">
                         <c:v>3.89</c:v>
+                      </c:pt>
+                      <c:pt idx="15" formatCode="General">
+                        <c:v>3.88</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3406,6 +3453,9 @@
                         <c:pt idx="14">
                           <c:v>24/jun</c:v>
                         </c:pt>
+                        <c:pt idx="15">
+                          <c:v>25/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3538,6 +3588,9 @@
                       <c:pt idx="14" formatCode="General">
                         <c:v>3.77</c:v>
                       </c:pt>
+                      <c:pt idx="15" formatCode="General">
+                        <c:v>3.76</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3548,7 +3601,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1931536144"/>
+        <c:axId val="1554213344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3591,7 +3644,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1931532880"/>
+        <c:crossAx val="1554213888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3599,7 +3652,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1931532880"/>
+        <c:axId val="1554213888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3650,7 +3703,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1931536144"/>
+        <c:crossAx val="1554213344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3664,6 +3717,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3745,6 +3799,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3876,6 +3931,9 @@
                   <c:pt idx="14">
                     <c:v>24/jun</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>25/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -4007,25 +4065,25 @@
                   <c:v>0.66428055233900019</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.66428055233900019</c:v>
+                  <c:v>0.70710176089649013</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.66428055233900019</c:v>
+                  <c:v>0.70710176089649013</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.66428055233900019</c:v>
+                  <c:v>0.70710176089649013</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.66428055233900019</c:v>
+                  <c:v>0.70710176089649013</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.66428055233900019</c:v>
+                  <c:v>0.70710176089649013</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.66428055233900019</c:v>
+                  <c:v>0.70710176089649013</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.66428055233900019</c:v>
+                  <c:v>0.70710176089649013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4128,6 +4186,9 @@
                   <c:pt idx="14">
                     <c:v>24/jun</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>25/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -4259,25 +4320,25 @@
                   <c:v>0.64441504321439136</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.64441504321439136</c:v>
+                  <c:v>0.68591188449690743</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.64441504321439136</c:v>
+                  <c:v>0.68591188449690743</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.64441504321439136</c:v>
+                  <c:v>0.68591188449690743</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.64441504321439136</c:v>
+                  <c:v>0.68591188449690743</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.64441504321439136</c:v>
+                  <c:v>0.68591188449690743</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.64441504321439136</c:v>
+                  <c:v>0.68591188449690743</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.64441504321439136</c:v>
+                  <c:v>0.68591188449690743</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4294,8 +4355,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1931532336"/>
-        <c:axId val="1931539952"/>
+        <c:axId val="1554219328"/>
+        <c:axId val="1554219872"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4403,6 +4464,9 @@
                         <c:pt idx="14">
                           <c:v>24/jun</c:v>
                         </c:pt>
+                        <c:pt idx="15">
+                          <c:v>25/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4534,6 +4598,9 @@
                       </c:pt>
                       <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1764.18</c:v>
+                      </c:pt>
+                      <c:pt idx="15" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1767.15</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4646,6 +4713,9 @@
                         <c:pt idx="14">
                           <c:v>24/jun</c:v>
                         </c:pt>
+                        <c:pt idx="15">
+                          <c:v>25/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4778,6 +4848,9 @@
                       <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1796.78</c:v>
                       </c:pt>
+                      <c:pt idx="15" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1799.79</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4788,7 +4861,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1931532336"/>
+        <c:axId val="1554219328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4831,7 +4904,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1931539952"/>
+        <c:crossAx val="1554219872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4839,7 +4912,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1931539952"/>
+        <c:axId val="1554219872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4890,7 +4963,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1931532336"/>
+        <c:crossAx val="1554219328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4904,6 +4977,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7908,8 +7982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AG4" sqref="AG4"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8271,8 +8345,12 @@
       <c r="AG3" s="23">
         <v>43640</v>
       </c>
-      <c r="AH3" s="22"/>
-      <c r="AI3" s="23"/>
+      <c r="AH3" s="22">
+        <v>43641</v>
+      </c>
+      <c r="AI3" s="23">
+        <v>43641</v>
+      </c>
       <c r="AJ3" s="22"/>
       <c r="AK3" s="23"/>
       <c r="AL3" s="22"/>
@@ -8458,8 +8536,12 @@
       <c r="AG4" s="32">
         <v>1764.18</v>
       </c>
-      <c r="AH4" s="31"/>
-      <c r="AI4" s="32"/>
+      <c r="AH4" s="31">
+        <v>3.88</v>
+      </c>
+      <c r="AI4" s="32">
+        <v>1767.15</v>
+      </c>
       <c r="AJ4" s="31"/>
       <c r="AK4" s="32"/>
       <c r="AL4" s="31"/>
@@ -8645,8 +8727,12 @@
       <c r="AG5" s="43">
         <v>1796.78</v>
       </c>
-      <c r="AH5" s="42"/>
-      <c r="AI5" s="15"/>
+      <c r="AH5" s="42">
+        <v>3.76</v>
+      </c>
+      <c r="AI5" s="43">
+        <v>1799.79</v>
+      </c>
       <c r="AJ5" s="42"/>
       <c r="AK5" s="43"/>
       <c r="AL5" s="42"/>
@@ -8791,13 +8877,13 @@
         <f t="shared" ref="AG6:AG7" si="25">(((AF4/365)*$B$7)/100)+AE6</f>
         <v>0.66428055233900019</v>
       </c>
-      <c r="AH6" s="46" t="e">
+      <c r="AH6" s="46">
         <f>$B$6/AI4</f>
-        <v>#DIV/0!</v>
+        <v>0.22841235575741298</v>
       </c>
       <c r="AI6" s="45">
         <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
-        <v>0.66428055233900019</v>
+        <v>0.70710176089649013</v>
       </c>
       <c r="AJ6" s="46" t="e">
         <f>$B$6/AK4</f>
@@ -8805,7 +8891,7 @@
       </c>
       <c r="AK6" s="45">
         <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
-        <v>0.66428055233900019</v>
+        <v>0.70710176089649013</v>
       </c>
       <c r="AL6" s="46" t="e">
         <f>$B$6/AM4</f>
@@ -8813,7 +8899,7 @@
       </c>
       <c r="AM6" s="45">
         <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>0.66428055233900019</v>
+        <v>0.70710176089649013</v>
       </c>
       <c r="AN6" s="46" t="e">
         <f>$B$6/AO4</f>
@@ -8821,7 +8907,7 @@
       </c>
       <c r="AO6" s="45">
         <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>0.66428055233900019</v>
+        <v>0.70710176089649013</v>
       </c>
       <c r="AP6" s="46" t="e">
         <f>$B$6/AQ4</f>
@@ -8829,7 +8915,7 @@
       </c>
       <c r="AQ6" s="45">
         <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>0.66428055233900019</v>
+        <v>0.70710176089649013</v>
       </c>
       <c r="AR6" s="46" t="e">
         <f>$B$6/AS4</f>
@@ -8837,7 +8923,7 @@
       </c>
       <c r="AS6" s="45">
         <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>0.66428055233900019</v>
+        <v>0.70710176089649013</v>
       </c>
       <c r="AT6" s="46" t="e">
         <f>$B$6/AU4</f>
@@ -8845,11 +8931,11 @@
       </c>
       <c r="AU6" s="45">
         <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>0.66428055233900019</v>
+        <v>0.70710176089649013</v>
       </c>
       <c r="AV6" s="49">
         <f>AU6-E6</f>
-        <v>0.61914170105030586</v>
+        <v>0.6619629096077958</v>
       </c>
     </row>
     <row r="7" spans="1:119" x14ac:dyDescent="0.25">
@@ -8983,13 +9069,13 @@
         <f t="shared" si="25"/>
         <v>0.64441504321439136</v>
       </c>
-      <c r="AH7" s="46" t="e">
+      <c r="AH7" s="46">
         <f>$B$6/AI5</f>
-        <v>#DIV/0!</v>
+        <v>0.22426999509760159</v>
       </c>
       <c r="AI7" s="45">
         <f t="shared" si="26"/>
-        <v>0.64441504321439136</v>
+        <v>0.68591188449690743</v>
       </c>
       <c r="AJ7" s="46" t="e">
         <f>$B$6/AK5</f>
@@ -8997,7 +9083,7 @@
       </c>
       <c r="AK7" s="45">
         <f t="shared" si="27"/>
-        <v>0.64441504321439136</v>
+        <v>0.68591188449690743</v>
       </c>
       <c r="AL7" s="46" t="e">
         <f>$B$6/AM5</f>
@@ -9005,7 +9091,7 @@
       </c>
       <c r="AM7" s="45">
         <f t="shared" si="28"/>
-        <v>0.64441504321439136</v>
+        <v>0.68591188449690743</v>
       </c>
       <c r="AN7" s="46" t="e">
         <f>$B$6/AO5</f>
@@ -9013,7 +9099,7 @@
       </c>
       <c r="AO7" s="45">
         <f t="shared" si="29"/>
-        <v>0.64441504321439136</v>
+        <v>0.68591188449690743</v>
       </c>
       <c r="AP7" s="46" t="e">
         <f>$B$6/AQ5</f>
@@ -9021,7 +9107,7 @@
       </c>
       <c r="AQ7" s="45">
         <f t="shared" si="30"/>
-        <v>0.64441504321439136</v>
+        <v>0.68591188449690743</v>
       </c>
       <c r="AR7" s="46" t="e">
         <f>$B$6/AS5</f>
@@ -9029,7 +9115,7 @@
       </c>
       <c r="AS7" s="45">
         <f t="shared" si="31"/>
-        <v>0.64441504321439136</v>
+        <v>0.68591188449690743</v>
       </c>
       <c r="AT7" s="46" t="e">
         <f>$B$6/AU5</f>
@@ -9037,17 +9123,17 @@
       </c>
       <c r="AU7" s="45">
         <f t="shared" si="32"/>
-        <v>0.64441504321439136</v>
+        <v>0.68591188449690743</v>
       </c>
       <c r="AV7" s="49">
         <f>AU7-E7</f>
-        <v>0.6006005592006709</v>
+        <v>0.64209740048318698</v>
       </c>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.25">
       <c r="AV8" s="49">
         <f>AV6-AV7</f>
-        <v>1.8541141849634957E-2</v>
+        <v>1.9865509124608827E-2</v>
       </c>
     </row>
     <row r="10" spans="1:119" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit atualizacao tesouro dia 26/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -527,7 +527,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -662,6 +661,9 @@
                   <c:pt idx="15">
                     <c:v>25/jun</c:v>
                   </c:pt>
+                  <c:pt idx="16">
+                    <c:v>26/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -794,6 +796,9 @@
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
                   <c:v>3.88</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>3.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -899,6 +904,9 @@
                   <c:pt idx="15">
                     <c:v>25/jun</c:v>
                   </c:pt>
+                  <c:pt idx="16">
+                    <c:v>26/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1032,6 +1040,9 @@
                 <c:pt idx="15" formatCode="General">
                   <c:v>3.76</c:v>
                 </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>3.73</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1047,8 +1058,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1554215520"/>
-        <c:axId val="1554216064"/>
+        <c:axId val="-70953584"/>
+        <c:axId val="-70962288"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1159,6 +1170,9 @@
                         <c:pt idx="15">
                           <c:v>25/jun</c:v>
                         </c:pt>
+                        <c:pt idx="16">
+                          <c:v>26/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1295,7 +1309,7 @@
                         <c:v>0.22841235575741298</c:v>
                       </c:pt>
                       <c:pt idx="16" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22737145088929517</c:v>
                       </c:pt>
                       <c:pt idx="17" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1426,6 +1440,9 @@
                         <c:pt idx="15">
                           <c:v>25/jun</c:v>
                         </c:pt>
+                        <c:pt idx="16">
+                          <c:v>26/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1562,7 +1579,7 @@
                         <c:v>0.22426999509760159</c:v>
                       </c:pt>
                       <c:pt idx="16" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22324789659281782</c:v>
                       </c:pt>
                       <c:pt idx="17" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1589,7 +1606,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1554215520"/>
+        <c:axId val="-70953584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1632,7 +1649,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1554216064"/>
+        <c:crossAx val="-70962288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1640,7 +1657,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1554216064"/>
+        <c:axId val="-70962288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1691,7 +1708,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1554215520"/>
+        <c:crossAx val="-70953584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1705,7 +1722,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1817,7 +1833,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1952,6 +1967,9 @@
                   <c:pt idx="15">
                     <c:v>25/jun</c:v>
                   </c:pt>
+                  <c:pt idx="16">
+                    <c:v>26/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2084,6 +2102,9 @@
                 </c:pt>
                 <c:pt idx="15" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1767.15</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1775.24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2189,6 +2210,9 @@
                   <c:pt idx="15">
                     <c:v>25/jun</c:v>
                   </c:pt>
+                  <c:pt idx="16">
+                    <c:v>26/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2322,6 +2346,9 @@
                 <c:pt idx="15" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1799.79</c:v>
                 </c:pt>
+                <c:pt idx="16" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1808.03</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2337,11 +2364,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1554212256"/>
-        <c:axId val="1554223680"/>
+        <c:axId val="-70954672"/>
+        <c:axId val="-70954128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1554212256"/>
+        <c:axId val="-70954672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2384,7 +2411,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1554223680"/>
+        <c:crossAx val="-70954128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2392,7 +2419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1554223680"/>
+        <c:axId val="-70954128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2443,7 +2470,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1554212256"/>
+        <c:crossAx val="-70954672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2457,7 +2484,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2539,7 +2565,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2674,6 +2699,9 @@
                   <c:pt idx="15">
                     <c:v>25/jun</c:v>
                   </c:pt>
+                  <c:pt idx="16">
+                    <c:v>26/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2808,7 +2836,7 @@
                   <c:v>0.22841235575741298</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22737145088929517</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2929,6 +2957,9 @@
                   <c:pt idx="15">
                     <c:v>25/jun</c:v>
                   </c:pt>
+                  <c:pt idx="16">
+                    <c:v>26/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3063,7 +3094,7 @@
                   <c:v>0.22426999509760159</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22324789659281782</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00">
                   <c:v>0</c:v>
@@ -3095,8 +3126,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1554213344"/>
-        <c:axId val="1554213888"/>
+        <c:axId val="-70952496"/>
+        <c:axId val="-70967184"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3207,6 +3238,9 @@
                         <c:pt idx="15">
                           <c:v>25/jun</c:v>
                         </c:pt>
+                        <c:pt idx="16">
+                          <c:v>26/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3341,6 +3375,9 @@
                       </c:pt>
                       <c:pt idx="15" formatCode="General">
                         <c:v>3.88</c:v>
+                      </c:pt>
+                      <c:pt idx="16" formatCode="General">
+                        <c:v>3.85</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3456,6 +3493,9 @@
                         <c:pt idx="15">
                           <c:v>25/jun</c:v>
                         </c:pt>
+                        <c:pt idx="16">
+                          <c:v>26/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3591,6 +3631,9 @@
                       <c:pt idx="15" formatCode="General">
                         <c:v>3.76</c:v>
                       </c:pt>
+                      <c:pt idx="16" formatCode="General">
+                        <c:v>3.73</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3601,7 +3644,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1554213344"/>
+        <c:axId val="-70952496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3644,7 +3687,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1554213888"/>
+        <c:crossAx val="-70967184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3652,7 +3695,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1554213888"/>
+        <c:axId val="-70967184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3703,7 +3746,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1554213344"/>
+        <c:crossAx val="-70952496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3717,7 +3760,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3799,7 +3841,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3934,6 +3975,9 @@
                   <c:pt idx="15">
                     <c:v>25/jun</c:v>
                   </c:pt>
+                  <c:pt idx="16">
+                    <c:v>26/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -4068,22 +4112,22 @@
                   <c:v>0.70710176089649013</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.70710176089649013</c:v>
+                  <c:v>0.7495918776352366</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.70710176089649013</c:v>
+                  <c:v>0.7495918776352366</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.70710176089649013</c:v>
+                  <c:v>0.7495918776352366</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.70710176089649013</c:v>
+                  <c:v>0.7495918776352366</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.70710176089649013</c:v>
+                  <c:v>0.7495918776352366</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.70710176089649013</c:v>
+                  <c:v>0.7495918776352366</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4189,6 +4233,9 @@
                   <c:pt idx="15">
                     <c:v>25/jun</c:v>
                   </c:pt>
+                  <c:pt idx="16">
+                    <c:v>26/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -4323,22 +4370,22 @@
                   <c:v>0.68591188449690743</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.68591188449690743</c:v>
+                  <c:v>0.72707763396068004</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.68591188449690743</c:v>
+                  <c:v>0.72707763396068004</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.68591188449690743</c:v>
+                  <c:v>0.72707763396068004</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.68591188449690743</c:v>
+                  <c:v>0.72707763396068004</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.68591188449690743</c:v>
+                  <c:v>0.72707763396068004</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.68591188449690743</c:v>
+                  <c:v>0.72707763396068004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4355,8 +4402,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1554219328"/>
-        <c:axId val="1554219872"/>
+        <c:axId val="-70960656"/>
+        <c:axId val="-70951952"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4467,6 +4514,9 @@
                         <c:pt idx="15">
                           <c:v>25/jun</c:v>
                         </c:pt>
+                        <c:pt idx="16">
+                          <c:v>26/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4601,6 +4651,9 @@
                       </c:pt>
                       <c:pt idx="15" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1767.15</c:v>
+                      </c:pt>
+                      <c:pt idx="16" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1775.24</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4716,6 +4769,9 @@
                         <c:pt idx="15">
                           <c:v>25/jun</c:v>
                         </c:pt>
+                        <c:pt idx="16">
+                          <c:v>26/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4851,6 +4907,9 @@
                       <c:pt idx="15" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1799.79</c:v>
                       </c:pt>
+                      <c:pt idx="16" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1808.03</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4861,7 +4920,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1554219328"/>
+        <c:axId val="-70960656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4904,7 +4963,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1554219872"/>
+        <c:crossAx val="-70951952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4912,7 +4971,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1554219872"/>
+        <c:axId val="-70951952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4963,7 +5022,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1554219328"/>
+        <c:crossAx val="-70960656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4977,7 +5036,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7982,8 +8040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AH5" sqref="AH5"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AK4" sqref="AK4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8351,8 +8409,12 @@
       <c r="AI3" s="23">
         <v>43641</v>
       </c>
-      <c r="AJ3" s="22"/>
-      <c r="AK3" s="23"/>
+      <c r="AJ3" s="22">
+        <v>43642</v>
+      </c>
+      <c r="AK3" s="23">
+        <v>43642</v>
+      </c>
       <c r="AL3" s="22"/>
       <c r="AM3" s="23"/>
       <c r="AN3" s="22"/>
@@ -8542,8 +8604,12 @@
       <c r="AI4" s="32">
         <v>1767.15</v>
       </c>
-      <c r="AJ4" s="31"/>
-      <c r="AK4" s="32"/>
+      <c r="AJ4" s="31">
+        <v>3.85</v>
+      </c>
+      <c r="AK4" s="32">
+        <v>1775.24</v>
+      </c>
       <c r="AL4" s="31"/>
       <c r="AM4" s="32"/>
       <c r="AN4" s="31"/>
@@ -8733,8 +8799,12 @@
       <c r="AI5" s="43">
         <v>1799.79</v>
       </c>
-      <c r="AJ5" s="42"/>
-      <c r="AK5" s="43"/>
+      <c r="AJ5" s="42">
+        <v>3.73</v>
+      </c>
+      <c r="AK5" s="43">
+        <v>1808.03</v>
+      </c>
       <c r="AL5" s="42"/>
       <c r="AM5" s="43"/>
       <c r="AN5" s="42"/>
@@ -8885,13 +8955,13 @@
         <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
         <v>0.70710176089649013</v>
       </c>
-      <c r="AJ6" s="46" t="e">
+      <c r="AJ6" s="46">
         <f>$B$6/AK4</f>
-        <v>#DIV/0!</v>
+        <v>0.22737145088929517</v>
       </c>
       <c r="AK6" s="45">
         <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
-        <v>0.70710176089649013</v>
+        <v>0.7495918776352366</v>
       </c>
       <c r="AL6" s="46" t="e">
         <f>$B$6/AM4</f>
@@ -8899,7 +8969,7 @@
       </c>
       <c r="AM6" s="45">
         <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>0.70710176089649013</v>
+        <v>0.7495918776352366</v>
       </c>
       <c r="AN6" s="46" t="e">
         <f>$B$6/AO4</f>
@@ -8907,7 +8977,7 @@
       </c>
       <c r="AO6" s="45">
         <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>0.70710176089649013</v>
+        <v>0.7495918776352366</v>
       </c>
       <c r="AP6" s="46" t="e">
         <f>$B$6/AQ4</f>
@@ -8915,7 +8985,7 @@
       </c>
       <c r="AQ6" s="45">
         <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>0.70710176089649013</v>
+        <v>0.7495918776352366</v>
       </c>
       <c r="AR6" s="46" t="e">
         <f>$B$6/AS4</f>
@@ -8923,7 +8993,7 @@
       </c>
       <c r="AS6" s="45">
         <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>0.70710176089649013</v>
+        <v>0.7495918776352366</v>
       </c>
       <c r="AT6" s="46" t="e">
         <f>$B$6/AU4</f>
@@ -8931,11 +9001,11 @@
       </c>
       <c r="AU6" s="45">
         <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>0.70710176089649013</v>
+        <v>0.7495918776352366</v>
       </c>
       <c r="AV6" s="49">
         <f>AU6-E6</f>
-        <v>0.6619629096077958</v>
+        <v>0.70445302634654228</v>
       </c>
     </row>
     <row r="7" spans="1:119" x14ac:dyDescent="0.25">
@@ -9077,13 +9147,13 @@
         <f t="shared" si="26"/>
         <v>0.68591188449690743</v>
       </c>
-      <c r="AJ7" s="46" t="e">
+      <c r="AJ7" s="46">
         <f>$B$6/AK5</f>
-        <v>#DIV/0!</v>
+        <v>0.22324789659281782</v>
       </c>
       <c r="AK7" s="45">
         <f t="shared" si="27"/>
-        <v>0.68591188449690743</v>
+        <v>0.72707763396068004</v>
       </c>
       <c r="AL7" s="46" t="e">
         <f>$B$6/AM5</f>
@@ -9091,7 +9161,7 @@
       </c>
       <c r="AM7" s="45">
         <f t="shared" si="28"/>
-        <v>0.68591188449690743</v>
+        <v>0.72707763396068004</v>
       </c>
       <c r="AN7" s="46" t="e">
         <f>$B$6/AO5</f>
@@ -9099,7 +9169,7 @@
       </c>
       <c r="AO7" s="45">
         <f t="shared" si="29"/>
-        <v>0.68591188449690743</v>
+        <v>0.72707763396068004</v>
       </c>
       <c r="AP7" s="46" t="e">
         <f>$B$6/AQ5</f>
@@ -9107,7 +9177,7 @@
       </c>
       <c r="AQ7" s="45">
         <f t="shared" si="30"/>
-        <v>0.68591188449690743</v>
+        <v>0.72707763396068004</v>
       </c>
       <c r="AR7" s="46" t="e">
         <f>$B$6/AS5</f>
@@ -9115,7 +9185,7 @@
       </c>
       <c r="AS7" s="45">
         <f t="shared" si="31"/>
-        <v>0.68591188449690743</v>
+        <v>0.72707763396068004</v>
       </c>
       <c r="AT7" s="46" t="e">
         <f>$B$6/AU5</f>
@@ -9123,17 +9193,17 @@
       </c>
       <c r="AU7" s="45">
         <f t="shared" si="32"/>
-        <v>0.68591188449690743</v>
+        <v>0.72707763396068004</v>
       </c>
       <c r="AV7" s="49">
         <f>AU7-E7</f>
-        <v>0.64209740048318698</v>
+        <v>0.68326314994695969</v>
       </c>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.25">
       <c r="AV8" s="49">
         <f>AV6-AV7</f>
-        <v>1.9865509124608827E-2</v>
+        <v>2.1189876399582586E-2</v>
       </c>
     </row>
     <row r="10" spans="1:119" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit atualizacao tesouro 28/06
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -664,6 +664,12 @@
                   <c:pt idx="16">
                     <c:v>26/jun</c:v>
                   </c:pt>
+                  <c:pt idx="17">
+                    <c:v>27/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>28/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -799,6 +805,12 @@
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
                   <c:v>3.85</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>3.84</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>3.74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -907,6 +919,12 @@
                   <c:pt idx="16">
                     <c:v>26/jun</c:v>
                   </c:pt>
+                  <c:pt idx="17">
+                    <c:v>27/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>28/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1043,6 +1061,12 @@
                 <c:pt idx="16" formatCode="General">
                   <c:v>3.73</c:v>
                 </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>3.72</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>3.62</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1058,8 +1082,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-70953584"/>
-        <c:axId val="-70962288"/>
+        <c:axId val="1216286112"/>
+        <c:axId val="1216288832"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1173,6 +1197,12 @@
                         <c:pt idx="16">
                           <c:v>26/jun</c:v>
                         </c:pt>
+                        <c:pt idx="17">
+                          <c:v>27/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="18">
+                          <c:v>28/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1312,10 +1342,10 @@
                         <c:v>0.22737145088929517</c:v>
                       </c:pt>
                       <c:pt idx="17" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22699424385285732</c:v>
                       </c:pt>
                       <c:pt idx="18" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22353225259408238</c:v>
                       </c:pt>
                       <c:pt idx="19" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1443,6 +1473,12 @@
                         <c:pt idx="16">
                           <c:v>26/jun</c:v>
                         </c:pt>
+                        <c:pt idx="17">
+                          <c:v>27/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="18">
+                          <c:v>28/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -1582,10 +1618,10 @@
                         <c:v>0.22324789659281782</c:v>
                       </c:pt>
                       <c:pt idx="17" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.22287685223778181</c:v>
                       </c:pt>
                       <c:pt idx="18" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>0.21947512355254031</c:v>
                       </c:pt>
                       <c:pt idx="19" formatCode="0.00">
                         <c:v>0</c:v>
@@ -1606,7 +1642,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-70953584"/>
+        <c:axId val="1216286112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1649,7 +1685,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-70962288"/>
+        <c:crossAx val="1216288832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1657,7 +1693,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-70962288"/>
+        <c:axId val="1216288832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1708,7 +1744,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-70953584"/>
+        <c:crossAx val="1216286112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1970,6 +2006,12 @@
                   <c:pt idx="16">
                     <c:v>26/jun</c:v>
                   </c:pt>
+                  <c:pt idx="17">
+                    <c:v>27/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>28/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2105,6 +2147,12 @@
                 </c:pt>
                 <c:pt idx="16" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1775.24</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1778.19</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1805.73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2213,6 +2261,12 @@
                   <c:pt idx="16">
                     <c:v>26/jun</c:v>
                   </c:pt>
+                  <c:pt idx="17">
+                    <c:v>27/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>28/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2349,6 +2403,12 @@
                 <c:pt idx="16" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1808.03</c:v>
                 </c:pt>
+                <c:pt idx="17" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1811.04</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1839.11</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2364,11 +2424,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-70954672"/>
-        <c:axId val="-70954128"/>
+        <c:axId val="1216277408"/>
+        <c:axId val="1216277952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-70954672"/>
+        <c:axId val="1216277408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2411,7 +2471,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-70954128"/>
+        <c:crossAx val="1216277952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2419,7 +2479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-70954128"/>
+        <c:axId val="1216277952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2470,7 +2530,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-70954672"/>
+        <c:crossAx val="1216277408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2702,6 +2762,12 @@
                   <c:pt idx="16">
                     <c:v>26/jun</c:v>
                   </c:pt>
+                  <c:pt idx="17">
+                    <c:v>27/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>28/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2839,10 +2905,10 @@
                   <c:v>0.22737145088929517</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22699424385285732</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22353225259408238</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00">
                   <c:v>0</c:v>
@@ -2960,6 +3026,12 @@
                   <c:pt idx="16">
                     <c:v>26/jun</c:v>
                   </c:pt>
+                  <c:pt idx="17">
+                    <c:v>27/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>28/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3097,10 +3169,10 @@
                   <c:v>0.22324789659281782</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.22287685223778181</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>0.21947512355254031</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00">
                   <c:v>0</c:v>
@@ -3126,8 +3198,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-70952496"/>
-        <c:axId val="-70967184"/>
+        <c:axId val="1219792736"/>
+        <c:axId val="1219779680"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3241,6 +3313,12 @@
                         <c:pt idx="16">
                           <c:v>26/jun</c:v>
                         </c:pt>
+                        <c:pt idx="17">
+                          <c:v>27/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="18">
+                          <c:v>28/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3378,6 +3456,12 @@
                       </c:pt>
                       <c:pt idx="16" formatCode="General">
                         <c:v>3.85</c:v>
+                      </c:pt>
+                      <c:pt idx="17" formatCode="General">
+                        <c:v>3.84</c:v>
+                      </c:pt>
+                      <c:pt idx="18" formatCode="General">
+                        <c:v>3.74</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3496,6 +3580,12 @@
                         <c:pt idx="16">
                           <c:v>26/jun</c:v>
                         </c:pt>
+                        <c:pt idx="17">
+                          <c:v>27/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="18">
+                          <c:v>28/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3634,6 +3724,12 @@
                       <c:pt idx="16" formatCode="General">
                         <c:v>3.73</c:v>
                       </c:pt>
+                      <c:pt idx="17" formatCode="General">
+                        <c:v>3.72</c:v>
+                      </c:pt>
+                      <c:pt idx="18" formatCode="General">
+                        <c:v>3.62</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -3644,7 +3740,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-70952496"/>
+        <c:axId val="1219792736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3687,7 +3783,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-70967184"/>
+        <c:crossAx val="1219779680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3695,7 +3791,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-70967184"/>
+        <c:axId val="1219779680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3746,7 +3842,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-70952496"/>
+        <c:crossAx val="1219792736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3978,6 +4074,12 @@
                   <c:pt idx="16">
                     <c:v>26/jun</c:v>
                   </c:pt>
+                  <c:pt idx="17">
+                    <c:v>27/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>28/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -4115,19 +4217,19 @@
                   <c:v>0.7495918776352366</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.7495918776352366</c:v>
+                  <c:v>0.79197163043440189</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.7495918776352366</c:v>
+                  <c:v>0.83324774383775557</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.7495918776352366</c:v>
+                  <c:v>0.83324774383775557</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.7495918776352366</c:v>
+                  <c:v>0.83324774383775557</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.7495918776352366</c:v>
+                  <c:v>0.83324774383775557</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4236,6 +4338,12 @@
                   <c:pt idx="16">
                     <c:v>26/jun</c:v>
                   </c:pt>
+                  <c:pt idx="17">
+                    <c:v>27/jun</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>28/jun</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -4373,19 +4481,19 @@
                   <c:v>0.72707763396068004</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.72707763396068004</c:v>
+                  <c:v>0.76813301948487145</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.72707763396068004</c:v>
+                  <c:v>0.80808476561325127</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.72707763396068004</c:v>
+                  <c:v>0.80808476561325127</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.72707763396068004</c:v>
+                  <c:v>0.80808476561325127</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.72707763396068004</c:v>
+                  <c:v>0.80808476561325127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4402,8 +4510,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-70960656"/>
-        <c:axId val="-70951952"/>
+        <c:axId val="1219780768"/>
+        <c:axId val="1219780224"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4517,6 +4625,12 @@
                         <c:pt idx="16">
                           <c:v>26/jun</c:v>
                         </c:pt>
+                        <c:pt idx="17">
+                          <c:v>27/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="18">
+                          <c:v>28/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4654,6 +4768,12 @@
                       </c:pt>
                       <c:pt idx="16" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1775.24</c:v>
+                      </c:pt>
+                      <c:pt idx="17" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1778.19</c:v>
+                      </c:pt>
+                      <c:pt idx="18" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1805.73</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4772,6 +4892,12 @@
                         <c:pt idx="16">
                           <c:v>26/jun</c:v>
                         </c:pt>
+                        <c:pt idx="17">
+                          <c:v>27/jun</c:v>
+                        </c:pt>
+                        <c:pt idx="18">
+                          <c:v>28/jun</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4910,6 +5036,12 @@
                       <c:pt idx="16" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1808.03</c:v>
                       </c:pt>
+                      <c:pt idx="17" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1811.04</c:v>
+                      </c:pt>
+                      <c:pt idx="18" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1839.11</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4920,7 +5052,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-70960656"/>
+        <c:axId val="1219780768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4963,7 +5095,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-70951952"/>
+        <c:crossAx val="1219780224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4971,7 +5103,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-70951952"/>
+        <c:axId val="1219780224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5022,7 +5154,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-70960656"/>
+        <c:crossAx val="1219780768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8041,7 +8173,7 @@
   <dimension ref="A2:DO11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AK4" sqref="AK4"/>
+      <selection activeCell="AO4" sqref="AO4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8415,10 +8547,18 @@
       <c r="AK3" s="23">
         <v>43642</v>
       </c>
-      <c r="AL3" s="22"/>
-      <c r="AM3" s="23"/>
-      <c r="AN3" s="22"/>
-      <c r="AO3" s="23"/>
+      <c r="AL3" s="22">
+        <v>43643</v>
+      </c>
+      <c r="AM3" s="23">
+        <v>43643</v>
+      </c>
+      <c r="AN3" s="22">
+        <v>43644</v>
+      </c>
+      <c r="AO3" s="23">
+        <v>43644</v>
+      </c>
       <c r="AP3" s="22"/>
       <c r="AQ3" s="23"/>
       <c r="AR3" s="22"/>
@@ -8610,10 +8750,18 @@
       <c r="AK4" s="32">
         <v>1775.24</v>
       </c>
-      <c r="AL4" s="31"/>
-      <c r="AM4" s="32"/>
-      <c r="AN4" s="31"/>
-      <c r="AO4" s="33"/>
+      <c r="AL4" s="31">
+        <v>3.84</v>
+      </c>
+      <c r="AM4" s="32">
+        <v>1778.19</v>
+      </c>
+      <c r="AN4" s="31">
+        <v>3.74</v>
+      </c>
+      <c r="AO4" s="32">
+        <v>1805.73</v>
+      </c>
       <c r="AP4" s="31"/>
       <c r="AQ4" s="32"/>
       <c r="AR4" s="31"/>
@@ -8805,10 +8953,18 @@
       <c r="AK5" s="43">
         <v>1808.03</v>
       </c>
-      <c r="AL5" s="42"/>
-      <c r="AM5" s="43"/>
-      <c r="AN5" s="42"/>
-      <c r="AO5" s="48"/>
+      <c r="AL5" s="42">
+        <v>3.72</v>
+      </c>
+      <c r="AM5" s="43">
+        <v>1811.04</v>
+      </c>
+      <c r="AN5" s="42">
+        <v>3.62</v>
+      </c>
+      <c r="AO5" s="43">
+        <v>1839.11</v>
+      </c>
       <c r="AP5" s="42"/>
       <c r="AQ5" s="43"/>
       <c r="AR5" s="42"/>
@@ -8963,21 +9119,21 @@
         <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
         <v>0.7495918776352366</v>
       </c>
-      <c r="AL6" s="46" t="e">
+      <c r="AL6" s="46">
         <f>$B$6/AM4</f>
-        <v>#DIV/0!</v>
+        <v>0.22699424385285732</v>
       </c>
       <c r="AM6" s="45">
         <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>0.7495918776352366</v>
-      </c>
-      <c r="AN6" s="46" t="e">
+        <v>0.79197163043440189</v>
+      </c>
+      <c r="AN6" s="46">
         <f>$B$6/AO4</f>
-        <v>#DIV/0!</v>
+        <v>0.22353225259408238</v>
       </c>
       <c r="AO6" s="45">
         <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>0.7495918776352366</v>
+        <v>0.83324774383775557</v>
       </c>
       <c r="AP6" s="46" t="e">
         <f>$B$6/AQ4</f>
@@ -8985,7 +9141,7 @@
       </c>
       <c r="AQ6" s="45">
         <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>0.7495918776352366</v>
+        <v>0.83324774383775557</v>
       </c>
       <c r="AR6" s="46" t="e">
         <f>$B$6/AS4</f>
@@ -8993,7 +9149,7 @@
       </c>
       <c r="AS6" s="45">
         <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>0.7495918776352366</v>
+        <v>0.83324774383775557</v>
       </c>
       <c r="AT6" s="46" t="e">
         <f>$B$6/AU4</f>
@@ -9001,11 +9157,11 @@
       </c>
       <c r="AU6" s="45">
         <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>0.7495918776352366</v>
+        <v>0.83324774383775557</v>
       </c>
       <c r="AV6" s="49">
         <f>AU6-E6</f>
-        <v>0.70445302634654228</v>
+        <v>0.78810889254906125</v>
       </c>
     </row>
     <row r="7" spans="1:119" x14ac:dyDescent="0.25">
@@ -9155,21 +9311,21 @@
         <f t="shared" si="27"/>
         <v>0.72707763396068004</v>
       </c>
-      <c r="AL7" s="46" t="e">
+      <c r="AL7" s="46">
         <f>$B$6/AM5</f>
-        <v>#DIV/0!</v>
+        <v>0.22287685223778181</v>
       </c>
       <c r="AM7" s="45">
         <f t="shared" si="28"/>
-        <v>0.72707763396068004</v>
-      </c>
-      <c r="AN7" s="46" t="e">
+        <v>0.76813301948487145</v>
+      </c>
+      <c r="AN7" s="46">
         <f>$B$6/AO5</f>
-        <v>#DIV/0!</v>
+        <v>0.21947512355254031</v>
       </c>
       <c r="AO7" s="45">
         <f t="shared" si="29"/>
-        <v>0.72707763396068004</v>
+        <v>0.80808476561325127</v>
       </c>
       <c r="AP7" s="46" t="e">
         <f>$B$6/AQ5</f>
@@ -9177,7 +9333,7 @@
       </c>
       <c r="AQ7" s="45">
         <f t="shared" si="30"/>
-        <v>0.72707763396068004</v>
+        <v>0.80808476561325127</v>
       </c>
       <c r="AR7" s="46" t="e">
         <f>$B$6/AS5</f>
@@ -9185,7 +9341,7 @@
       </c>
       <c r="AS7" s="45">
         <f t="shared" si="31"/>
-        <v>0.72707763396068004</v>
+        <v>0.80808476561325127</v>
       </c>
       <c r="AT7" s="46" t="e">
         <f>$B$6/AU5</f>
@@ -9193,17 +9349,17 @@
       </c>
       <c r="AU7" s="45">
         <f t="shared" si="32"/>
-        <v>0.72707763396068004</v>
+        <v>0.80808476561325127</v>
       </c>
       <c r="AV7" s="49">
         <f>AU7-E7</f>
-        <v>0.68326314994695969</v>
+        <v>0.76427028159953081</v>
       </c>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.25">
       <c r="AV8" s="49">
         <f>AV6-AV7</f>
-        <v>2.1189876399582586E-2</v>
+        <v>2.3838610949530437E-2</v>
       </c>
     </row>
     <row r="10" spans="1:119" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit atualizacao tesouro 02/07
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO - 0619.xlsx
+++ b/TITULO COMPRADO - LIVIO - 0619.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
   <si>
     <t>DATA COMPRA</t>
   </si>
@@ -527,6 +527,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -605,13 +606,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AO$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3,GRAFICO!$AP$2:$AP$3,GRAFICO!$AR$2:$AR$3,GRAFICO!$AT$2:$AT$3)</c:f>
+              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>03/06</c:v>
@@ -727,15 +728,6 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -747,14 +739,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$4:$AU$4</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$4:$AO$4</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4,GRAFICO!$AB$4,GRAFICO!$AD$4,GRAFICO!$AF$4,GRAFICO!$AH$4,GRAFICO!$AJ$4,GRAFICO!$AL$4,GRAFICO!$AN$4,GRAFICO!$AP$4,GRAFICO!$AR$4,GRAFICO!$AT$4)</c:f>
+              <c:f>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4,GRAFICO!$AB$4,GRAFICO!$AD$4,GRAFICO!$AF$4,GRAFICO!$AH$4,GRAFICO!$AJ$4,GRAFICO!$AL$4,GRAFICO!$AN$4)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>4.09</c:v>
                 </c:pt>
@@ -860,13 +852,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AO$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3,GRAFICO!$AP$2:$AP$3,GRAFICO!$AR$2:$AR$3,GRAFICO!$AT$2:$AT$3)</c:f>
+              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>03/06</c:v>
@@ -982,15 +974,6 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1002,14 +985,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$5:$AU$5</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$5:$AO$5</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5,GRAFICO!$AB$5,GRAFICO!$AD$5,GRAFICO!$AF$5,GRAFICO!$AH$5,GRAFICO!$AJ$5,GRAFICO!$AL$5,GRAFICO!$AN$5,GRAFICO!$AP$5,GRAFICO!$AR$5,GRAFICO!$AT$5)</c:f>
+              <c:f>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5,GRAFICO!$AB$5,GRAFICO!$AD$5,GRAFICO!$AF$5,GRAFICO!$AH$5,GRAFICO!$AJ$5,GRAFICO!$AL$5,GRAFICO!$AN$5)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>3.97</c:v>
                 </c:pt>
@@ -1082,8 +1065,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1216286112"/>
-        <c:axId val="1216288832"/>
+        <c:axId val="627770176"/>
+        <c:axId val="627772352"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1136,15 +1119,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AO$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3,GRAFICO!$AP$2:$AP$3,GRAFICO!$AR$2:$AR$3,GRAFICO!$AT$2:$AT$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="22"/>
+                      <c:ptCount val="19"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>03/06</c:v>
@@ -1260,15 +1243,6 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="18">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                        </c:pt>
-                        <c:pt idx="19">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                        </c:pt>
-                        <c:pt idx="20">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                        </c:pt>
-                        <c:pt idx="21">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -1280,81 +1254,72 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$6:$AU$6</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$6:$AO$6</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6,GRAFICO!$AB$6,GRAFICO!$AD$6,GRAFICO!$AF$6,GRAFICO!$AH$6,GRAFICO!$AJ$6,GRAFICO!$AL$6,GRAFICO!$AN$6,GRAFICO!$AP$6,GRAFICO!$AR$6,GRAFICO!$AT$6)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6,GRAFICO!$AB$6,GRAFICO!$AD$6,GRAFICO!$AF$6,GRAFICO!$AH$6,GRAFICO!$AJ$6,GRAFICO!$AL$6,GRAFICO!$AN$6)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="22"/>
+                      <c:ptCount val="19"/>
                       <c:pt idx="0" formatCode="0.00">
-                        <c:v>0.23635021341885021</c:v>
+                        <c:v>5.45</c:v>
                       </c:pt>
                       <c:pt idx="1" formatCode="0.00">
-                        <c:v>0.23342387244852411</c:v>
+                        <c:v>5.6834238724485244</c:v>
                       </c:pt>
                       <c:pt idx="2" formatCode="0.00">
-                        <c:v>0.23479936621722805</c:v>
+                        <c:v>5.9182232386657523</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00">
-                        <c:v>0.23510297547657491</c:v>
+                        <c:v>6.1533262141423268</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00">
-                        <c:v>0.23486904489006116</c:v>
+                        <c:v>6.3881952590323881</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00">
-                        <c:v>0.23482258784736396</c:v>
+                        <c:v>6.623017846879752</c:v>
                       </c:pt>
                       <c:pt idx="6" formatCode="0.00">
-                        <c:v>0.233703634028922</c:v>
+                        <c:v>6.8567214809086741</c:v>
                       </c:pt>
                       <c:pt idx="7" formatCode="0.00">
-                        <c:v>0.23330109730926896</c:v>
+                        <c:v>7.0900225782179431</c:v>
                       </c:pt>
                       <c:pt idx="8" formatCode="0.00">
-                        <c:v>0.23361030568789315</c:v>
+                        <c:v>7.3236328839058364</c:v>
                       </c:pt>
                       <c:pt idx="9" formatCode="0.00">
-                        <c:v>0.23391897915256724</c:v>
+                        <c:v>7.5575518630584035</c:v>
                       </c:pt>
                       <c:pt idx="10" formatCode="0.00">
-                        <c:v>0.23317036923366918</c:v>
+                        <c:v>7.7907222322920724</c:v>
                       </c:pt>
                       <c:pt idx="11" formatCode="0.00">
-                        <c:v>0.23277772012659234</c:v>
+                        <c:v>8.0234999524186641</c:v>
                       </c:pt>
                       <c:pt idx="12" formatCode="0.00">
-                        <c:v>0.23309496403817884</c:v>
+                        <c:v>8.2565949164568426</c:v>
                       </c:pt>
                       <c:pt idx="13" formatCode="0.00">
-                        <c:v>0.22883191006157477</c:v>
+                        <c:v>8.4854268265184167</c:v>
                       </c:pt>
                       <c:pt idx="14" formatCode="0.00">
-                        <c:v>0.22879688834286319</c:v>
+                        <c:v>8.71422371486128</c:v>
                       </c:pt>
                       <c:pt idx="15" formatCode="0.00">
-                        <c:v>0.22841235575741298</c:v>
+                        <c:v>8.9426360706186934</c:v>
                       </c:pt>
                       <c:pt idx="16" formatCode="0.00">
-                        <c:v>0.22737145088929517</c:v>
+                        <c:v>9.1700075215079888</c:v>
                       </c:pt>
                       <c:pt idx="17" formatCode="0.00">
-                        <c:v>0.22699424385285732</c:v>
+                        <c:v>9.3970017653608462</c:v>
                       </c:pt>
                       <c:pt idx="18" formatCode="0.00">
-                        <c:v>0.22353225259408238</c:v>
-                      </c:pt>
-                      <c:pt idx="19" formatCode="0.00">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="20" formatCode="0.00">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="21" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>9.6205340179549292</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1412,15 +1377,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AO$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3,GRAFICO!$AP$2:$AP$3,GRAFICO!$AR$2:$AR$3,GRAFICO!$AT$2:$AT$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="22"/>
+                      <c:ptCount val="19"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>03/06</c:v>
@@ -1536,15 +1501,6 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="18">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                        </c:pt>
-                        <c:pt idx="19">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                        </c:pt>
-                        <c:pt idx="20">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                        </c:pt>
-                        <c:pt idx="21">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -1556,81 +1512,72 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$7:$AU$7</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$7:$AO$7</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$7,GRAFICO!$F$7,GRAFICO!$H$7,GRAFICO!$J$7,GRAFICO!$L$7,GRAFICO!$N$7,GRAFICO!$P$7,GRAFICO!$R$7,GRAFICO!$T$7,GRAFICO!$V$7,GRAFICO!$X$7,GRAFICO!$Z$7,GRAFICO!$AB$7,GRAFICO!$AD$7,GRAFICO!$AF$7,GRAFICO!$AH$7,GRAFICO!$AJ$7,GRAFICO!$AL$7,GRAFICO!$AN$7,GRAFICO!$AP$7,GRAFICO!$AR$7,GRAFICO!$AT$7)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$7,GRAFICO!$F$7,GRAFICO!$H$7,GRAFICO!$J$7,GRAFICO!$L$7,GRAFICO!$N$7,GRAFICO!$P$7,GRAFICO!$R$7,GRAFICO!$T$7,GRAFICO!$V$7,GRAFICO!$X$7,GRAFICO!$Z$7,GRAFICO!$AB$7,GRAFICO!$AD$7,GRAFICO!$AF$7,GRAFICO!$AH$7,GRAFICO!$AJ$7,GRAFICO!$AL$7,GRAFICO!$AN$7)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="22"/>
+                      <c:ptCount val="19"/>
                       <c:pt idx="0" formatCode="0.00">
-                        <c:v>0.23158909024970126</c:v>
+                        <c:v>5.38</c:v>
                       </c:pt>
                       <c:pt idx="1" formatCode="0.00">
-                        <c:v>0.22918011530391397</c:v>
+                        <c:v>5.6091801153039142</c:v>
                       </c:pt>
                       <c:pt idx="2" formatCode="0.00">
-                        <c:v>0.23053355406491119</c:v>
+                        <c:v>5.8397136693688259</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00">
-                        <c:v>0.23083282501441846</c:v>
+                        <c:v>6.0705464943832439</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00">
-                        <c:v>0.23060467590865394</c:v>
+                        <c:v>6.3011511702918979</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00">
-                        <c:v>0.23055989037277438</c:v>
+                        <c:v>6.531711060664672</c:v>
                       </c:pt>
                       <c:pt idx="6" formatCode="0.00">
-                        <c:v>0.2294602260708509</c:v>
+                        <c:v>6.7611712867355225</c:v>
                       </c:pt>
                       <c:pt idx="7" formatCode="0.00">
-                        <c:v>0.22906566245961513</c:v>
+                        <c:v>6.9902369491951379</c:v>
                       </c:pt>
                       <c:pt idx="8" formatCode="0.00">
-                        <c:v>0.22937155889252647</c:v>
+                        <c:v>7.2196085080876644</c:v>
                       </c:pt>
                       <c:pt idx="9" formatCode="0.00">
-                        <c:v>0.22967696650585082</c:v>
+                        <c:v>7.4492854745935153</c:v>
                       </c:pt>
                       <c:pt idx="10" formatCode="0.00">
-                        <c:v>0.22894093511699048</c:v>
+                        <c:v>7.678226409710506</c:v>
                       </c:pt>
                       <c:pt idx="11" formatCode="0.00">
-                        <c:v>0.2285559185956787</c:v>
+                        <c:v>7.9067823283061847</c:v>
                       </c:pt>
                       <c:pt idx="12" formatCode="0.00">
-                        <c:v>0.22886824020725002</c:v>
+                        <c:v>8.1356505685134355</c:v>
                       </c:pt>
                       <c:pt idx="13" formatCode="0.00">
-                        <c:v>0.22467945877101289</c:v>
+                        <c:v>8.3603300272844479</c:v>
                       </c:pt>
                       <c:pt idx="14" formatCode="0.00">
-                        <c:v>0.22464569645516558</c:v>
+                        <c:v>8.584975723739614</c:v>
                       </c:pt>
                       <c:pt idx="15" formatCode="0.00">
-                        <c:v>0.22426999509760159</c:v>
+                        <c:v>8.8092457188372162</c:v>
                       </c:pt>
                       <c:pt idx="16" formatCode="0.00">
-                        <c:v>0.22324789659281782</c:v>
+                        <c:v>9.0324936154300346</c:v>
                       </c:pt>
                       <c:pt idx="17" formatCode="0.00">
-                        <c:v>0.22287685223778181</c:v>
+                        <c:v>9.2553704676678166</c:v>
                       </c:pt>
                       <c:pt idx="18" formatCode="0.00">
-                        <c:v>0.21947512355254031</c:v>
-                      </c:pt>
-                      <c:pt idx="19" formatCode="0.00">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="20" formatCode="0.00">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="21" formatCode="0.00">
-                        <c:v>0</c:v>
+                        <c:v>9.4748455912203564</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1642,7 +1589,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1216286112"/>
+        <c:axId val="627770176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1685,7 +1632,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1216288832"/>
+        <c:crossAx val="627772352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1693,7 +1640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1216288832"/>
+        <c:axId val="627772352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1744,7 +1691,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1216286112"/>
+        <c:crossAx val="627770176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1758,6 +1705,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1869,6 +1817,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1944,16 +1893,9 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3,GRAFICO!$AI$2:$AI$3,GRAFICO!$AK$2:$AK$3,GRAFICO!$AM$2:$AM$3,GRAFICO!$AO$2:$AO$3,GRAFICO!$AQ$2:$AQ$3,GRAFICO!$AS$2:$AS$3,GRAFICO!$AU$2:$AU$3)</c:f>
+              <c:f>GRAFICO!$B$2:$AO$3</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>03/06</c:v>
@@ -2069,15 +2011,6 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>Preço Unitário</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>Preço Unitário</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Preço Unitário</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2089,14 +2022,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$4:$AU$4</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$4:$AO$4</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4,GRAFICO!$AE$4,GRAFICO!$AG$4,GRAFICO!$AI$4,GRAFICO!$AK$4,GRAFICO!$AM$4,GRAFICO!$AO$4,GRAFICO!$AQ$4,GRAFICO!$AS$4,GRAFICO!$AU$4)</c:f>
+              <c:f>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4,GRAFICO!$AE$4,GRAFICO!$AG$4,GRAFICO!$AI$4,GRAFICO!$AK$4,GRAFICO!$AM$4,GRAFICO!$AO$4)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1707.8</c:v>
                 </c:pt>
@@ -2199,16 +2132,9 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3,GRAFICO!$AI$2:$AI$3,GRAFICO!$AK$2:$AK$3,GRAFICO!$AM$2:$AM$3,GRAFICO!$AO$2:$AO$3,GRAFICO!$AQ$2:$AQ$3,GRAFICO!$AS$2:$AS$3,GRAFICO!$AU$2:$AU$3)</c:f>
+              <c:f>GRAFICO!$B$2:$AO$3</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>03/06</c:v>
@@ -2324,15 +2250,6 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>Preço Unitário</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>Preço Unitário</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Preço Unitário</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2344,14 +2261,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$5:$AU$5</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$5:$AO$5</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5,GRAFICO!$AE$5,GRAFICO!$AG$5,GRAFICO!$AI$5,GRAFICO!$AK$5,GRAFICO!$AM$5,GRAFICO!$AO$5,GRAFICO!$AQ$5,GRAFICO!$AS$5,GRAFICO!$AU$5)</c:f>
+              <c:f>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5,GRAFICO!$AE$5,GRAFICO!$AG$5,GRAFICO!$AI$5,GRAFICO!$AK$5,GRAFICO!$AM$5,GRAFICO!$AO$5)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1739.41</c:v>
                 </c:pt>
@@ -2424,11 +2341,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1216277408"/>
-        <c:axId val="1216277952"/>
+        <c:axId val="627774528"/>
+        <c:axId val="627783776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1216277408"/>
+        <c:axId val="627774528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2471,7 +2388,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1216277952"/>
+        <c:crossAx val="627783776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2479,7 +2396,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1216277952"/>
+        <c:axId val="627783776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2530,7 +2447,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1216277408"/>
+        <c:crossAx val="627774528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2544,6 +2461,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2625,6 +2543,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2703,13 +2622,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AO$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3,GRAFICO!$AP$2:$AP$3,GRAFICO!$AR$2:$AR$3,GRAFICO!$AT$2:$AT$3)</c:f>
+              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>03/06</c:v>
@@ -2825,15 +2744,6 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2845,79 +2755,70 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$6:$AU$6</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$6:$AO$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6,GRAFICO!$AB$6,GRAFICO!$AD$6,GRAFICO!$AF$6,GRAFICO!$AH$6,GRAFICO!$AJ$6,GRAFICO!$AL$6,GRAFICO!$AN$6,GRAFICO!$AP$6,GRAFICO!$AR$6,GRAFICO!$AT$6)</c:f>
+              <c:f>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6,GRAFICO!$AB$6,GRAFICO!$AD$6,GRAFICO!$AF$6,GRAFICO!$AH$6,GRAFICO!$AJ$6,GRAFICO!$AL$6,GRAFICO!$AN$6)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0" formatCode="0.00">
-                  <c:v>0.23635021341885021</c:v>
+                  <c:v>5.45</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="0.00">
-                  <c:v>0.23342387244852411</c:v>
+                  <c:v>5.6834238724485244</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00">
-                  <c:v>0.23479936621722805</c:v>
+                  <c:v>5.9182232386657523</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00">
-                  <c:v>0.23510297547657491</c:v>
+                  <c:v>6.1533262141423268</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00">
-                  <c:v>0.23486904489006116</c:v>
+                  <c:v>6.3881952590323881</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
-                  <c:v>0.23482258784736396</c:v>
+                  <c:v>6.623017846879752</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>0.233703634028922</c:v>
+                  <c:v>6.8567214809086741</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00">
-                  <c:v>0.23330109730926896</c:v>
+                  <c:v>7.0900225782179431</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00">
-                  <c:v>0.23361030568789315</c:v>
+                  <c:v>7.3236328839058364</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
-                  <c:v>0.23391897915256724</c:v>
+                  <c:v>7.5575518630584035</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00">
-                  <c:v>0.23317036923366918</c:v>
+                  <c:v>7.7907222322920724</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00">
-                  <c:v>0.23277772012659234</c:v>
+                  <c:v>8.0234999524186641</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00">
-                  <c:v>0.23309496403817884</c:v>
+                  <c:v>8.2565949164568426</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00">
-                  <c:v>0.22883191006157477</c:v>
+                  <c:v>8.4854268265184167</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00">
-                  <c:v>0.22879688834286319</c:v>
+                  <c:v>8.71422371486128</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00">
-                  <c:v>0.22841235575741298</c:v>
+                  <c:v>8.9426360706186934</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00">
-                  <c:v>0.22737145088929517</c:v>
+                  <c:v>9.1700075215079888</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00">
-                  <c:v>0.22699424385285732</c:v>
+                  <c:v>9.3970017653608462</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00">
-                  <c:v>0.22353225259408238</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="0.00">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20" formatCode="0.00">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>9.6205340179549292</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2967,13 +2868,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AO$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3,GRAFICO!$AP$2:$AP$3,GRAFICO!$AR$2:$AR$3,GRAFICO!$AT$2:$AT$3)</c:f>
+              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>03/06</c:v>
@@ -3089,15 +2990,6 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -3109,79 +3001,70 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$7:$AU$7</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$7:$AO$7</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$7,GRAFICO!$F$7,GRAFICO!$H$7,GRAFICO!$J$7,GRAFICO!$L$7,GRAFICO!$N$7,GRAFICO!$P$7,GRAFICO!$R$7,GRAFICO!$T$7,GRAFICO!$V$7,GRAFICO!$X$7,GRAFICO!$Z$7,GRAFICO!$AB$7,GRAFICO!$AD$7,GRAFICO!$AF$7,GRAFICO!$AH$7,GRAFICO!$AJ$7,GRAFICO!$AL$7,GRAFICO!$AN$7,GRAFICO!$AP$7,GRAFICO!$AR$7,GRAFICO!$AT$7)</c:f>
+              <c:f>(GRAFICO!$D$7,GRAFICO!$F$7,GRAFICO!$H$7,GRAFICO!$J$7,GRAFICO!$L$7,GRAFICO!$N$7,GRAFICO!$P$7,GRAFICO!$R$7,GRAFICO!$T$7,GRAFICO!$V$7,GRAFICO!$X$7,GRAFICO!$Z$7,GRAFICO!$AB$7,GRAFICO!$AD$7,GRAFICO!$AF$7,GRAFICO!$AH$7,GRAFICO!$AJ$7,GRAFICO!$AL$7,GRAFICO!$AN$7)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0" formatCode="0.00">
-                  <c:v>0.23158909024970126</c:v>
+                  <c:v>5.38</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="0.00">
-                  <c:v>0.22918011530391397</c:v>
+                  <c:v>5.6091801153039142</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00">
-                  <c:v>0.23053355406491119</c:v>
+                  <c:v>5.8397136693688259</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00">
-                  <c:v>0.23083282501441846</c:v>
+                  <c:v>6.0705464943832439</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00">
-                  <c:v>0.23060467590865394</c:v>
+                  <c:v>6.3011511702918979</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
-                  <c:v>0.23055989037277438</c:v>
+                  <c:v>6.531711060664672</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>0.2294602260708509</c:v>
+                  <c:v>6.7611712867355225</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00">
-                  <c:v>0.22906566245961513</c:v>
+                  <c:v>6.9902369491951379</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00">
-                  <c:v>0.22937155889252647</c:v>
+                  <c:v>7.2196085080876644</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00">
-                  <c:v>0.22967696650585082</c:v>
+                  <c:v>7.4492854745935153</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00">
-                  <c:v>0.22894093511699048</c:v>
+                  <c:v>7.678226409710506</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00">
-                  <c:v>0.2285559185956787</c:v>
+                  <c:v>7.9067823283061847</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00">
-                  <c:v>0.22886824020725002</c:v>
+                  <c:v>8.1356505685134355</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00">
-                  <c:v>0.22467945877101289</c:v>
+                  <c:v>8.3603300272844479</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00">
-                  <c:v>0.22464569645516558</c:v>
+                  <c:v>8.584975723739614</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00">
-                  <c:v>0.22426999509760159</c:v>
+                  <c:v>8.8092457188372162</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00">
-                  <c:v>0.22324789659281782</c:v>
+                  <c:v>9.0324936154300346</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00">
-                  <c:v>0.22287685223778181</c:v>
+                  <c:v>9.2553704676678166</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00">
-                  <c:v>0.21947512355254031</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="0.00">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20" formatCode="0.00">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21" formatCode="0.00">
-                  <c:v>0</c:v>
+                  <c:v>9.4748455912203564</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3198,8 +3081,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1219792736"/>
-        <c:axId val="1219779680"/>
+        <c:axId val="627783232"/>
+        <c:axId val="627784320"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3252,15 +3135,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AO$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3,GRAFICO!$AP$2:$AP$3,GRAFICO!$AR$2:$AR$3,GRAFICO!$AT$2:$AT$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="22"/>
+                      <c:ptCount val="19"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>03/06</c:v>
@@ -3376,15 +3259,6 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="18">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                        </c:pt>
-                        <c:pt idx="19">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                        </c:pt>
-                        <c:pt idx="20">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                        </c:pt>
-                        <c:pt idx="21">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -3396,16 +3270,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$4:$AU$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$4:$AO$4</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4,GRAFICO!$AB$4,GRAFICO!$AD$4,GRAFICO!$AF$4,GRAFICO!$AH$4,GRAFICO!$AJ$4,GRAFICO!$AL$4,GRAFICO!$AN$4,GRAFICO!$AP$4,GRAFICO!$AR$4,GRAFICO!$AT$4)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4,GRAFICO!$AB$4,GRAFICO!$AD$4,GRAFICO!$AF$4,GRAFICO!$AH$4,GRAFICO!$AJ$4,GRAFICO!$AL$4,GRAFICO!$AN$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="22"/>
+                      <c:ptCount val="19"/>
                       <c:pt idx="0" formatCode="General">
                         <c:v>4.09</c:v>
                       </c:pt>
@@ -3519,15 +3393,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AO$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3,GRAFICO!$AP$2:$AP$3,GRAFICO!$AR$2:$AR$3,GRAFICO!$AT$2:$AT$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3,GRAFICO!$AL$2:$AL$3,GRAFICO!$AN$2:$AN$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="22"/>
+                      <c:ptCount val="19"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>03/06</c:v>
@@ -3643,15 +3517,6 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="18">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                        </c:pt>
-                        <c:pt idx="19">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                        </c:pt>
-                        <c:pt idx="20">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
-                        </c:pt>
-                        <c:pt idx="21">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -3663,16 +3528,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$5:$AU$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$5:$AO$5</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5,GRAFICO!$AB$5,GRAFICO!$AD$5,GRAFICO!$AF$5,GRAFICO!$AH$5,GRAFICO!$AJ$5,GRAFICO!$AL$5,GRAFICO!$AN$5,GRAFICO!$AP$5,GRAFICO!$AR$5,GRAFICO!$AT$5)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5,GRAFICO!$AB$5,GRAFICO!$AD$5,GRAFICO!$AF$5,GRAFICO!$AH$5,GRAFICO!$AJ$5,GRAFICO!$AL$5,GRAFICO!$AN$5)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="22"/>
+                      <c:ptCount val="19"/>
                       <c:pt idx="0" formatCode="General">
                         <c:v>3.97</c:v>
                       </c:pt>
@@ -3740,7 +3605,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1219792736"/>
+        <c:axId val="627783232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3783,7 +3648,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1219779680"/>
+        <c:crossAx val="627784320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3791,7 +3656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1219779680"/>
+        <c:axId val="627784320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3842,7 +3707,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1219792736"/>
+        <c:crossAx val="627783232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3856,6 +3721,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3937,6 +3803,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4012,16 +3879,9 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3,GRAFICO!$AI$2:$AI$3,GRAFICO!$AK$2:$AK$3,GRAFICO!$AM$2:$AM$3,GRAFICO!$AO$2:$AO$3,GRAFICO!$AQ$2:$AQ$3,GRAFICO!$AS$2:$AS$3,GRAFICO!$AU$2:$AU$3)</c:f>
+              <c:f>GRAFICO!$B$2:$AO$3</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>03/06</c:v>
@@ -4137,15 +3997,6 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>Preço Unitário</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>Preço Unitário</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Preço Unitário</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -4157,79 +4008,70 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$6:$AU$6</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$6:$AO$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6,GRAFICO!$AA$6,GRAFICO!$AC$6,GRAFICO!$AE$6,GRAFICO!$AG$6,GRAFICO!$AI$6,GRAFICO!$AK$6,GRAFICO!$AM$6,GRAFICO!$AO$6,GRAFICO!$AQ$6,GRAFICO!$AS$6,GRAFICO!$AU$6)</c:f>
+              <c:f>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6,GRAFICO!$AA$6,GRAFICO!$AC$6,GRAFICO!$AE$6,GRAFICO!$AG$6,GRAFICO!$AI$6,GRAFICO!$AK$6,GRAFICO!$AM$6,GRAFICO!$AO$6)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>4.5138851288694319E-2</c:v>
+                  <c:v>1.06</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.9394791060739359E-2</c:v>
+                  <c:v>1.1042559397720451</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.13409218659110902</c:v>
+                  <c:v>1.1489533353024148</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17889994606105986</c:v>
+                  <c:v>1.1937610947723656</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.22359734159142952</c:v>
+                  <c:v>1.2384584903027354</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26829473712179919</c:v>
+                  <c:v>1.2831558858331051</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.31266104083342539</c:v>
+                  <c:v>1.3275221895447313</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.35691698060547045</c:v>
+                  <c:v>1.3717781293167763</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.40128328431709664</c:v>
+                  <c:v>1.4161444330284025</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.44575995196830398</c:v>
+                  <c:v>1.4606211006796099</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.49001589174034904</c:v>
+                  <c:v>1.5048770404516549</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.53416146757281291</c:v>
+                  <c:v>1.5490226162841187</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.57841740734485791</c:v>
+                  <c:v>1.5932785560561638</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.62134897984192905</c:v>
+                  <c:v>1.6362101285532349</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.66428055233900019</c:v>
+                  <c:v>1.679141701050306</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.70710176089649013</c:v>
+                  <c:v>1.721962909607796</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.7495918776352366</c:v>
+                  <c:v>1.7644530263465426</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.79197163043440189</c:v>
+                  <c:v>1.8068327791457079</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.83324774383775557</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.83324774383775557</c:v>
-                </c:pt>
-                <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.83324774383775557</c:v>
-                </c:pt>
-                <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.83324774383775557</c:v>
+                  <c:v>1.8481088925490616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4276,16 +4118,9 @@
           </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3,GRAFICO!$AI$2:$AI$3,GRAFICO!$AK$2:$AK$3,GRAFICO!$AM$2:$AM$3,GRAFICO!$AO$2:$AO$3,GRAFICO!$AQ$2:$AQ$3,GRAFICO!$AS$2:$AS$3,GRAFICO!$AU$2:$AU$3)</c:f>
+              <c:f>GRAFICO!$B$2:$AO$3</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>03/06</c:v>
@@ -4401,15 +4236,6 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>Preço Unitário</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>Preço Unitário</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Preço Unitário</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -4421,79 +4247,70 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$7:$AU$7</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$7:$AO$7</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$7,GRAFICO!$G$7,GRAFICO!$I$7,GRAFICO!$K$7,GRAFICO!$M$7,GRAFICO!$O$7,GRAFICO!$Q$7,GRAFICO!$S$7,GRAFICO!$U$7,GRAFICO!$W$7,GRAFICO!$Y$7,GRAFICO!$AA$7,GRAFICO!$AC$7,GRAFICO!$AE$7,GRAFICO!$AG$7,GRAFICO!$AI$7,GRAFICO!$AK$7,GRAFICO!$AM$7,GRAFICO!$AO$7,GRAFICO!$AQ$7,GRAFICO!$AS$7,GRAFICO!$AU$7)</c:f>
+              <c:f>(GRAFICO!$E$7,GRAFICO!$G$7,GRAFICO!$I$7,GRAFICO!$K$7,GRAFICO!$M$7,GRAFICO!$O$7,GRAFICO!$Q$7,GRAFICO!$S$7,GRAFICO!$U$7,GRAFICO!$W$7,GRAFICO!$Y$7,GRAFICO!$AA$7,GRAFICO!$AC$7,GRAFICO!$AE$7,GRAFICO!$AG$7,GRAFICO!$AI$7,GRAFICO!$AK$7,GRAFICO!$AM$7,GRAFICO!$AO$7)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>4.3814484013720401E-2</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>8.6746056510791536E-2</c:v>
+                  <c:v>1.0829315724970712</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.1301190847661873</c:v>
+                  <c:v>1.1263046007524669</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.17360247696116421</c:v>
+                  <c:v>1.1697879929474437</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.21697550521655998</c:v>
+                  <c:v>1.2131610212028394</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.26034853347195575</c:v>
+                  <c:v>1.2565340494582351</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.30339046990860802</c:v>
+                  <c:v>1.2995759858948874</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.34632204240567915</c:v>
+                  <c:v>1.3425075583919586</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38936397884233143</c:v>
+                  <c:v>1.3855494948286109</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43251627921856484</c:v>
+                  <c:v>1.4287017952048444</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.47544785171563597</c:v>
+                  <c:v>1.4716333677019156</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.51826906027312591</c:v>
+                  <c:v>1.5144545762594055</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.56120063277019705</c:v>
+                  <c:v>1.5573861487564766</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.6028078379922942</c:v>
+                  <c:v>1.5989933539785739</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.64441504321439136</c:v>
+                  <c:v>1.6406005592006712</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.68591188449690743</c:v>
+                  <c:v>1.6820974004831872</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.72707763396068004</c:v>
+                  <c:v>1.7232631499469597</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.76813301948487145</c:v>
+                  <c:v>1.764318535471151</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.80808476561325127</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.80808476561325127</c:v>
-                </c:pt>
-                <c:pt idx="20" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.80808476561325127</c:v>
-                </c:pt>
-                <c:pt idx="21" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.80808476561325127</c:v>
+                  <c:v>1.8042702815995308</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4510,8 +4327,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1219780768"/>
-        <c:axId val="1219780224"/>
+        <c:axId val="627779968"/>
+        <c:axId val="627777792"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4563,16 +4380,13 @@
                   <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
-                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3,GRAFICO!$AI$2:$AI$3,GRAFICO!$AK$2:$AK$3,GRAFICO!$AM$2:$AM$3,GRAFICO!$AO$2:$AO$3,GRAFICO!$AQ$2:$AQ$3,GRAFICO!$AS$2:$AS$3,GRAFICO!$AU$2:$AU$3)</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AO$3</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="22"/>
+                      <c:ptCount val="19"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>03/06</c:v>
@@ -4688,15 +4502,6 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="18">
-                          <c:v>Preço Unitário</c:v>
-                        </c:pt>
-                        <c:pt idx="19">
-                          <c:v>Preço Unitário</c:v>
-                        </c:pt>
-                        <c:pt idx="20">
-                          <c:v>Preço Unitário</c:v>
-                        </c:pt>
-                        <c:pt idx="21">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -4708,16 +4513,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$4:$AU$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$4:$AO$4</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4,GRAFICO!$AE$4,GRAFICO!$AG$4,GRAFICO!$AI$4,GRAFICO!$AK$4,GRAFICO!$AM$4,GRAFICO!$AO$4,GRAFICO!$AQ$4,GRAFICO!$AS$4,GRAFICO!$AU$4)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4,GRAFICO!$AE$4,GRAFICO!$AG$4,GRAFICO!$AI$4,GRAFICO!$AK$4,GRAFICO!$AM$4,GRAFICO!$AO$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="22"/>
+                      <c:ptCount val="19"/>
                       <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1707.8</c:v>
                       </c:pt>
@@ -4830,16 +4635,13 @@
                   <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$2:$AU$3</c15:sqref>
-                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3,GRAFICO!$AI$2:$AI$3,GRAFICO!$AK$2:$AK$3,GRAFICO!$AM$2:$AM$3,GRAFICO!$AO$2:$AO$3,GRAFICO!$AQ$2:$AQ$3,GRAFICO!$AS$2:$AS$3,GRAFICO!$AU$2:$AU$3)</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AO$3</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="22"/>
+                      <c:ptCount val="19"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>03/06</c:v>
@@ -4955,15 +4757,6 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="18">
-                          <c:v>Preço Unitário</c:v>
-                        </c:pt>
-                        <c:pt idx="19">
-                          <c:v>Preço Unitário</c:v>
-                        </c:pt>
-                        <c:pt idx="20">
-                          <c:v>Preço Unitário</c:v>
-                        </c:pt>
-                        <c:pt idx="21">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -4975,16 +4768,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$5:$AU$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$5:$AO$5</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5,GRAFICO!$AE$5,GRAFICO!$AG$5,GRAFICO!$AI$5,GRAFICO!$AK$5,GRAFICO!$AM$5,GRAFICO!$AO$5,GRAFICO!$AQ$5,GRAFICO!$AS$5,GRAFICO!$AU$5)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5,GRAFICO!$AE$5,GRAFICO!$AG$5,GRAFICO!$AI$5,GRAFICO!$AK$5,GRAFICO!$AM$5,GRAFICO!$AO$5)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="22"/>
+                      <c:ptCount val="19"/>
                       <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1739.41</c:v>
                       </c:pt>
@@ -5052,7 +4845,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1219780768"/>
+        <c:axId val="627779968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5095,7 +4888,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1219780224"/>
+        <c:crossAx val="627777792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5103,7 +4896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1219780224"/>
+        <c:axId val="627777792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5154,7 +4947,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1219780768"/>
+        <c:crossAx val="627779968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5168,6 +4961,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8170,10 +7964,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:DO11"/>
+  <dimension ref="A2:DI11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AO4" sqref="AO4"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AQ10" sqref="AQ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8219,16 +8013,10 @@
     <col min="39" max="39" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="28.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="28.85546875" style="40" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="28.85546875" style="40" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="28.85546875" style="40" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
-    <col min="48" max="119" width="9.140625" style="40"/>
+    <col min="42" max="113" width="9.140625" style="40"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:119" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:113" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
         <v>9</v>
       </c>
@@ -8349,24 +8137,12 @@
       <c r="AO2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AP2" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="AQ2" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="AR2" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="AS2" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT2" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="AU2" s="19" t="s">
-        <v>12</v>
-      </c>
+      <c r="AP2" s="39"/>
+      <c r="AQ2" s="39"/>
+      <c r="AR2" s="39"/>
+      <c r="AS2" s="39"/>
+      <c r="AT2" s="39"/>
+      <c r="AU2" s="39"/>
       <c r="AV2" s="39"/>
       <c r="AW2" s="39"/>
       <c r="AX2" s="39"/>
@@ -8433,14 +8209,8 @@
       <c r="DG2" s="39"/>
       <c r="DH2" s="39"/>
       <c r="DI2" s="39"/>
-      <c r="DJ2" s="39"/>
-      <c r="DK2" s="39"/>
-      <c r="DL2" s="39"/>
-      <c r="DM2" s="39"/>
-      <c r="DN2" s="39"/>
-      <c r="DO2" s="39"/>
     </row>
-    <row r="3" spans="1:119" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:113" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
         <v>13</v>
       </c>
@@ -8559,12 +8329,12 @@
       <c r="AO3" s="23">
         <v>43644</v>
       </c>
-      <c r="AP3" s="22"/>
-      <c r="AQ3" s="23"/>
-      <c r="AR3" s="22"/>
-      <c r="AS3" s="23"/>
-      <c r="AT3" s="22"/>
-      <c r="AU3" s="23"/>
+      <c r="AP3" s="39"/>
+      <c r="AQ3" s="39"/>
+      <c r="AR3" s="39"/>
+      <c r="AS3" s="39"/>
+      <c r="AT3" s="39"/>
+      <c r="AU3" s="39"/>
       <c r="AV3" s="39"/>
       <c r="AW3" s="39"/>
       <c r="AX3" s="39"/>
@@ -8631,14 +8401,8 @@
       <c r="DG3" s="39"/>
       <c r="DH3" s="39"/>
       <c r="DI3" s="39"/>
-      <c r="DJ3" s="39"/>
-      <c r="DK3" s="39"/>
-      <c r="DL3" s="39"/>
-      <c r="DM3" s="39"/>
-      <c r="DN3" s="39"/>
-      <c r="DO3" s="39"/>
     </row>
-    <row r="4" spans="1:119" s="34" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:113" s="34" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>14</v>
       </c>
@@ -8762,12 +8526,12 @@
       <c r="AO4" s="32">
         <v>1805.73</v>
       </c>
-      <c r="AP4" s="31"/>
-      <c r="AQ4" s="32"/>
-      <c r="AR4" s="31"/>
-      <c r="AS4" s="32"/>
-      <c r="AT4" s="31"/>
-      <c r="AU4" s="32"/>
+      <c r="AP4" s="39"/>
+      <c r="AQ4" s="39"/>
+      <c r="AR4" s="39"/>
+      <c r="AS4" s="39"/>
+      <c r="AT4" s="39"/>
+      <c r="AU4" s="39"/>
       <c r="AV4" s="39"/>
       <c r="AW4" s="39"/>
       <c r="AX4" s="39"/>
@@ -8834,14 +8598,8 @@
       <c r="DG4" s="39"/>
       <c r="DH4" s="39"/>
       <c r="DI4" s="39"/>
-      <c r="DJ4" s="39"/>
-      <c r="DK4" s="39"/>
-      <c r="DL4" s="39"/>
-      <c r="DM4" s="39"/>
-      <c r="DN4" s="39"/>
-      <c r="DO4" s="39"/>
     </row>
-    <row r="5" spans="1:119" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:113" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>15</v>
       </c>
@@ -8965,14 +8723,8 @@
       <c r="AO5" s="43">
         <v>1839.11</v>
       </c>
-      <c r="AP5" s="42"/>
-      <c r="AQ5" s="43"/>
-      <c r="AR5" s="42"/>
-      <c r="AS5" s="43"/>
-      <c r="AT5" s="42"/>
-      <c r="AU5" s="43"/>
     </row>
-    <row r="6" spans="1:119" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:113" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>16</v>
       </c>
@@ -8984,187 +8736,161 @@
         <v>43587</v>
       </c>
       <c r="D6" s="46">
-        <f>$B$6/E4</f>
-        <v>0.23635021341885021</v>
+        <v>5.45</v>
       </c>
       <c r="E6" s="45">
-        <f>(((D4/365)*$B$7)/100)</f>
-        <v>4.5138851288694319E-2</v>
+        <v>1.06</v>
       </c>
       <c r="F6" s="46">
-        <f>$B$6/G4</f>
-        <v>0.23342387244852411</v>
+        <f>D6+($B$6/G4)</f>
+        <v>5.6834238724485244</v>
       </c>
       <c r="G6" s="45">
         <f>(((F4/365)*$B$7)/100)+E6</f>
-        <v>8.9394791060739359E-2</v>
+        <v>1.1042559397720451</v>
       </c>
       <c r="H6" s="46">
-        <f t="shared" ref="H6" si="0">$B$6/I4</f>
-        <v>0.23479936621722805</v>
+        <f t="shared" ref="H6:H7" si="0">F6+($B$6/I4)</f>
+        <v>5.9182232386657523</v>
       </c>
       <c r="I6" s="45">
         <f t="shared" ref="I6:I7" si="1">(((H4/365)*$B$7)/100)+G6</f>
-        <v>0.13409218659110902</v>
+        <v>1.1489533353024148</v>
       </c>
       <c r="J6" s="46">
-        <f t="shared" ref="J6" si="2">$B$6/K4</f>
-        <v>0.23510297547657491</v>
+        <f t="shared" ref="J6:J7" si="2">H6+($B$6/K4)</f>
+        <v>6.1533262141423268</v>
       </c>
       <c r="K6" s="45">
         <f t="shared" ref="K6:K7" si="3">(((J4/365)*$B$7)/100)+I6</f>
-        <v>0.17889994606105986</v>
+        <v>1.1937610947723656</v>
       </c>
       <c r="L6" s="46">
-        <f t="shared" ref="L6" si="4">$B$6/M4</f>
-        <v>0.23486904489006116</v>
+        <f t="shared" ref="L6:L7" si="4">J6+($B$6/M4)</f>
+        <v>6.3881952590323881</v>
       </c>
       <c r="M6" s="45">
         <f t="shared" ref="M6:M7" si="5">(((L4/365)*$B$7)/100)+K6</f>
-        <v>0.22359734159142952</v>
+        <v>1.2384584903027354</v>
       </c>
       <c r="N6" s="46">
-        <f t="shared" ref="N6" si="6">$B$6/O4</f>
-        <v>0.23482258784736396</v>
+        <f t="shared" ref="N6:N7" si="6">L6+($B$6/O4)</f>
+        <v>6.623017846879752</v>
       </c>
       <c r="O6" s="45">
         <f t="shared" ref="O6:O7" si="7">(((N4/365)*$B$7)/100)+M6</f>
-        <v>0.26829473712179919</v>
+        <v>1.2831558858331051</v>
       </c>
       <c r="P6" s="46">
-        <f t="shared" ref="P6" si="8">$B$6/Q4</f>
-        <v>0.233703634028922</v>
+        <f t="shared" ref="P6:P7" si="8">N6+($B$6/Q4)</f>
+        <v>6.8567214809086741</v>
       </c>
       <c r="Q6" s="45">
         <f t="shared" ref="Q6:Q7" si="9">(((P4/365)*$B$7)/100)+O6</f>
-        <v>0.31266104083342539</v>
+        <v>1.3275221895447313</v>
       </c>
       <c r="R6" s="46">
-        <f t="shared" ref="R6" si="10">$B$6/S4</f>
-        <v>0.23330109730926896</v>
+        <f t="shared" ref="R6:R7" si="10">P6+($B$6/S4)</f>
+        <v>7.0900225782179431</v>
       </c>
       <c r="S6" s="45">
         <f t="shared" ref="S6:S7" si="11">(((R4/365)*$B$7)/100)+Q6</f>
-        <v>0.35691698060547045</v>
+        <v>1.3717781293167763</v>
       </c>
       <c r="T6" s="46">
-        <f t="shared" ref="T6" si="12">$B$6/U4</f>
-        <v>0.23361030568789315</v>
+        <f t="shared" ref="T6:T7" si="12">R6+($B$6/U4)</f>
+        <v>7.3236328839058364</v>
       </c>
       <c r="U6" s="45">
         <f t="shared" ref="U6:U7" si="13">(((T4/365)*$B$7)/100)+S6</f>
-        <v>0.40128328431709664</v>
+        <v>1.4161444330284025</v>
       </c>
       <c r="V6" s="46">
-        <f t="shared" ref="V6" si="14">$B$6/W4</f>
-        <v>0.23391897915256724</v>
+        <f t="shared" ref="V6:V7" si="14">T6+($B$6/W4)</f>
+        <v>7.5575518630584035</v>
       </c>
       <c r="W6" s="45">
         <f t="shared" ref="W6:W7" si="15">(((V4/365)*$B$7)/100)+U6</f>
-        <v>0.44575995196830398</v>
+        <v>1.4606211006796099</v>
       </c>
       <c r="X6" s="46">
-        <f t="shared" ref="X6" si="16">$B$6/Y4</f>
-        <v>0.23317036923366918</v>
+        <f t="shared" ref="X6:X7" si="16">V6+($B$6/Y4)</f>
+        <v>7.7907222322920724</v>
       </c>
       <c r="Y6" s="45">
         <f t="shared" ref="Y6:Y7" si="17">(((X4/365)*$B$7)/100)+W6</f>
-        <v>0.49001589174034904</v>
+        <v>1.5048770404516549</v>
       </c>
       <c r="Z6" s="46">
-        <f t="shared" ref="Z6" si="18">$B$6/AA4</f>
-        <v>0.23277772012659234</v>
+        <f t="shared" ref="Z6:Z7" si="18">X6+($B$6/AA4)</f>
+        <v>8.0234999524186641</v>
       </c>
       <c r="AA6" s="45">
         <f t="shared" ref="AA6:AA7" si="19">(((Z4/365)*$B$7)/100)+Y6</f>
-        <v>0.53416146757281291</v>
+        <v>1.5490226162841187</v>
       </c>
       <c r="AB6" s="46">
-        <f t="shared" ref="AB6" si="20">$B$6/AC4</f>
-        <v>0.23309496403817884</v>
+        <f t="shared" ref="AB6:AB7" si="20">Z6+($B$6/AC4)</f>
+        <v>8.2565949164568426</v>
       </c>
       <c r="AC6" s="45">
         <f t="shared" ref="AC6:AC7" si="21">(((AB4/365)*$B$7)/100)+AA6</f>
-        <v>0.57841740734485791</v>
+        <v>1.5932785560561638</v>
       </c>
       <c r="AD6" s="46">
-        <f t="shared" ref="AD6" si="22">$B$6/AE4</f>
-        <v>0.22883191006157477</v>
+        <f t="shared" ref="AD6:AD7" si="22">AB6+($B$6/AE4)</f>
+        <v>8.4854268265184167</v>
       </c>
       <c r="AE6" s="45">
         <f t="shared" ref="AE6:AE7" si="23">(((AD4/365)*$B$7)/100)+AC6</f>
-        <v>0.62134897984192905</v>
+        <v>1.6362101285532349</v>
       </c>
       <c r="AF6" s="46">
-        <f t="shared" ref="AF6" si="24">$B$6/AG4</f>
-        <v>0.22879688834286319</v>
+        <f t="shared" ref="AF6:AF7" si="24">AD6+($B$6/AG4)</f>
+        <v>8.71422371486128</v>
       </c>
       <c r="AG6" s="45">
         <f t="shared" ref="AG6:AG7" si="25">(((AF4/365)*$B$7)/100)+AE6</f>
-        <v>0.66428055233900019</v>
+        <v>1.679141701050306</v>
       </c>
       <c r="AH6" s="46">
-        <f>$B$6/AI4</f>
-        <v>0.22841235575741298</v>
+        <f t="shared" ref="AH6:AH7" si="26">AF6+($B$6/AI4)</f>
+        <v>8.9426360706186934</v>
       </c>
       <c r="AI6" s="45">
-        <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
-        <v>0.70710176089649013</v>
+        <f t="shared" ref="AI6:AI7" si="27">(((AH4/365)*$B$7)/100)+AG6</f>
+        <v>1.721962909607796</v>
       </c>
       <c r="AJ6" s="46">
-        <f>$B$6/AK4</f>
-        <v>0.22737145088929517</v>
+        <f t="shared" ref="AJ6:AJ7" si="28">AH6+($B$6/AK4)</f>
+        <v>9.1700075215079888</v>
       </c>
       <c r="AK6" s="45">
-        <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
-        <v>0.7495918776352366</v>
+        <f t="shared" ref="AK6:AK7" si="29">(((AJ4/365)*$B$7)/100)+AI6</f>
+        <v>1.7644530263465426</v>
       </c>
       <c r="AL6" s="46">
-        <f>$B$6/AM4</f>
-        <v>0.22699424385285732</v>
+        <f t="shared" ref="AL6:AL7" si="30">AJ6+($B$6/AM4)</f>
+        <v>9.3970017653608462</v>
       </c>
       <c r="AM6" s="45">
-        <f t="shared" ref="AM6:AM7" si="28">(((AL4/365)*$B$7)/100)+AK6</f>
-        <v>0.79197163043440189</v>
+        <f t="shared" ref="AM6:AM7" si="31">(((AL4/365)*$B$7)/100)+AK6</f>
+        <v>1.8068327791457079</v>
       </c>
       <c r="AN6" s="46">
-        <f>$B$6/AO4</f>
-        <v>0.22353225259408238</v>
+        <f t="shared" ref="AN6:AN7" si="32">AL6+($B$6/AO4)</f>
+        <v>9.6205340179549292</v>
       </c>
       <c r="AO6" s="45">
-        <f t="shared" ref="AO6:AO7" si="29">(((AN4/365)*$B$7)/100)+AM6</f>
-        <v>0.83324774383775557</v>
-      </c>
-      <c r="AP6" s="46" t="e">
-        <f>$B$6/AQ4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AQ6" s="45">
-        <f t="shared" ref="AQ6:AQ7" si="30">(((AP4/365)*$B$7)/100)+AO6</f>
-        <v>0.83324774383775557</v>
-      </c>
-      <c r="AR6" s="46" t="e">
-        <f>$B$6/AS4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AS6" s="45">
-        <f t="shared" ref="AS6:AS7" si="31">(((AR4/365)*$B$7)/100)+AQ6</f>
-        <v>0.83324774383775557</v>
-      </c>
-      <c r="AT6" s="46" t="e">
-        <f>$B$6/AU4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AU6" s="45">
-        <f t="shared" ref="AU6:AU7" si="32">(((AT4/365)*$B$7)/100)+AS6</f>
-        <v>0.83324774383775557</v>
-      </c>
-      <c r="AV6" s="49">
-        <f>AU6-E6</f>
-        <v>0.78810889254906125</v>
+        <f t="shared" ref="AO6:AO7" si="33">(((AN4/365)*$B$7)/100)+AM6</f>
+        <v>1.8481088925490616</v>
+      </c>
+      <c r="AP6" s="49">
+        <f>AO6-E6</f>
+        <v>0.78810889254906158</v>
       </c>
     </row>
-    <row r="7" spans="1:119" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:113" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>17</v>
       </c>
@@ -9176,196 +8902,170 @@
         <v>43587</v>
       </c>
       <c r="D7" s="46">
-        <f>$B$7/E5</f>
-        <v>0.23158909024970126</v>
+        <v>5.38</v>
       </c>
       <c r="E7" s="45">
-        <f>(((D5/365)*$B$7)/100)</f>
-        <v>4.3814484013720401E-2</v>
+        <v>1.04</v>
       </c>
       <c r="F7" s="46">
-        <f>$B$6/G5</f>
-        <v>0.22918011530391397</v>
+        <f>D7+($B$6/G5)</f>
+        <v>5.6091801153039142</v>
       </c>
       <c r="G7" s="45">
         <f>(((F5/365)*$B$7)/100)+E7</f>
-        <v>8.6746056510791536E-2</v>
+        <v>1.0829315724970712</v>
       </c>
       <c r="H7" s="46">
-        <f t="shared" ref="H7" si="33">$B$6/I5</f>
-        <v>0.23053355406491119</v>
+        <f t="shared" si="0"/>
+        <v>5.8397136693688259</v>
       </c>
       <c r="I7" s="45">
         <f t="shared" si="1"/>
-        <v>0.1301190847661873</v>
+        <v>1.1263046007524669</v>
       </c>
       <c r="J7" s="46">
-        <f t="shared" ref="J7" si="34">$B$6/K5</f>
-        <v>0.23083282501441846</v>
+        <f t="shared" si="2"/>
+        <v>6.0705464943832439</v>
       </c>
       <c r="K7" s="45">
         <f t="shared" si="3"/>
-        <v>0.17360247696116421</v>
+        <v>1.1697879929474437</v>
       </c>
       <c r="L7" s="46">
-        <f t="shared" ref="L7" si="35">$B$6/M5</f>
-        <v>0.23060467590865394</v>
+        <f t="shared" si="4"/>
+        <v>6.3011511702918979</v>
       </c>
       <c r="M7" s="45">
         <f t="shared" si="5"/>
-        <v>0.21697550521655998</v>
+        <v>1.2131610212028394</v>
       </c>
       <c r="N7" s="46">
-        <f t="shared" ref="N7" si="36">$B$6/O5</f>
-        <v>0.23055989037277438</v>
+        <f t="shared" si="6"/>
+        <v>6.531711060664672</v>
       </c>
       <c r="O7" s="45">
         <f t="shared" si="7"/>
-        <v>0.26034853347195575</v>
+        <v>1.2565340494582351</v>
       </c>
       <c r="P7" s="46">
-        <f t="shared" ref="P7" si="37">$B$6/Q5</f>
-        <v>0.2294602260708509</v>
+        <f t="shared" si="8"/>
+        <v>6.7611712867355225</v>
       </c>
       <c r="Q7" s="45">
         <f t="shared" si="9"/>
-        <v>0.30339046990860802</v>
+        <v>1.2995759858948874</v>
       </c>
       <c r="R7" s="46">
-        <f t="shared" ref="R7" si="38">$B$6/S5</f>
-        <v>0.22906566245961513</v>
+        <f t="shared" si="10"/>
+        <v>6.9902369491951379</v>
       </c>
       <c r="S7" s="45">
         <f t="shared" si="11"/>
-        <v>0.34632204240567915</v>
+        <v>1.3425075583919586</v>
       </c>
       <c r="T7" s="46">
-        <f t="shared" ref="T7" si="39">$B$6/U5</f>
-        <v>0.22937155889252647</v>
+        <f t="shared" si="12"/>
+        <v>7.2196085080876644</v>
       </c>
       <c r="U7" s="45">
         <f t="shared" si="13"/>
-        <v>0.38936397884233143</v>
+        <v>1.3855494948286109</v>
       </c>
       <c r="V7" s="46">
-        <f t="shared" ref="V7" si="40">$B$6/W5</f>
-        <v>0.22967696650585082</v>
+        <f t="shared" si="14"/>
+        <v>7.4492854745935153</v>
       </c>
       <c r="W7" s="45">
         <f t="shared" si="15"/>
-        <v>0.43251627921856484</v>
+        <v>1.4287017952048444</v>
       </c>
       <c r="X7" s="46">
-        <f t="shared" ref="X7" si="41">$B$6/Y5</f>
-        <v>0.22894093511699048</v>
+        <f t="shared" si="16"/>
+        <v>7.678226409710506</v>
       </c>
       <c r="Y7" s="45">
         <f t="shared" si="17"/>
-        <v>0.47544785171563597</v>
+        <v>1.4716333677019156</v>
       </c>
       <c r="Z7" s="46">
-        <f t="shared" ref="Z7" si="42">$B$6/AA5</f>
-        <v>0.2285559185956787</v>
+        <f t="shared" si="18"/>
+        <v>7.9067823283061847</v>
       </c>
       <c r="AA7" s="45">
         <f t="shared" si="19"/>
-        <v>0.51826906027312591</v>
+        <v>1.5144545762594055</v>
       </c>
       <c r="AB7" s="46">
-        <f t="shared" ref="AB7" si="43">$B$6/AC5</f>
-        <v>0.22886824020725002</v>
+        <f t="shared" si="20"/>
+        <v>8.1356505685134355</v>
       </c>
       <c r="AC7" s="45">
         <f t="shared" si="21"/>
-        <v>0.56120063277019705</v>
+        <v>1.5573861487564766</v>
       </c>
       <c r="AD7" s="46">
-        <f t="shared" ref="AD7" si="44">$B$6/AE5</f>
-        <v>0.22467945877101289</v>
+        <f t="shared" si="22"/>
+        <v>8.3603300272844479</v>
       </c>
       <c r="AE7" s="45">
         <f t="shared" si="23"/>
-        <v>0.6028078379922942</v>
+        <v>1.5989933539785739</v>
       </c>
       <c r="AF7" s="46">
-        <f>$B$6/AG5</f>
-        <v>0.22464569645516558</v>
+        <f t="shared" si="24"/>
+        <v>8.584975723739614</v>
       </c>
       <c r="AG7" s="45">
         <f t="shared" si="25"/>
-        <v>0.64441504321439136</v>
+        <v>1.6406005592006712</v>
       </c>
       <c r="AH7" s="46">
-        <f>$B$6/AI5</f>
-        <v>0.22426999509760159</v>
+        <f t="shared" si="26"/>
+        <v>8.8092457188372162</v>
       </c>
       <c r="AI7" s="45">
-        <f t="shared" si="26"/>
-        <v>0.68591188449690743</v>
+        <f t="shared" si="27"/>
+        <v>1.6820974004831872</v>
       </c>
       <c r="AJ7" s="46">
-        <f>$B$6/AK5</f>
-        <v>0.22324789659281782</v>
+        <f t="shared" si="28"/>
+        <v>9.0324936154300346</v>
       </c>
       <c r="AK7" s="45">
-        <f t="shared" si="27"/>
-        <v>0.72707763396068004</v>
+        <f t="shared" si="29"/>
+        <v>1.7232631499469597</v>
       </c>
       <c r="AL7" s="46">
-        <f>$B$6/AM5</f>
-        <v>0.22287685223778181</v>
+        <f t="shared" si="30"/>
+        <v>9.2553704676678166</v>
       </c>
       <c r="AM7" s="45">
-        <f t="shared" si="28"/>
-        <v>0.76813301948487145</v>
+        <f t="shared" si="31"/>
+        <v>1.764318535471151</v>
       </c>
       <c r="AN7" s="46">
-        <f>$B$6/AO5</f>
-        <v>0.21947512355254031</v>
+        <f t="shared" si="32"/>
+        <v>9.4748455912203564</v>
       </c>
       <c r="AO7" s="45">
-        <f t="shared" si="29"/>
-        <v>0.80808476561325127</v>
-      </c>
-      <c r="AP7" s="46" t="e">
-        <f>$B$6/AQ5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AQ7" s="45">
-        <f t="shared" si="30"/>
-        <v>0.80808476561325127</v>
-      </c>
-      <c r="AR7" s="46" t="e">
-        <f>$B$6/AS5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AS7" s="45">
-        <f t="shared" si="31"/>
-        <v>0.80808476561325127</v>
-      </c>
-      <c r="AT7" s="46" t="e">
-        <f>$B$6/AU5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AU7" s="45">
-        <f t="shared" si="32"/>
-        <v>0.80808476561325127</v>
-      </c>
-      <c r="AV7" s="49">
-        <f>AU7-E7</f>
+        <f t="shared" si="33"/>
+        <v>1.8042702815995308</v>
+      </c>
+      <c r="AP7" s="49">
+        <f>AO7-E7</f>
         <v>0.76427028159953081</v>
       </c>
     </row>
-    <row r="8" spans="1:119" x14ac:dyDescent="0.25">
-      <c r="AV8" s="49">
-        <f>AV6-AV7</f>
-        <v>2.3838610949530437E-2</v>
+    <row r="8" spans="1:113" x14ac:dyDescent="0.25">
+      <c r="AP8" s="49">
+        <f>AP6-AP7</f>
+        <v>2.383861094953077E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:119" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:113" x14ac:dyDescent="0.25">
       <c r="AC10" s="6"/>
     </row>
-    <row r="11" spans="1:119" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:113" x14ac:dyDescent="0.25">
       <c r="AC11" s="6"/>
     </row>
   </sheetData>

</xml_diff>